<commit_message>
Mid attempt to add spreadsheet update
</commit_message>
<xml_diff>
--- a/BotC-Stats.xlsx
+++ b/BotC-Stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://strath-my.sharepoint.com/personal/lewis_alexander_2022_uni_strath_ac_uk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rainb\Documents\code\BotC-GroupTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="704" documentId="8_{FCFB571D-E77E-4428-ABC3-E78C6D727C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71585A32-DAAC-482B-9AF7-C5CBCDBEB6B9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25849236-BBFB-4A29-8AF8-53846B5C566F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{6A883E2E-6B2D-4BEF-9626-D6F4FED911C1}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{6A883E2E-6B2D-4BEF-9626-D6F4FED911C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1046,10 +1046,10 @@
   <dimension ref="A1:EV159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="EU157" sqref="EU157"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33136,11 +33136,11 @@
         <v>0</v>
       </c>
       <c r="D73" s="1">
-        <f t="shared" ref="D70:D73" si="123">SUM(I73,N73,S73,X73,AC73,AH73,AM73,AR73,AW73,BB73,BG73,BL73,BQ73,BV73,CA73,CF73,CK73,CP73,CU73,CZ73,DE73,DJ73,DO73,DT73,DY73,ED73,EI73,EN73)</f>
+        <f t="shared" ref="D73" si="123">SUM(I73,N73,S73,X73,AC73,AH73,AM73,AR73,AW73,BB73,BG73,BL73,BQ73,BV73,CA73,CF73,CK73,CP73,CU73,CZ73,DE73,DJ73,DO73,DT73,DY73,ED73,EI73,EN73)</f>
         <v>0</v>
       </c>
       <c r="E73" s="1">
-        <f t="shared" ref="E70:E73" si="124">SUM(J73,O73,T73,Y73,AD73,AI73,AN73,AS73,AX73,BC73,BH73,BM73,BR73,BW73,CB73,CG73,CL73,CQ73,CV73,DA73,DF73,DK73,DP73,DU73,DZ73,EE73,EJ73,EO73)</f>
+        <f t="shared" ref="E73" si="124">SUM(J73,O73,T73,Y73,AD73,AI73,AN73,AS73,AX73,BC73,BH73,BM73,BR73,BW73,CB73,CG73,CL73,CQ73,CV73,DA73,DF73,DK73,DP73,DU73,DZ73,EE73,EJ73,EO73)</f>
         <v>0</v>
       </c>
       <c r="F73" s="1" t="str">
@@ -44428,7 +44428,7 @@
       </c>
       <c r="B99" s="5"/>
       <c r="C99" s="2">
-        <f t="shared" ref="C78:E99" si="188">SUM(H99,M99,R99,W99,AB99,AG99,AL99,AQ99,AV99,BA99,BF99,BK99,BP99,BU99,BZ99,CE99,CJ99,CO99,CT99,CY99,DD99,DI99,DN99,DS99,DX99,EC99,EH99,EM99)</f>
+        <f t="shared" ref="C99:E99" si="188">SUM(H99,M99,R99,W99,AB99,AG99,AL99,AQ99,AV99,BA99,BF99,BK99,BP99,BU99,BZ99,CE99,CJ99,CO99,CT99,CY99,DD99,DI99,DN99,DS99,DX99,EC99,EH99,EM99)</f>
         <v>0</v>
       </c>
       <c r="D99" s="2">

</xml_diff>

<commit_message>
fixed issue with excel sheet
</commit_message>
<xml_diff>
--- a/BotC-Stats.xlsx
+++ b/BotC-Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rainb\Documents\code\BotC-GroupTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3644342C-57BD-43F4-9710-89EA54164BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58EC4A0-E4AE-4ED7-9825-094DEA5B3DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{6A883E2E-6B2D-4BEF-9626-D6F4FED911C1}"/>
+    <workbookView xWindow="-32805" yWindow="2535" windowWidth="28800" windowHeight="15885" xr2:uid="{6A883E2E-6B2D-4BEF-9626-D6F4FED911C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1045,11 +1045,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8A5E5A-9AF3-4435-B5F4-E9654445F5CB}">
   <dimension ref="A1:EV159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D107" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G101" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S141" sqref="S141"/>
+      <selection pane="bottomRight" activeCell="S113" sqref="S113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3363,11 +3363,11 @@
       <c r="B8" s="2"/>
       <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
@@ -3375,7 +3375,7 @@
       </c>
       <c r="F8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="1">
@@ -3500,17 +3500,17 @@
       <c r="AU8" s="2"/>
       <c r="AV8" s="1">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AW8" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AX8" s="1">
         <v>0</v>
       </c>
       <c r="AY8" s="1" t="str">
         <f t="shared" si="20"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AZ8" s="2"/>
       <c r="BA8" s="1">
@@ -33133,11 +33133,11 @@
       <c r="B73" s="2"/>
       <c r="C73" s="1">
         <f>SUM(C5:C72)</f>
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D73" s="1">
         <f t="shared" ref="D73" si="123">SUM(I73,N73,S73,X73,AC73,AH73,AM73,AR73,AW73,BB73,BG73,BL73,BQ73,BV73,CA73,CF73,CK73,CP73,CU73,CZ73,DE73,DJ73,DO73,DT73,DY73,ED73,EI73,EN73)</f>
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E73" s="1">
         <f t="shared" ref="E73" si="124">SUM(J73,O73,T73,Y73,AD73,AI73,AN73,AS73,AX73,BC73,BH73,BM73,BR73,BW73,CB73,CG73,CL73,CQ73,CV73,DA73,DF73,DK73,DP73,DU73,DZ73,EE73,EJ73,EO73)</f>
@@ -33145,7 +33145,7 @@
       </c>
       <c r="F73" s="1" t="str">
         <f>IF(C73,D73/C73*100,0) &amp; "%"</f>
-        <v>71.4285714285714%</v>
+        <v>92.5925925925926%</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="1">
@@ -33286,11 +33286,11 @@
       <c r="AU73" s="2"/>
       <c r="AV73" s="1">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AW73" s="1">
         <f>SUM(AW5:AW72)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AX73" s="1">
         <f>SUM(AX5:AX72)</f>
@@ -33298,7 +33298,7 @@
       </c>
       <c r="AY73" s="1" t="str">
         <f t="shared" si="82"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AZ73" s="2"/>
       <c r="BA73" s="1">
@@ -42139,11 +42139,11 @@
       <c r="B94" s="5"/>
       <c r="C94" s="2">
         <f t="shared" si="127"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D94" s="2">
         <f t="shared" si="186"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E94" s="2">
         <f t="shared" si="187"/>
@@ -42151,7 +42151,7 @@
       </c>
       <c r="F94" s="2" t="str">
         <f t="shared" si="126"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G94" s="5"/>
       <c r="H94" s="2">
@@ -42276,17 +42276,17 @@
       <c r="AU94" s="5"/>
       <c r="AV94" s="2">
         <f t="shared" si="144"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AW94" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AX94" s="2">
         <v>0</v>
       </c>
       <c r="AY94" s="2" t="str">
         <f t="shared" si="145"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AZ94" s="5"/>
       <c r="BA94" s="2">
@@ -44429,11 +44429,11 @@
       <c r="B99" s="5"/>
       <c r="C99" s="2">
         <f t="shared" ref="C99:E99" si="188">SUM(H99,M99,R99,W99,AB99,AG99,AL99,AQ99,AV99,BA99,BF99,BK99,BP99,BU99,BZ99,CE99,CJ99,CO99,CT99,CY99,DD99,DI99,DN99,DS99,DX99,EC99,EH99,EM99)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D99" s="2">
         <f t="shared" si="188"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E99" s="2">
         <f t="shared" si="188"/>
@@ -44441,7 +44441,7 @@
       </c>
       <c r="F99" s="2" t="str">
         <f>IF(C99,D99/C99*100,0) &amp; "%"</f>
-        <v>0%</v>
+        <v>83.3333333333333%</v>
       </c>
       <c r="G99" s="5"/>
       <c r="H99" s="2">
@@ -44582,11 +44582,11 @@
       <c r="AU99" s="5"/>
       <c r="AV99" s="2">
         <f t="shared" si="144"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AW99" s="2">
         <f>SUM(AW77:AW98)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AX99" s="2">
         <f>SUM(AX77:AX98)</f>
@@ -44594,7 +44594,7 @@
       </c>
       <c r="AY99" s="2" t="str">
         <f>IF(AV99,AW99/AV99*100,0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AZ99" s="5"/>
       <c r="BA99" s="2">
@@ -45258,7 +45258,7 @@
       <c r="E102" s="9"/>
       <c r="F102" s="9" t="str">
         <f>IF(SUM(D73,D99),SUM(D73,D99)*100/SUM(C73,C99),0) &amp; "%"</f>
-        <v>62.5%</v>
+        <v>90.9090909090909%</v>
       </c>
       <c r="G102" s="10"/>
       <c r="H102" s="9" t="s">
@@ -45348,7 +45348,7 @@
       <c r="AX102" s="9"/>
       <c r="AY102" s="9" t="str">
         <f>IF(SUM(AW73,AW99),SUM(AW73,AW99)*100/SUM(AV73,AV99),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AZ102" s="10"/>
       <c r="BA102" s="9" t="s">
@@ -56339,11 +56339,11 @@
       <c r="B128" s="8"/>
       <c r="C128" s="7">
         <f t="shared" si="191"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D128" s="7">
         <f t="shared" si="250"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E128" s="7">
         <f t="shared" si="251"/>
@@ -56351,7 +56351,7 @@
       </c>
       <c r="F128" s="7" t="str">
         <f t="shared" si="190"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G128" s="8"/>
       <c r="H128" s="7">
@@ -56476,17 +56476,17 @@
       <c r="AU128" s="8"/>
       <c r="AV128" s="7">
         <f t="shared" si="208"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW128" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX128" s="7">
         <v>0</v>
       </c>
       <c r="AY128" s="7" t="str">
         <f t="shared" si="209"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AZ128" s="8"/>
       <c r="BA128" s="7">
@@ -57255,11 +57255,11 @@
       <c r="B130" s="8"/>
       <c r="C130" s="7">
         <f>SUM(C106:C129)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D130" s="7">
         <f>SUM(D106:D129)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E130" s="7">
         <f>SUM(E106:E129)</f>
@@ -57408,11 +57408,11 @@
       <c r="AU130" s="8"/>
       <c r="AV130" s="7">
         <f>SUM(AV106:AV129)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW130" s="7">
         <f>SUM(AW106:AW129)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX130" s="7">
         <f>SUM(AX106:AX129)</f>
@@ -57420,7 +57420,7 @@
       </c>
       <c r="AY130" s="7" t="str">
         <f>IF(AV130,AW130/AV130*100,0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AZ130" s="8"/>
       <c r="BA130" s="7">
@@ -61223,11 +61223,11 @@
       <c r="B140" s="11"/>
       <c r="C140" s="12">
         <f t="shared" si="254"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D140" s="12">
         <f t="shared" si="252"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E140" s="12">
         <f t="shared" si="252"/>
@@ -61235,7 +61235,7 @@
       </c>
       <c r="F140" s="13" t="str">
         <f t="shared" si="253"/>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="G140" s="11"/>
       <c r="H140" s="12">
@@ -61270,17 +61270,17 @@
       <c r="Q140" s="11"/>
       <c r="R140" s="12">
         <f t="shared" si="259"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S140" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T140" s="13">
         <v>0</v>
       </c>
       <c r="U140" s="13" t="str">
         <f t="shared" si="260"/>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="V140" s="11"/>
       <c r="W140" s="12">
@@ -65345,11 +65345,11 @@
       <c r="B149" s="11"/>
       <c r="C149" s="12">
         <f t="shared" si="254"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D149" s="12">
         <f t="shared" si="252"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E149" s="12">
         <f t="shared" si="252"/>
@@ -65357,7 +65357,7 @@
       </c>
       <c r="F149" s="13" t="str">
         <f t="shared" si="253"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G149" s="11"/>
       <c r="H149" s="12">
@@ -65482,17 +65482,17 @@
       <c r="AU149" s="11"/>
       <c r="AV149" s="12">
         <f t="shared" si="271"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW149" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX149" s="13">
         <v>0</v>
       </c>
       <c r="AY149" s="13" t="str">
         <f t="shared" si="272"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AZ149" s="11"/>
       <c r="BA149" s="12">
@@ -67228,11 +67228,11 @@
       <c r="Q153" s="11"/>
       <c r="R153" s="13">
         <f>SUM(R129:R152)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S153" s="12">
         <f>SUM(S134:S151)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T153" s="12">
         <f>SUM(T134:T151)</f>
@@ -67240,7 +67240,7 @@
       </c>
       <c r="U153" s="13" t="str">
         <f>IF(R153,S153/R153*100,0) &amp; "%"</f>
-        <v>16.6666666666667%</v>
+        <v>0%</v>
       </c>
       <c r="V153" s="11"/>
       <c r="W153" s="13">
@@ -67330,11 +67330,11 @@
       <c r="AU153" s="11"/>
       <c r="AV153" s="13">
         <f>SUM(AV129:AV152)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AW153" s="12">
         <f>SUM(AW134:AW151)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX153" s="12">
         <f>SUM(AX134:AX151)</f>
@@ -67342,7 +67342,7 @@
       </c>
       <c r="AY153" s="13" t="str">
         <f>IF(AV153,AW153/AV153*100,0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="AZ153" s="11"/>
       <c r="BA153" s="13">
@@ -68006,7 +68006,7 @@
       <c r="E156" s="9"/>
       <c r="F156" s="9" t="str">
         <f>IF(SUM(D130,D153),SUM(D130,D153)*100/SUM(C130,C153),0) &amp; "%"</f>
-        <v>66.6666666666667%</v>
+        <v>71.4285714285714%</v>
       </c>
       <c r="G156" s="10"/>
       <c r="H156" s="9" t="s">
@@ -68036,7 +68036,7 @@
       <c r="T156" s="9"/>
       <c r="U156" s="9" t="str">
         <f>IF(SUM(S130,S153),SUM(S130,S153)*100/SUM(R130,R153),0) &amp; "%"</f>
-        <v>44.4444444444444%</v>
+        <v>37.5%</v>
       </c>
       <c r="V156" s="10"/>
       <c r="W156" s="9" t="s">
@@ -68096,7 +68096,7 @@
       <c r="AX156" s="9"/>
       <c r="AY156" s="9" t="str">
         <f>IF(SUM(AW130,AW153),SUM(AW130,AW153)*100/SUM(AV130,AV153),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>66.6666666666667%</v>
       </c>
       <c r="AZ156" s="10"/>
       <c r="BA156" s="9" t="s">
@@ -68309,8 +68309,8 @@
       <c r="D157" s="9"/>
       <c r="E157" s="9"/>
       <c r="F157" s="9" t="str">
-        <f>IF(SUM(F156,F102),SUM(F156,F102)/SUM(NOT(COUNTIF(F156,"0%")),NOT(COUNTIF(F102,"0%"))),0) &amp; "%"</f>
-        <v>0%</v>
+        <f>((F156 + F102)/2)*100 &amp; "%"</f>
+        <v>81.1688311688311%</v>
       </c>
       <c r="G157" s="10"/>
       <c r="H157" s="9" t="s">
@@ -68319,7 +68319,7 @@
       <c r="I157" s="9"/>
       <c r="J157" s="9"/>
       <c r="K157" s="9" t="str">
-        <f>IF(SUM(K156,K102),SUM(K156,K102)/SUM(NOT(COUNTIF(K156,"0%")),NOT(COUNTIF(K102,"0%"))),0) &amp; "%"</f>
+        <f>((K156 + K102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="L157" s="10"/>
@@ -68329,7 +68329,7 @@
       <c r="N157" s="9"/>
       <c r="O157" s="9"/>
       <c r="P157" s="9" t="str">
-        <f>IF(SUM(P156,P102),SUM(P156,P102)/SUM(NOT(COUNTIF(P156,"0%")),NOT(COUNTIF(P102,"0%"))),0) &amp; "%"</f>
+        <f>((P156 + P102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="Q157" s="10"/>
@@ -68339,8 +68339,8 @@
       <c r="S157" s="9"/>
       <c r="T157" s="9"/>
       <c r="U157" s="9" t="str">
-        <f>IF(SUM(U156,U102),SUM(U156,U102)/SUM(NOT(COUNTIF(U156,"0%")),NOT(COUNTIF(U102,"0%"))),0) &amp; "%"</f>
-        <v>0%</v>
+        <f>((U156 + U102)/2)*100 &amp; "%"</f>
+        <v>50%</v>
       </c>
       <c r="V157" s="10"/>
       <c r="W157" s="9" t="s">
@@ -68349,7 +68349,7 @@
       <c r="X157" s="9"/>
       <c r="Y157" s="9"/>
       <c r="Z157" s="9" t="str">
-        <f>IF(SUM(Z156,Z102),SUM(Z156,Z102)/SUM(NOT(COUNTIF(Z156,"0%")),NOT(COUNTIF(Z102,"0%"))),0) &amp; "%"</f>
+        <f>((Z156 + Z102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="AA157" s="10"/>
@@ -68359,7 +68359,7 @@
       <c r="AC157" s="9"/>
       <c r="AD157" s="9"/>
       <c r="AE157" s="9" t="str">
-        <f>IF(SUM(AE156,AE102),SUM(AE156,AE102)/SUM(NOT(COUNTIF(AE156,"0%")),NOT(COUNTIF(AE102,"0%"))),0) &amp; "%"</f>
+        <f>((AE156 + AE102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="AF157" s="10"/>
@@ -68369,7 +68369,7 @@
       <c r="AH157" s="9"/>
       <c r="AI157" s="9"/>
       <c r="AJ157" s="9" t="str">
-        <f>IF(SUM(AJ156,AJ102),SUM(AJ156,AJ102)/SUM(NOT(COUNTIF(AJ156,"0%")),NOT(COUNTIF(AJ102,"0%"))),0) &amp; "%"</f>
+        <f>((AJ156 + AJ102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="AK157" s="10"/>
@@ -68379,7 +68379,7 @@
       <c r="AM157" s="9"/>
       <c r="AN157" s="9"/>
       <c r="AO157" s="9" t="str">
-        <f>IF(SUM(AO156,AO102),SUM(AO156,AO102)/SUM(NOT(COUNTIF(AO156,"0%")),NOT(COUNTIF(AO102,"0%"))),0) &amp; "%"</f>
+        <f>((AO156 + AO102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="AP157" s="10"/>
@@ -68389,7 +68389,7 @@
       <c r="AR157" s="9"/>
       <c r="AS157" s="9"/>
       <c r="AT157" s="9" t="str">
-        <f>IF(SUM(AT156,AT102),SUM(AT156,AT102)/SUM(NOT(COUNTIF(AT156,"0%")),NOT(COUNTIF(AT102,"0%"))),0) &amp; "%"</f>
+        <f>((AT156 + AT102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="AU157" s="10"/>
@@ -68399,8 +68399,8 @@
       <c r="AW157" s="9"/>
       <c r="AX157" s="9"/>
       <c r="AY157" s="9" t="str">
-        <f>IF(SUM(AY156,AY102),SUM(AY156,AY102)/SUM(NOT(COUNTIF(AY156,"0%")),NOT(COUNTIF(AY102,"0%"))),0) &amp; "%"</f>
-        <v>0%</v>
+        <f>((AY156 + AY102)/2)*100 &amp; "%"</f>
+        <v>83.3333333333333%</v>
       </c>
       <c r="AZ157" s="10"/>
       <c r="BA157" s="9" t="s">
@@ -68409,7 +68409,7 @@
       <c r="BB157" s="9"/>
       <c r="BC157" s="9"/>
       <c r="BD157" s="9" t="str">
-        <f>IF(SUM(BD156,BD102),SUM(BD156,BD102)/SUM(NOT(COUNTIF(BD156,"0%")),NOT(COUNTIF(BD102,"0%"))),0) &amp; "%"</f>
+        <f>((BD156 + BD102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="BE157" s="10"/>
@@ -68419,7 +68419,7 @@
       <c r="BG157" s="9"/>
       <c r="BH157" s="9"/>
       <c r="BI157" s="9" t="str">
-        <f>IF(SUM(BI156,BI102),SUM(BI156,BI102)/SUM(NOT(COUNTIF(BI156,"0%")),NOT(COUNTIF(BI102,"0%"))),0) &amp; "%"</f>
+        <f>((BI156 + BI102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="BJ157" s="10"/>
@@ -68429,7 +68429,7 @@
       <c r="BL157" s="9"/>
       <c r="BM157" s="9"/>
       <c r="BN157" s="9" t="str">
-        <f>IF(SUM(BN156,BN102),SUM(BN156,BN102)/SUM(NOT(COUNTIF(BN156,"0%")),NOT(COUNTIF(BN102,"0%"))),0) &amp; "%"</f>
+        <f>((BN156 + BN102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="BO157" s="10"/>
@@ -68439,7 +68439,7 @@
       <c r="BQ157" s="9"/>
       <c r="BR157" s="9"/>
       <c r="BS157" s="9" t="str">
-        <f>IF(SUM(BS156,BS102),SUM(BS156,BS102)/SUM(NOT(COUNTIF(BS156,"0%")),NOT(COUNTIF(BS102,"0%"))),0) &amp; "%"</f>
+        <f>((BS156 + BS102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="BT157" s="10"/>
@@ -68449,7 +68449,7 @@
       <c r="BV157" s="9"/>
       <c r="BW157" s="9"/>
       <c r="BX157" s="9" t="str">
-        <f>IF(SUM(BX156,BX102),SUM(BX156,BX102)/SUM(NOT(COUNTIF(BX156,"0%")),NOT(COUNTIF(BX102,"0%"))),0) &amp; "%"</f>
+        <f>((BX156 + BX102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="BY157" s="10"/>
@@ -68459,7 +68459,7 @@
       <c r="CA157" s="9"/>
       <c r="CB157" s="9"/>
       <c r="CC157" s="9" t="str">
-        <f>IF(SUM(CC156,CC102),SUM(CC156,CC102)/SUM(NOT(COUNTIF(CC156,"0%")),NOT(COUNTIF(CC102,"0%"))),0) &amp; "%"</f>
+        <f>((CC156 + CC102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="CD157" s="10"/>
@@ -68469,7 +68469,7 @@
       <c r="CF157" s="9"/>
       <c r="CG157" s="9"/>
       <c r="CH157" s="9" t="str">
-        <f>IF(SUM(CH156,CH102),SUM(CH156,CH102)/SUM(NOT(COUNTIF(CH156,"0%")),NOT(COUNTIF(CH102,"0%"))),0) &amp; "%"</f>
+        <f>((CH156 + CH102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="CI157" s="10"/>
@@ -68479,7 +68479,7 @@
       <c r="CK157" s="9"/>
       <c r="CL157" s="9"/>
       <c r="CM157" s="9" t="str">
-        <f>IF(SUM(CM156,CM102),SUM(CM156,CM102)/SUM(NOT(COUNTIF(CM156,"0%")),NOT(COUNTIF(CM102,"0%"))),0) &amp; "%"</f>
+        <f>((CM156 + CM102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="CN157" s="10"/>
@@ -68489,7 +68489,7 @@
       <c r="CP157" s="9"/>
       <c r="CQ157" s="9"/>
       <c r="CR157" s="9" t="str">
-        <f>IF(SUM(CR156,CR102),SUM(CR156,CR102)/SUM(NOT(COUNTIF(CR156,"0%")),NOT(COUNTIF(CR102,"0%"))),0) &amp; "%"</f>
+        <f>((CR156 + CR102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="CS157" s="10"/>
@@ -68499,7 +68499,7 @@
       <c r="CU157" s="9"/>
       <c r="CV157" s="9"/>
       <c r="CW157" s="9" t="str">
-        <f>IF(SUM(CW156,CW102),SUM(CW156,CW102)/SUM(NOT(COUNTIF(CW156,"0%")),NOT(COUNTIF(CW102,"0%"))),0) &amp; "%"</f>
+        <f>((CW156 + CW102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="CX157" s="10"/>
@@ -68509,7 +68509,7 @@
       <c r="CZ157" s="9"/>
       <c r="DA157" s="9"/>
       <c r="DB157" s="9" t="str">
-        <f>IF(SUM(DB156,DB102),SUM(DB156,DB102)/SUM(NOT(COUNTIF(DB156,"0%")),NOT(COUNTIF(DB102,"0%"))),0) &amp; "%"</f>
+        <f>((DB156 + DB102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="DC157" s="10"/>
@@ -68519,7 +68519,7 @@
       <c r="DE157" s="9"/>
       <c r="DF157" s="9"/>
       <c r="DG157" s="9" t="str">
-        <f>IF(SUM(DG156,DG102),SUM(DG156,DG102)/SUM(NOT(COUNTIF(DG156,"0%")),NOT(COUNTIF(DG102,"0%"))),0) &amp; "%"</f>
+        <f>((DG156 + DG102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="DH157" s="10"/>
@@ -68529,7 +68529,7 @@
       <c r="DJ157" s="9"/>
       <c r="DK157" s="9"/>
       <c r="DL157" s="9" t="str">
-        <f>IF(SUM(DL156,DL102),SUM(DL156,DL102)/SUM(NOT(COUNTIF(DL156,"0%")),NOT(COUNTIF(DL102,"0%"))),0) &amp; "%"</f>
+        <f>((DL156 + DL102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="DM157" s="10"/>
@@ -68539,7 +68539,7 @@
       <c r="DO157" s="9"/>
       <c r="DP157" s="9"/>
       <c r="DQ157" s="9" t="str">
-        <f>IF(SUM(DQ156,DQ102),SUM(DQ156,DQ102)/SUM(NOT(COUNTIF(DQ156,"0%")),NOT(COUNTIF(DQ102,"0%"))),0) &amp; "%"</f>
+        <f>((DQ156 + DQ102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="DR157" s="10"/>
@@ -68549,7 +68549,7 @@
       <c r="DT157" s="9"/>
       <c r="DU157" s="9"/>
       <c r="DV157" s="9" t="str">
-        <f>IF(SUM(DV156,DV102),SUM(DV156,DV102)/SUM(NOT(COUNTIF(DV156,"0%")),NOT(COUNTIF(DV102,"0%"))),0) &amp; "%"</f>
+        <f>((DV156 + DV102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="DW157" s="10"/>
@@ -68559,7 +68559,7 @@
       <c r="DY157" s="9"/>
       <c r="DZ157" s="9"/>
       <c r="EA157" s="9" t="str">
-        <f>IF(SUM(EA156,EA102),SUM(EA156,EA102)/SUM(NOT(COUNTIF(EA156,"0%")),NOT(COUNTIF(EA102,"0%"))),0) &amp; "%"</f>
+        <f>((EA156 + EA102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="EB157" s="10"/>
@@ -68569,7 +68569,7 @@
       <c r="ED157" s="9"/>
       <c r="EE157" s="9"/>
       <c r="EF157" s="9" t="str">
-        <f>IF(SUM(EF156,EF102),SUM(EF156,EF102)/SUM(NOT(COUNTIF(EF156,"0%")),NOT(COUNTIF(EF102,"0%"))),0) &amp; "%"</f>
+        <f>((EF156 + EF102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="EG157" s="10"/>
@@ -68579,7 +68579,7 @@
       <c r="EI157" s="9"/>
       <c r="EJ157" s="9"/>
       <c r="EK157" s="9" t="str">
-        <f>IF(SUM(EK156,EK102),SUM(EK156,EK102)/SUM(NOT(COUNTIF(EK156,"0%")),NOT(COUNTIF(EK102,"0%"))),0) &amp; "%"</f>
+        <f>((EK156 + EK102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="EL157" s="10"/>
@@ -68589,7 +68589,7 @@
       <c r="EN157" s="9"/>
       <c r="EO157" s="9"/>
       <c r="EP157" s="9" t="str">
-        <f>IF(SUM(EP156,EP102),SUM(EP156,EP102)/SUM(NOT(COUNTIF(EP156,"0%")),NOT(COUNTIF(EP102,"0%"))),0) &amp; "%"</f>
+        <f>((EP156 + EP102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="EQ157" s="15"/>
@@ -68599,7 +68599,7 @@
       <c r="ES157" s="9"/>
       <c r="ET157" s="9"/>
       <c r="EU157" s="9" t="str">
-        <f>IF(SUM(EU156,EU102),SUM(EU156,EU102)/SUM(NOT(COUNTIF(EU156,"0%")),NOT(COUNTIF(EU102,"0%"))),0) &amp; "%"</f>
+        <f>((EU156 + EU102)/2)*100 &amp; "%"</f>
         <v>0%</v>
       </c>
       <c r="EV157" s="3"/>
@@ -68919,14 +68919,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d74e12c9-bdf3-447e-ac63-b8aa30cb912e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006D6901F31B669244A77CF3DC592DC06F" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f07ba37d9f6a9a16ab78a3833be08f3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d74e12c9-bdf3-447e-ac63-b8aa30cb912e" xmlns:ns4="7ce3718d-1d19-4340-bc07-211e3ea25757" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3d76b4510715f63c0dd84a4bd0fa290f" ns3:_="" ns4:_="">
     <xsd:import namespace="d74e12c9-bdf3-447e-ac63-b8aa30cb912e"/>
@@ -69141,6 +69133,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d74e12c9-bdf3-447e-ac63-b8aa30cb912e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -69151,23 +69151,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E2E85D4-37C6-4843-9D21-AD40AB5F6E3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d74e12c9-bdf3-447e-ac63-b8aa30cb912e"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7ce3718d-1d19-4340-bc07-211e3ea25757"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D93BBC3-F948-4065-9078-5D0662F77D28}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -69186,6 +69169,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E2E85D4-37C6-4843-9D21-AD40AB5F6E3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d74e12c9-bdf3-447e-ac63-b8aa30cb912e"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7ce3718d-1d19-4340-bc07-211e3ea25757"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF8F943-7811-4141-8F4E-8FF466B07D87}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Added new functionality and fixed a couple more bugs in the excel sheet
</commit_message>
<xml_diff>
--- a/BotC-Stats.xlsx
+++ b/BotC-Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rainb\Documents\code\BotC-GroupTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58EC4A0-E4AE-4ED7-9825-094DEA5B3DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB4D034-6272-418A-995C-A80AE3E90E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32805" yWindow="2535" windowWidth="28800" windowHeight="15885" xr2:uid="{6A883E2E-6B2D-4BEF-9626-D6F4FED911C1}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{6A883E2E-6B2D-4BEF-9626-D6F4FED911C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1046,10 +1046,10 @@
   <dimension ref="A1:EV159"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G101" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S113" sqref="S113"/>
+      <selection pane="bottomRight" activeCell="P162" sqref="P162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1989,19 +1989,19 @@
       <c r="B5" s="2"/>
       <c r="C5" s="1">
         <f>SUM(H5,M5,R5,W5,AB5,AG5,AL5,AQ5,AV5,BA5,BF5,BK5,BP5,BU5,BZ5,CE5,CJ5,CO5,CT5,CY5,DD5,DI5,DN5,DS5,DX5,EC5,EH5,EM5,ER5)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" ref="D5:E20" si="0">SUM(I5,N5,S5,X5,AC5,AH5,AM5,AR5,AW5,BB5,BG5,BL5,BQ5,BV5,CA5,CF5,CK5,CP5,CU5,CZ5,DE5,DJ5,DO5,DT5,DY5,ED5,EI5,EN5,ES5)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1" t="str">
         <f>IF(C5,D5/C5*100,0) &amp; "%"</f>
-        <v>60%</v>
+        <v>0%</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="1">
@@ -2036,17 +2036,17 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="1">
         <f>SUM(S5,T5)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S5" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T5" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U5" s="1" t="str">
         <f>IF(R5,S5/R5*100,0) &amp; "%"</f>
-        <v>60%</v>
+        <v>0%</v>
       </c>
       <c r="V5" s="2"/>
       <c r="W5" s="1">
@@ -3363,11 +3363,11 @@
       <c r="B8" s="2"/>
       <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
@@ -3375,7 +3375,7 @@
       </c>
       <c r="F8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="1">
@@ -3500,17 +3500,17 @@
       <c r="AU8" s="2"/>
       <c r="AV8" s="1">
         <f t="shared" si="19"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AW8" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AX8" s="1">
         <v>0</v>
       </c>
       <c r="AY8" s="1" t="str">
         <f t="shared" si="20"/>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="AZ8" s="2"/>
       <c r="BA8" s="1">
@@ -27637,11 +27637,11 @@
       <c r="B61" s="2"/>
       <c r="C61" s="1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D61" s="1">
         <f t="shared" si="61"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E61" s="1">
         <f t="shared" si="62"/>
@@ -27649,7 +27649,7 @@
       </c>
       <c r="F61" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="1">
@@ -27684,17 +27684,17 @@
       <c r="Q61" s="2"/>
       <c r="R61" s="1">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S61" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T61" s="1">
         <v>0</v>
       </c>
       <c r="U61" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="V61" s="2"/>
       <c r="W61" s="1">
@@ -33133,19 +33133,19 @@
       <c r="B73" s="2"/>
       <c r="C73" s="1">
         <f>SUM(C5:C72)</f>
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D73" s="1">
         <f t="shared" ref="D73" si="123">SUM(I73,N73,S73,X73,AC73,AH73,AM73,AR73,AW73,BB73,BG73,BL73,BQ73,BV73,CA73,CF73,CK73,CP73,CU73,CZ73,DE73,DJ73,DO73,DT73,DY73,ED73,EI73,EN73)</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E73" s="1">
         <f t="shared" ref="E73" si="124">SUM(J73,O73,T73,Y73,AD73,AI73,AN73,AS73,AX73,BC73,BH73,BM73,BR73,BW73,CB73,CG73,CL73,CQ73,CV73,DA73,DF73,DK73,DP73,DU73,DZ73,EE73,EJ73,EO73)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F73" s="1" t="str">
         <f>IF(C73,D73/C73*100,0) &amp; "%"</f>
-        <v>92.5925925925926%</v>
+        <v>0%</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="1">
@@ -33184,19 +33184,19 @@
       <c r="Q73" s="2"/>
       <c r="R73" s="1">
         <f t="shared" si="69"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="S73" s="1">
         <f>SUM(S5:S72)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T73" s="1">
         <f>SUM(T5:T72)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U73" s="1" t="str">
         <f t="shared" si="70"/>
-        <v>71.4285714285714%</v>
+        <v>0%</v>
       </c>
       <c r="V73" s="2"/>
       <c r="W73" s="1">
@@ -33286,11 +33286,11 @@
       <c r="AU73" s="2"/>
       <c r="AV73" s="1">
         <f t="shared" si="81"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AW73" s="1">
         <f>SUM(AW5:AW72)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AX73" s="1">
         <f>SUM(AX5:AX72)</f>
@@ -33298,7 +33298,7 @@
       </c>
       <c r="AY73" s="1" t="str">
         <f t="shared" si="82"/>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="AZ73" s="2"/>
       <c r="BA73" s="1">
@@ -38933,7 +38933,7 @@
       <c r="B87" s="5"/>
       <c r="C87" s="2">
         <f t="shared" si="127"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D87" s="2">
         <f t="shared" si="125"/>
@@ -38941,7 +38941,7 @@
       </c>
       <c r="E87" s="2">
         <f t="shared" si="125"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F87" s="2" t="str">
         <f t="shared" si="126"/>
@@ -38980,13 +38980,13 @@
       <c r="Q87" s="5"/>
       <c r="R87" s="2">
         <f t="shared" si="132"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S87" s="2">
         <v>0</v>
       </c>
       <c r="T87" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U87" s="2" t="str">
         <f t="shared" si="133"/>
@@ -42139,11 +42139,11 @@
       <c r="B94" s="5"/>
       <c r="C94" s="2">
         <f t="shared" si="127"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D94" s="2">
         <f t="shared" si="186"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E94" s="2">
         <f t="shared" si="187"/>
@@ -42151,7 +42151,7 @@
       </c>
       <c r="F94" s="2" t="str">
         <f t="shared" si="126"/>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="G94" s="5"/>
       <c r="H94" s="2">
@@ -42276,17 +42276,17 @@
       <c r="AU94" s="5"/>
       <c r="AV94" s="2">
         <f t="shared" si="144"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AW94" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AX94" s="2">
         <v>0</v>
       </c>
       <c r="AY94" s="2" t="str">
         <f t="shared" si="145"/>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="AZ94" s="5"/>
       <c r="BA94" s="2">
@@ -44429,19 +44429,19 @@
       <c r="B99" s="5"/>
       <c r="C99" s="2">
         <f t="shared" ref="C99:E99" si="188">SUM(H99,M99,R99,W99,AB99,AG99,AL99,AQ99,AV99,BA99,BF99,BK99,BP99,BU99,BZ99,CE99,CJ99,CO99,CT99,CY99,DD99,DI99,DN99,DS99,DX99,EC99,EH99,EM99)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D99" s="2">
         <f t="shared" si="188"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E99" s="2">
         <f t="shared" si="188"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F99" s="2" t="str">
         <f>IF(C99,D99/C99*100,0) &amp; "%"</f>
-        <v>83.3333333333333%</v>
+        <v>0%</v>
       </c>
       <c r="G99" s="5"/>
       <c r="H99" s="2">
@@ -44480,7 +44480,7 @@
       <c r="Q99" s="5"/>
       <c r="R99" s="2">
         <f t="shared" si="132"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S99" s="2">
         <f>SUM(S77:S98)</f>
@@ -44488,7 +44488,7 @@
       </c>
       <c r="T99" s="2">
         <f>SUM(T77:T98)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U99" s="2" t="str">
         <f>IF(R99,S99/R99*100,0) &amp; "%"</f>
@@ -44582,11 +44582,11 @@
       <c r="AU99" s="5"/>
       <c r="AV99" s="2">
         <f t="shared" si="144"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AW99" s="2">
         <f>SUM(AW77:AW98)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AX99" s="2">
         <f>SUM(AX77:AX98)</f>
@@ -44594,7 +44594,7 @@
       </c>
       <c r="AY99" s="2" t="str">
         <f>IF(AV99,AW99/AV99*100,0) &amp; "%"</f>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="AZ99" s="5"/>
       <c r="BA99" s="2">
@@ -45258,7 +45258,7 @@
       <c r="E102" s="9"/>
       <c r="F102" s="9" t="str">
         <f>IF(SUM(D73,D99),SUM(D73,D99)*100/SUM(C73,C99),0) &amp; "%"</f>
-        <v>90.9090909090909%</v>
+        <v>0%</v>
       </c>
       <c r="G102" s="10"/>
       <c r="H102" s="9" t="s">
@@ -45288,7 +45288,7 @@
       <c r="T102" s="9"/>
       <c r="U102" s="9" t="str">
         <f>IF(SUM(S73,S99),SUM(S73,S99)*100/SUM(R73,R99),0) &amp; "%"</f>
-        <v>62.5%</v>
+        <v>0%</v>
       </c>
       <c r="V102" s="10"/>
       <c r="W102" s="9" t="s">
@@ -45348,7 +45348,7 @@
       <c r="AX102" s="9"/>
       <c r="AY102" s="9" t="str">
         <f>IF(SUM(AW73,AW99),SUM(AW73,AW99)*100/SUM(AV73,AV99),0) &amp; "%"</f>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="AZ102" s="10"/>
       <c r="BA102" s="9" t="s">
@@ -49469,11 +49469,11 @@
       <c r="B113" s="8"/>
       <c r="C113" s="7">
         <f t="shared" si="191"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D113" s="7">
         <f t="shared" si="189"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E113" s="7">
         <f t="shared" si="189"/>
@@ -49481,7 +49481,7 @@
       </c>
       <c r="F113" s="7" t="str">
         <f t="shared" si="190"/>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="G113" s="8"/>
       <c r="H113" s="7">
@@ -49516,17 +49516,17 @@
       <c r="Q113" s="8"/>
       <c r="R113" s="7">
         <f t="shared" si="196"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S113" s="7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T113" s="7">
         <v>0</v>
       </c>
       <c r="U113" s="7" t="str">
         <f t="shared" si="197"/>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="V113" s="8"/>
       <c r="W113" s="7">
@@ -56339,11 +56339,11 @@
       <c r="B128" s="8"/>
       <c r="C128" s="7">
         <f t="shared" si="191"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D128" s="7">
         <f t="shared" si="250"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E128" s="7">
         <f t="shared" si="251"/>
@@ -56351,7 +56351,7 @@
       </c>
       <c r="F128" s="7" t="str">
         <f t="shared" si="190"/>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="G128" s="8"/>
       <c r="H128" s="7">
@@ -56476,17 +56476,17 @@
       <c r="AU128" s="8"/>
       <c r="AV128" s="7">
         <f t="shared" si="208"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW128" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX128" s="7">
         <v>0</v>
       </c>
       <c r="AY128" s="7" t="str">
         <f t="shared" si="209"/>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="AZ128" s="8"/>
       <c r="BA128" s="7">
@@ -57255,11 +57255,11 @@
       <c r="B130" s="8"/>
       <c r="C130" s="7">
         <f>SUM(C106:C129)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D130" s="7">
         <f>SUM(D106:D129)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E130" s="7">
         <f>SUM(E106:E129)</f>
@@ -57267,7 +57267,7 @@
       </c>
       <c r="F130" s="7" t="str">
         <f>IF(C130,D130/C130*100,0) &amp; "%"</f>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="G130" s="8"/>
       <c r="H130" s="7">
@@ -57306,11 +57306,11 @@
       <c r="Q130" s="8"/>
       <c r="R130" s="7">
         <f>SUM(R106:R129)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S130" s="7">
         <f>SUM(S106:S129)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T130" s="7">
         <f>SUM(T106:T129)</f>
@@ -57318,7 +57318,7 @@
       </c>
       <c r="U130" s="7" t="str">
         <f>IF(R130,S130/R130*100,0) &amp; "%"</f>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="V130" s="8"/>
       <c r="W130" s="7">
@@ -57408,11 +57408,11 @@
       <c r="AU130" s="8"/>
       <c r="AV130" s="7">
         <f>SUM(AV106:AV129)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW130" s="7">
         <f>SUM(AW106:AW129)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX130" s="7">
         <f>SUM(AX106:AX129)</f>
@@ -57420,7 +57420,7 @@
       </c>
       <c r="AY130" s="7" t="str">
         <f>IF(AV130,AW130/AV130*100,0) &amp; "%"</f>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="AZ130" s="8"/>
       <c r="BA130" s="7">
@@ -58933,7 +58933,7 @@
       <c r="B135" s="11"/>
       <c r="C135" s="12">
         <f t="shared" ref="C135:C152" si="254">SUM(H135,M135,R135,W135,AB135,AG135,AL135,AQ135,AV135,BA135,BF135,BK135,BP135,BU135,BZ135,CE135,CJ135,CO135,CT135,CY135,DD135,DI135,DN135,DS135,DX135,EC135,EH135,EM135,ER135)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D135" s="12">
         <f t="shared" si="252"/>
@@ -58941,7 +58941,7 @@
       </c>
       <c r="E135" s="12">
         <f t="shared" si="252"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F135" s="13" t="str">
         <f t="shared" si="253"/>
@@ -58980,13 +58980,13 @@
       <c r="Q135" s="11"/>
       <c r="R135" s="12">
         <f t="shared" ref="R135:R152" si="259">+SUM(S135,T135)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S135" s="13">
         <v>0</v>
       </c>
       <c r="T135" s="13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U135" s="13" t="str">
         <f t="shared" ref="U135:U152" si="260">IF(R135,S135/R135*100,0) &amp; "%"</f>
@@ -65345,11 +65345,11 @@
       <c r="B149" s="11"/>
       <c r="C149" s="12">
         <f t="shared" si="254"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D149" s="12">
         <f t="shared" si="252"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E149" s="12">
         <f t="shared" si="252"/>
@@ -65357,7 +65357,7 @@
       </c>
       <c r="F149" s="13" t="str">
         <f t="shared" si="253"/>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="G149" s="11"/>
       <c r="H149" s="12">
@@ -65482,17 +65482,17 @@
       <c r="AU149" s="11"/>
       <c r="AV149" s="12">
         <f t="shared" si="271"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW149" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX149" s="13">
         <v>0</v>
       </c>
       <c r="AY149" s="13" t="str">
         <f t="shared" si="272"/>
-        <v>100%</v>
+        <v>0%</v>
       </c>
       <c r="AZ149" s="11"/>
       <c r="BA149" s="12">
@@ -67175,25 +67175,25 @@
         <v>98</v>
       </c>
       <c r="B153" s="11"/>
-      <c r="C153" s="12">
-        <f>SUM(C134:C151)</f>
-        <v>3</v>
+      <c r="C153" s="13">
+        <f>SUM(C134:C152)</f>
+        <v>0</v>
       </c>
       <c r="D153" s="12">
         <f>SUM(D134:D151)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E153" s="12">
         <f>SUM(E134:E151)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F153" s="13" t="str">
         <f>IF(C153,D153/C153*100,0) &amp; "%"</f>
-        <v>33.3333333333333%</v>
+        <v>0%</v>
       </c>
       <c r="G153" s="11"/>
       <c r="H153" s="13">
-        <f>SUM(H129:H152)</f>
+        <f>SUM(H134:H152)</f>
         <v>0</v>
       </c>
       <c r="I153" s="12">
@@ -67210,7 +67210,7 @@
       </c>
       <c r="L153" s="11"/>
       <c r="M153" s="13">
-        <f>SUM(M129:M152)</f>
+        <f>SUM(M134:M152)</f>
         <v>0</v>
       </c>
       <c r="N153" s="12">
@@ -67227,8 +67227,8 @@
       </c>
       <c r="Q153" s="11"/>
       <c r="R153" s="13">
-        <f>SUM(R129:R152)</f>
-        <v>5</v>
+        <f>SUM(R134:R152)</f>
+        <v>0</v>
       </c>
       <c r="S153" s="12">
         <f>SUM(S134:S151)</f>
@@ -67236,7 +67236,7 @@
       </c>
       <c r="T153" s="12">
         <f>SUM(T134:T151)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U153" s="13" t="str">
         <f>IF(R153,S153/R153*100,0) &amp; "%"</f>
@@ -67244,7 +67244,7 @@
       </c>
       <c r="V153" s="11"/>
       <c r="W153" s="13">
-        <f>SUM(W129:W152)</f>
+        <f>SUM(W134:W152)</f>
         <v>0</v>
       </c>
       <c r="X153" s="12">
@@ -67261,7 +67261,7 @@
       </c>
       <c r="AA153" s="11"/>
       <c r="AB153" s="13">
-        <f>SUM(AB129:AB152)</f>
+        <f>SUM(AB134:AB152)</f>
         <v>0</v>
       </c>
       <c r="AC153" s="12">
@@ -67278,7 +67278,7 @@
       </c>
       <c r="AF153" s="11"/>
       <c r="AG153" s="13">
-        <f>SUM(AG129:AG152)</f>
+        <f>SUM(AG134:AG152)</f>
         <v>0</v>
       </c>
       <c r="AH153" s="12">
@@ -67295,7 +67295,7 @@
       </c>
       <c r="AK153" s="11"/>
       <c r="AL153" s="13">
-        <f>SUM(AL129:AL152)</f>
+        <f>SUM(AL134:AL152)</f>
         <v>0</v>
       </c>
       <c r="AM153" s="12">
@@ -67312,7 +67312,7 @@
       </c>
       <c r="AP153" s="11"/>
       <c r="AQ153" s="13">
-        <f>SUM(AQ129:AQ152)</f>
+        <f>SUM(AQ134:AQ152)</f>
         <v>0</v>
       </c>
       <c r="AR153" s="12">
@@ -67329,12 +67329,12 @@
       </c>
       <c r="AU153" s="11"/>
       <c r="AV153" s="13">
-        <f>SUM(AV129:AV152)</f>
-        <v>2</v>
+        <f>SUM(AV134:AV152)</f>
+        <v>0</v>
       </c>
       <c r="AW153" s="12">
         <f>SUM(AW134:AW151)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX153" s="12">
         <f>SUM(AX134:AX151)</f>
@@ -67342,11 +67342,11 @@
       </c>
       <c r="AY153" s="13" t="str">
         <f>IF(AV153,AW153/AV153*100,0) &amp; "%"</f>
-        <v>50%</v>
+        <v>0%</v>
       </c>
       <c r="AZ153" s="11"/>
       <c r="BA153" s="13">
-        <f>SUM(BA129:BA152)</f>
+        <f>SUM(BA134:BA152)</f>
         <v>0</v>
       </c>
       <c r="BB153" s="12">
@@ -67363,7 +67363,7 @@
       </c>
       <c r="BE153" s="11"/>
       <c r="BF153" s="13">
-        <f>SUM(BF129:BF152)</f>
+        <f>SUM(BF134:BF152)</f>
         <v>0</v>
       </c>
       <c r="BG153" s="12">
@@ -67380,7 +67380,7 @@
       </c>
       <c r="BJ153" s="11"/>
       <c r="BK153" s="13">
-        <f>SUM(BK129:BK152)</f>
+        <f>SUM(BK134:BK152)</f>
         <v>0</v>
       </c>
       <c r="BL153" s="12">
@@ -67397,7 +67397,7 @@
       </c>
       <c r="BO153" s="11"/>
       <c r="BP153" s="13">
-        <f>SUM(BP129:BP152)</f>
+        <f>SUM(BP134:BP152)</f>
         <v>0</v>
       </c>
       <c r="BQ153" s="12">
@@ -67414,7 +67414,7 @@
       </c>
       <c r="BT153" s="11"/>
       <c r="BU153" s="13">
-        <f>SUM(BU129:BU152)</f>
+        <f>SUM(BU134:BU152)</f>
         <v>0</v>
       </c>
       <c r="BV153" s="12">
@@ -67431,7 +67431,7 @@
       </c>
       <c r="BY153" s="11"/>
       <c r="BZ153" s="13">
-        <f>SUM(BZ129:BZ152)</f>
+        <f>SUM(BZ134:BZ152)</f>
         <v>0</v>
       </c>
       <c r="CA153" s="12">
@@ -67448,7 +67448,7 @@
       </c>
       <c r="CD153" s="11"/>
       <c r="CE153" s="13">
-        <f>SUM(CE129:CE152)</f>
+        <f>SUM(CE134:CE152)</f>
         <v>0</v>
       </c>
       <c r="CF153" s="12">
@@ -67465,7 +67465,7 @@
       </c>
       <c r="CI153" s="11"/>
       <c r="CJ153" s="13">
-        <f>SUM(CJ129:CJ152)</f>
+        <f>SUM(CJ134:CJ152)</f>
         <v>0</v>
       </c>
       <c r="CK153" s="12">
@@ -67482,7 +67482,7 @@
       </c>
       <c r="CN153" s="11"/>
       <c r="CO153" s="13">
-        <f>SUM(CO129:CO152)</f>
+        <f>SUM(CO134:CO152)</f>
         <v>0</v>
       </c>
       <c r="CP153" s="12">
@@ -67499,7 +67499,7 @@
       </c>
       <c r="CS153" s="11"/>
       <c r="CT153" s="13">
-        <f>SUM(CT129:CT152)</f>
+        <f>SUM(CT134:CT152)</f>
         <v>0</v>
       </c>
       <c r="CU153" s="12">
@@ -67516,7 +67516,7 @@
       </c>
       <c r="CX153" s="11"/>
       <c r="CY153" s="13">
-        <f>SUM(CY129:CY152)</f>
+        <f>SUM(CY134:CY152)</f>
         <v>0</v>
       </c>
       <c r="CZ153" s="12">
@@ -67533,7 +67533,7 @@
       </c>
       <c r="DC153" s="11"/>
       <c r="DD153" s="13">
-        <f>SUM(DD129:DD152)</f>
+        <f>SUM(DD134:DD152)</f>
         <v>0</v>
       </c>
       <c r="DE153" s="12">
@@ -67550,7 +67550,7 @@
       </c>
       <c r="DH153" s="11"/>
       <c r="DI153" s="13">
-        <f>SUM(DI129:DI152)</f>
+        <f>SUM(DI134:DI152)</f>
         <v>0</v>
       </c>
       <c r="DJ153" s="12">
@@ -67567,7 +67567,7 @@
       </c>
       <c r="DM153" s="11"/>
       <c r="DN153" s="13">
-        <f>SUM(DN129:DN152)</f>
+        <f>SUM(DN134:DN152)</f>
         <v>0</v>
       </c>
       <c r="DO153" s="12">
@@ -67584,7 +67584,7 @@
       </c>
       <c r="DR153" s="11"/>
       <c r="DS153" s="13">
-        <f>SUM(DS129:DS152)</f>
+        <f>SUM(DS134:DS152)</f>
         <v>0</v>
       </c>
       <c r="DT153" s="12">
@@ -67601,7 +67601,7 @@
       </c>
       <c r="DW153" s="11"/>
       <c r="DX153" s="13">
-        <f>SUM(DX129:DX152)</f>
+        <f>SUM(DX134:DX152)</f>
         <v>0</v>
       </c>
       <c r="DY153" s="12">
@@ -67618,7 +67618,7 @@
       </c>
       <c r="EB153" s="11"/>
       <c r="EC153" s="13">
-        <f>SUM(EC129:EC152)</f>
+        <f>SUM(EC134:EC152)</f>
         <v>0</v>
       </c>
       <c r="ED153" s="12">
@@ -67635,7 +67635,7 @@
       </c>
       <c r="EG153" s="11"/>
       <c r="EH153" s="13">
-        <f>SUM(EH129:EH152)</f>
+        <f>SUM(EH134:EH152)</f>
         <v>0</v>
       </c>
       <c r="EI153" s="12">
@@ -67652,7 +67652,7 @@
       </c>
       <c r="EL153" s="11"/>
       <c r="EM153" s="13">
-        <f>SUM(EM129:EM152)</f>
+        <f>SUM(EM134:EM152)</f>
         <v>0</v>
       </c>
       <c r="EN153" s="12">
@@ -67669,7 +67669,7 @@
       </c>
       <c r="EQ153" s="14"/>
       <c r="ER153" s="13">
-        <f>SUM(ER129:ER152)</f>
+        <f>SUM(ER134:ER152)</f>
         <v>0</v>
       </c>
       <c r="ES153" s="12">
@@ -68006,7 +68006,7 @@
       <c r="E156" s="9"/>
       <c r="F156" s="9" t="str">
         <f>IF(SUM(D130,D153),SUM(D130,D153)*100/SUM(C130,C153),0) &amp; "%"</f>
-        <v>71.4285714285714%</v>
+        <v>0%</v>
       </c>
       <c r="G156" s="10"/>
       <c r="H156" s="9" t="s">
@@ -68036,7 +68036,7 @@
       <c r="T156" s="9"/>
       <c r="U156" s="9" t="str">
         <f>IF(SUM(S130,S153),SUM(S130,S153)*100/SUM(R130,R153),0) &amp; "%"</f>
-        <v>37.5%</v>
+        <v>0%</v>
       </c>
       <c r="V156" s="10"/>
       <c r="W156" s="9" t="s">
@@ -68096,7 +68096,7 @@
       <c r="AX156" s="9"/>
       <c r="AY156" s="9" t="str">
         <f>IF(SUM(AW130,AW153),SUM(AW130,AW153)*100/SUM(AV130,AV153),0) &amp; "%"</f>
-        <v>66.6666666666667%</v>
+        <v>0%</v>
       </c>
       <c r="AZ156" s="10"/>
       <c r="BA156" s="9" t="s">
@@ -68310,7 +68310,7 @@
       <c r="E157" s="9"/>
       <c r="F157" s="9" t="str">
         <f>((F156 + F102)/2)*100 &amp; "%"</f>
-        <v>81.1688311688311%</v>
+        <v>0%</v>
       </c>
       <c r="G157" s="10"/>
       <c r="H157" s="9" t="s">
@@ -68340,7 +68340,7 @@
       <c r="T157" s="9"/>
       <c r="U157" s="9" t="str">
         <f>((U156 + U102)/2)*100 &amp; "%"</f>
-        <v>50%</v>
+        <v>0%</v>
       </c>
       <c r="V157" s="10"/>
       <c r="W157" s="9" t="s">
@@ -68400,7 +68400,7 @@
       <c r="AX157" s="9"/>
       <c r="AY157" s="9" t="str">
         <f>((AY156 + AY102)/2)*100 &amp; "%"</f>
-        <v>83.3333333333333%</v>
+        <v>0%</v>
       </c>
       <c r="AZ157" s="10"/>
       <c r="BA157" s="9" t="s">
@@ -68919,6 +68919,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d74e12c9-bdf3-447e-ac63-b8aa30cb912e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006D6901F31B669244A77CF3DC592DC06F" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f07ba37d9f6a9a16ab78a3833be08f3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d74e12c9-bdf3-447e-ac63-b8aa30cb912e" xmlns:ns4="7ce3718d-1d19-4340-bc07-211e3ea25757" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3d76b4510715f63c0dd84a4bd0fa290f" ns3:_="" ns4:_="">
     <xsd:import namespace="d74e12c9-bdf3-447e-ac63-b8aa30cb912e"/>
@@ -69133,14 +69141,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d74e12c9-bdf3-447e-ac63-b8aa30cb912e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -69151,6 +69151,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E2E85D4-37C6-4843-9D21-AD40AB5F6E3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d74e12c9-bdf3-447e-ac63-b8aa30cb912e"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7ce3718d-1d19-4340-bc07-211e3ea25757"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D93BBC3-F948-4065-9078-5D0662F77D28}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -69169,23 +69186,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E2E85D4-37C6-4843-9D21-AD40AB5F6E3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d74e12c9-bdf3-447e-ac63-b8aa30cb912e"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7ce3718d-1d19-4340-bc07-211e3ea25757"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF8F943-7811-4141-8F4E-8FF466B07D87}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
added start of update roles function
</commit_message>
<xml_diff>
--- a/BotC-Stats.xlsx
+++ b/BotC-Stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rainb\Documents\code\BotC-GroupTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB4D034-6272-418A-995C-A80AE3E90E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9D6CB0-3C09-41F0-9699-9C355B4258C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{6A883E2E-6B2D-4BEF-9626-D6F4FED911C1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="180">
   <si>
     <t>Players</t>
   </si>
@@ -574,6 +574,9 @@
   <si>
     <t>Total Average win%</t>
   </si>
+  <si>
+    <t>Total Played</t>
+  </si>
 </sst>
 </file>
 
@@ -1043,13 +1046,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8A5E5A-9AF3-4435-B5F4-E9654445F5CB}">
-  <dimension ref="A1:EV159"/>
+  <dimension ref="A1:EV160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B125" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P162" sqref="P162"/>
+      <selection pane="bottomRight" activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2905,11 +2908,11 @@
       <c r="B7" s="2"/>
       <c r="C7" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
@@ -2917,7 +2920,7 @@
       </c>
       <c r="F7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="1">
@@ -2952,17 +2955,17 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="S7" s="1">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="T7" s="1">
         <v>0</v>
       </c>
       <c r="U7" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="V7" s="2"/>
       <c r="W7" s="1">
@@ -33133,11 +33136,11 @@
       <c r="B73" s="2"/>
       <c r="C73" s="1">
         <f>SUM(C5:C72)</f>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="D73" s="1">
         <f t="shared" ref="D73" si="123">SUM(I73,N73,S73,X73,AC73,AH73,AM73,AR73,AW73,BB73,BG73,BL73,BQ73,BV73,CA73,CF73,CK73,CP73,CU73,CZ73,DE73,DJ73,DO73,DT73,DY73,ED73,EI73,EN73)</f>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="E73" s="1">
         <f t="shared" ref="E73" si="124">SUM(J73,O73,T73,Y73,AD73,AI73,AN73,AS73,AX73,BC73,BH73,BM73,BR73,BW73,CB73,CG73,CL73,CQ73,CV73,DA73,DF73,DK73,DP73,DU73,DZ73,EE73,EJ73,EO73)</f>
@@ -33145,7 +33148,7 @@
       </c>
       <c r="F73" s="1" t="str">
         <f>IF(C73,D73/C73*100,0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="1">
@@ -33184,11 +33187,11 @@
       <c r="Q73" s="2"/>
       <c r="R73" s="1">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="S73" s="1">
         <f>SUM(S5:S72)</f>
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="T73" s="1">
         <f>SUM(T5:T72)</f>
@@ -33196,7 +33199,7 @@
       </c>
       <c r="U73" s="1" t="str">
         <f t="shared" si="70"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="V73" s="2"/>
       <c r="W73" s="1">
@@ -45258,7 +45261,7 @@
       <c r="E102" s="9"/>
       <c r="F102" s="9" t="str">
         <f>IF(SUM(D73,D99),SUM(D73,D99)*100/SUM(C73,C99),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G102" s="10"/>
       <c r="H102" s="9" t="s">
@@ -45288,7 +45291,7 @@
       <c r="T102" s="9"/>
       <c r="U102" s="9" t="str">
         <f>IF(SUM(S73,S99),SUM(S73,S99)*100/SUM(R73,R99),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="V102" s="10"/>
       <c r="W102" s="9" t="s">
@@ -68310,7 +68313,7 @@
       <c r="E157" s="9"/>
       <c r="F157" s="9" t="str">
         <f>((F156 + F102)/2)*100 &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="G157" s="10"/>
       <c r="H157" s="9" t="s">
@@ -68340,7 +68343,7 @@
       <c r="T157" s="9"/>
       <c r="U157" s="9" t="str">
         <f>((U156 + U102)/2)*100 &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="V157" s="10"/>
       <c r="W157" s="9" t="s">
@@ -68605,157 +68608,307 @@
       <c r="EV157" s="3"/>
     </row>
     <row r="158" spans="1:152" x14ac:dyDescent="0.25">
-      <c r="A158" s="3"/>
-      <c r="B158" s="3"/>
-      <c r="C158" s="3"/>
-      <c r="D158" s="3"/>
-      <c r="E158" s="3"/>
-      <c r="F158" s="3"/>
-      <c r="G158" s="3"/>
-      <c r="H158" s="3"/>
-      <c r="I158" s="3"/>
-      <c r="J158" s="3"/>
-      <c r="K158" s="3"/>
-      <c r="L158" s="3"/>
-      <c r="M158" s="3"/>
-      <c r="N158" s="3"/>
-      <c r="O158" s="3"/>
-      <c r="P158" s="3"/>
-      <c r="Q158" s="3"/>
-      <c r="R158" s="3"/>
-      <c r="S158" s="3"/>
-      <c r="T158" s="3"/>
-      <c r="U158" s="3"/>
-      <c r="V158" s="3"/>
-      <c r="W158" s="3"/>
-      <c r="X158" s="3"/>
-      <c r="Y158" s="3"/>
-      <c r="Z158" s="3"/>
-      <c r="AA158" s="3"/>
-      <c r="AB158" s="3"/>
-      <c r="AC158" s="3"/>
-      <c r="AD158" s="3"/>
-      <c r="AE158" s="3"/>
-      <c r="AF158" s="3"/>
-      <c r="AG158" s="3"/>
-      <c r="AH158" s="3"/>
-      <c r="AI158" s="3"/>
-      <c r="AJ158" s="3"/>
-      <c r="AK158" s="3"/>
-      <c r="AL158" s="3"/>
-      <c r="AM158" s="3"/>
-      <c r="AN158" s="3"/>
-      <c r="AO158" s="3"/>
-      <c r="AP158" s="3"/>
-      <c r="AQ158" s="3"/>
-      <c r="AR158" s="3"/>
-      <c r="AS158" s="3"/>
-      <c r="AT158" s="3"/>
-      <c r="AU158" s="3"/>
-      <c r="AV158" s="3"/>
-      <c r="AW158" s="3"/>
-      <c r="AX158" s="3"/>
-      <c r="AY158" s="3"/>
-      <c r="AZ158" s="3"/>
-      <c r="BA158" s="3"/>
-      <c r="BB158" s="3"/>
-      <c r="BC158" s="3"/>
-      <c r="BD158" s="3"/>
-      <c r="BE158" s="3"/>
-      <c r="BF158" s="3"/>
-      <c r="BG158" s="3"/>
-      <c r="BH158" s="3"/>
-      <c r="BI158" s="3"/>
-      <c r="BJ158" s="3"/>
-      <c r="BK158" s="3"/>
-      <c r="BL158" s="3"/>
-      <c r="BM158" s="3"/>
-      <c r="BN158" s="3"/>
-      <c r="BO158" s="3"/>
-      <c r="BP158" s="3"/>
-      <c r="BQ158" s="3"/>
-      <c r="BR158" s="3"/>
-      <c r="BS158" s="3"/>
-      <c r="BT158" s="3"/>
-      <c r="BU158" s="3"/>
-      <c r="BV158" s="3"/>
-      <c r="BW158" s="3"/>
-      <c r="BX158" s="3"/>
-      <c r="BY158" s="3"/>
-      <c r="BZ158" s="3"/>
-      <c r="CA158" s="3"/>
-      <c r="CB158" s="3"/>
-      <c r="CC158" s="3"/>
-      <c r="CD158" s="3"/>
-      <c r="CE158" s="3"/>
-      <c r="CF158" s="3"/>
-      <c r="CG158" s="3"/>
-      <c r="CH158" s="3"/>
-      <c r="CI158" s="3"/>
-      <c r="CJ158" s="3"/>
-      <c r="CK158" s="3"/>
-      <c r="CL158" s="3"/>
-      <c r="CM158" s="3"/>
-      <c r="CN158" s="3"/>
-      <c r="CO158" s="3"/>
-      <c r="CP158" s="3"/>
-      <c r="CQ158" s="3"/>
-      <c r="CR158" s="3"/>
-      <c r="CS158" s="3"/>
-      <c r="CT158" s="3"/>
-      <c r="CU158" s="3"/>
-      <c r="CV158" s="3"/>
-      <c r="CW158" s="3"/>
-      <c r="CX158" s="3"/>
-      <c r="CY158" s="3"/>
-      <c r="CZ158" s="3"/>
-      <c r="DA158" s="3"/>
-      <c r="DB158" s="3"/>
-      <c r="DC158" s="3"/>
-      <c r="DD158" s="3"/>
-      <c r="DE158" s="3"/>
-      <c r="DF158" s="3"/>
-      <c r="DG158" s="3"/>
-      <c r="DH158" s="3"/>
-      <c r="DI158" s="3"/>
-      <c r="DJ158" s="3"/>
-      <c r="DK158" s="3"/>
-      <c r="DL158" s="3"/>
-      <c r="DM158" s="3"/>
-      <c r="DN158" s="3"/>
-      <c r="DO158" s="3"/>
-      <c r="DP158" s="3"/>
-      <c r="DQ158" s="3"/>
-      <c r="DR158" s="3"/>
-      <c r="DS158" s="3"/>
-      <c r="DT158" s="3"/>
-      <c r="DU158" s="3"/>
-      <c r="DV158" s="3"/>
-      <c r="DW158" s="3"/>
-      <c r="DX158" s="3"/>
-      <c r="DY158" s="3"/>
-      <c r="DZ158" s="3"/>
-      <c r="EA158" s="3"/>
-      <c r="EB158" s="3"/>
-      <c r="EC158" s="3"/>
-      <c r="ED158" s="3"/>
-      <c r="EE158" s="3"/>
-      <c r="EF158" s="3"/>
-      <c r="EG158" s="3"/>
-      <c r="EH158" s="3"/>
-      <c r="EI158" s="3"/>
-      <c r="EJ158" s="3"/>
-      <c r="EK158" s="3"/>
-      <c r="EL158" s="3"/>
-      <c r="EM158" s="3"/>
-      <c r="EN158" s="3"/>
-      <c r="EO158" s="3"/>
-      <c r="EP158" s="3"/>
-      <c r="EQ158" s="3"/>
-      <c r="ER158" s="3"/>
-      <c r="ES158" s="3"/>
-      <c r="ET158" s="3"/>
-      <c r="EU158" s="3"/>
+      <c r="A158" s="9"/>
+      <c r="B158" s="10"/>
+      <c r="C158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D158" s="9"/>
+      <c r="E158" s="9"/>
+      <c r="F158" s="9">
+        <f>+SUM(C153,C130,C99,C73)</f>
+        <v>61</v>
+      </c>
+      <c r="G158" s="10"/>
+      <c r="H158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="I158" s="9"/>
+      <c r="J158" s="9"/>
+      <c r="K158" s="9">
+        <f>+SUM(H153,H130,H99,H73)</f>
+        <v>0</v>
+      </c>
+      <c r="L158" s="10"/>
+      <c r="M158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="N158" s="9"/>
+      <c r="O158" s="9"/>
+      <c r="P158" s="9">
+        <f>+SUM(M153,M130,M99,M73)</f>
+        <v>0</v>
+      </c>
+      <c r="Q158" s="10"/>
+      <c r="R158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="S158" s="9"/>
+      <c r="T158" s="9"/>
+      <c r="U158" s="9">
+        <f>+SUM(R153,R130,R99,R73)</f>
+        <v>61</v>
+      </c>
+      <c r="V158" s="10"/>
+      <c r="W158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="X158" s="9"/>
+      <c r="Y158" s="9"/>
+      <c r="Z158" s="9">
+        <f>+SUM(W153,W130,W99,W73)</f>
+        <v>0</v>
+      </c>
+      <c r="AA158" s="10"/>
+      <c r="AB158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="AC158" s="9"/>
+      <c r="AD158" s="9"/>
+      <c r="AE158" s="9">
+        <f>+SUM(AB153,AB130,AB99,AB73)</f>
+        <v>0</v>
+      </c>
+      <c r="AF158" s="10"/>
+      <c r="AG158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="AH158" s="9"/>
+      <c r="AI158" s="9"/>
+      <c r="AJ158" s="9">
+        <f>+SUM(AG153,AG130,AG99,AG73)</f>
+        <v>0</v>
+      </c>
+      <c r="AK158" s="10"/>
+      <c r="AL158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="AM158" s="9"/>
+      <c r="AN158" s="9"/>
+      <c r="AO158" s="9">
+        <f>+SUM(AL153,AL130,AL99,AL73)</f>
+        <v>0</v>
+      </c>
+      <c r="AP158" s="10"/>
+      <c r="AQ158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="AR158" s="9"/>
+      <c r="AS158" s="9"/>
+      <c r="AT158" s="9">
+        <f>+SUM(AQ153,AQ130,AQ99,AQ73)</f>
+        <v>0</v>
+      </c>
+      <c r="AU158" s="10"/>
+      <c r="AV158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="AW158" s="9"/>
+      <c r="AX158" s="9"/>
+      <c r="AY158" s="9">
+        <f>+SUM(AV153,AV130,AV99,AV73)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ158" s="10"/>
+      <c r="BA158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="BB158" s="9"/>
+      <c r="BC158" s="9"/>
+      <c r="BD158" s="9">
+        <f>+SUM(BA153,BA130,BA99,BA73)</f>
+        <v>0</v>
+      </c>
+      <c r="BE158" s="10"/>
+      <c r="BF158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="BG158" s="9"/>
+      <c r="BH158" s="9"/>
+      <c r="BI158" s="9">
+        <f>+SUM(BF153,BF130,BF99,BF73)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ158" s="10"/>
+      <c r="BK158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="BL158" s="9"/>
+      <c r="BM158" s="9"/>
+      <c r="BN158" s="9">
+        <f>+SUM(BK153,BK130,BK99,BK73)</f>
+        <v>0</v>
+      </c>
+      <c r="BO158" s="10"/>
+      <c r="BP158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="BQ158" s="9"/>
+      <c r="BR158" s="9"/>
+      <c r="BS158" s="9">
+        <f>+SUM(BP153,BP130,BP99,BP73)</f>
+        <v>0</v>
+      </c>
+      <c r="BT158" s="10"/>
+      <c r="BU158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="BV158" s="9"/>
+      <c r="BW158" s="9"/>
+      <c r="BX158" s="9">
+        <f>+SUM(BU153,BU130,BU99,BU73)</f>
+        <v>0</v>
+      </c>
+      <c r="BY158" s="10"/>
+      <c r="BZ158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="CA158" s="9"/>
+      <c r="CB158" s="9"/>
+      <c r="CC158" s="9">
+        <f>+SUM(BZ153,BZ130,BZ99,BZ73)</f>
+        <v>0</v>
+      </c>
+      <c r="CD158" s="10"/>
+      <c r="CE158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="CF158" s="9"/>
+      <c r="CG158" s="9"/>
+      <c r="CH158" s="9">
+        <f>+SUM(CE153,CE130,CE99,CE73)</f>
+        <v>0</v>
+      </c>
+      <c r="CI158" s="10"/>
+      <c r="CJ158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="CK158" s="9"/>
+      <c r="CL158" s="9"/>
+      <c r="CM158" s="9">
+        <f>+SUM(CJ153,CJ130,CJ99,CJ73)</f>
+        <v>0</v>
+      </c>
+      <c r="CN158" s="10"/>
+      <c r="CO158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="CP158" s="9"/>
+      <c r="CQ158" s="9"/>
+      <c r="CR158" s="9">
+        <f>+SUM(CO153,CO130,CO99,CO73)</f>
+        <v>0</v>
+      </c>
+      <c r="CS158" s="10"/>
+      <c r="CT158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="CU158" s="9"/>
+      <c r="CV158" s="9"/>
+      <c r="CW158" s="9">
+        <f>+SUM(CT153,CT130,CT99,CT73)</f>
+        <v>0</v>
+      </c>
+      <c r="CX158" s="10"/>
+      <c r="CY158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="CZ158" s="9"/>
+      <c r="DA158" s="9"/>
+      <c r="DB158" s="9">
+        <f>+SUM(CY153,CY130,CY99,CY73)</f>
+        <v>0</v>
+      </c>
+      <c r="DC158" s="10"/>
+      <c r="DD158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="DE158" s="9"/>
+      <c r="DF158" s="9"/>
+      <c r="DG158" s="9">
+        <f>+SUM(DD153,DD130,DD99,DD73)</f>
+        <v>0</v>
+      </c>
+      <c r="DH158" s="10"/>
+      <c r="DI158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="DJ158" s="9"/>
+      <c r="DK158" s="9"/>
+      <c r="DL158" s="9">
+        <f>+SUM(DI153,DI130,DI99,DI73)</f>
+        <v>0</v>
+      </c>
+      <c r="DM158" s="10"/>
+      <c r="DN158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="DO158" s="9"/>
+      <c r="DP158" s="9"/>
+      <c r="DQ158" s="9">
+        <f>+SUM(DN153,DN130,DN99,DN73)</f>
+        <v>0</v>
+      </c>
+      <c r="DR158" s="10"/>
+      <c r="DS158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="DT158" s="9"/>
+      <c r="DU158" s="9"/>
+      <c r="DV158" s="9">
+        <f>+SUM(DS153,DS130,DS99,DS73)</f>
+        <v>0</v>
+      </c>
+      <c r="DW158" s="10"/>
+      <c r="DX158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="DY158" s="9"/>
+      <c r="DZ158" s="9"/>
+      <c r="EA158" s="9">
+        <f>+SUM(DX153,DX130,DX99,DX73)</f>
+        <v>0</v>
+      </c>
+      <c r="EB158" s="10"/>
+      <c r="EC158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="ED158" s="9"/>
+      <c r="EE158" s="9"/>
+      <c r="EF158" s="9">
+        <f>+SUM(EC153,EC130,EC99,EC73)</f>
+        <v>0</v>
+      </c>
+      <c r="EG158" s="10"/>
+      <c r="EH158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="EI158" s="9"/>
+      <c r="EJ158" s="9"/>
+      <c r="EK158" s="9">
+        <f>+SUM(EH153,EH130,EH99,EH73)</f>
+        <v>0</v>
+      </c>
+      <c r="EL158" s="10"/>
+      <c r="EM158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="EN158" s="9"/>
+      <c r="EO158" s="9"/>
+      <c r="EP158" s="9">
+        <f>+SUM(EM153,EM130,EM99,EM73)</f>
+        <v>0</v>
+      </c>
+      <c r="EQ158" s="15"/>
+      <c r="ER158" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="ES158" s="9"/>
+      <c r="ET158" s="9"/>
+      <c r="EU158" s="9">
+        <f>+SUM(ER153,ER130,ER99,ER73)</f>
+        <v>0</v>
+      </c>
       <c r="EV158" s="3"/>
     </row>
     <row r="159" spans="1:152" x14ac:dyDescent="0.25">
@@ -68912,6 +69065,160 @@
       <c r="EU159" s="3"/>
       <c r="EV159" s="3"/>
     </row>
+    <row r="160" spans="1:152" x14ac:dyDescent="0.25">
+      <c r="A160" s="3"/>
+      <c r="B160" s="3"/>
+      <c r="C160" s="3"/>
+      <c r="D160" s="3"/>
+      <c r="E160" s="3"/>
+      <c r="F160" s="3"/>
+      <c r="G160" s="3"/>
+      <c r="H160" s="3"/>
+      <c r="I160" s="3"/>
+      <c r="J160" s="3"/>
+      <c r="K160" s="3"/>
+      <c r="L160" s="3"/>
+      <c r="M160" s="3"/>
+      <c r="N160" s="3"/>
+      <c r="O160" s="3"/>
+      <c r="P160" s="3"/>
+      <c r="Q160" s="3"/>
+      <c r="R160" s="3"/>
+      <c r="S160" s="3"/>
+      <c r="T160" s="3"/>
+      <c r="U160" s="3"/>
+      <c r="V160" s="3"/>
+      <c r="W160" s="3"/>
+      <c r="X160" s="3"/>
+      <c r="Y160" s="3"/>
+      <c r="Z160" s="3"/>
+      <c r="AA160" s="3"/>
+      <c r="AB160" s="3"/>
+      <c r="AC160" s="3"/>
+      <c r="AD160" s="3"/>
+      <c r="AE160" s="3"/>
+      <c r="AF160" s="3"/>
+      <c r="AG160" s="3"/>
+      <c r="AH160" s="3"/>
+      <c r="AI160" s="3"/>
+      <c r="AJ160" s="3"/>
+      <c r="AK160" s="3"/>
+      <c r="AL160" s="3"/>
+      <c r="AM160" s="3"/>
+      <c r="AN160" s="3"/>
+      <c r="AO160" s="3"/>
+      <c r="AP160" s="3"/>
+      <c r="AQ160" s="3"/>
+      <c r="AR160" s="3"/>
+      <c r="AS160" s="3"/>
+      <c r="AT160" s="3"/>
+      <c r="AU160" s="3"/>
+      <c r="AV160" s="3"/>
+      <c r="AW160" s="3"/>
+      <c r="AX160" s="3"/>
+      <c r="AY160" s="3"/>
+      <c r="AZ160" s="3"/>
+      <c r="BA160" s="3"/>
+      <c r="BB160" s="3"/>
+      <c r="BC160" s="3"/>
+      <c r="BD160" s="3"/>
+      <c r="BE160" s="3"/>
+      <c r="BF160" s="3"/>
+      <c r="BG160" s="3"/>
+      <c r="BH160" s="3"/>
+      <c r="BI160" s="3"/>
+      <c r="BJ160" s="3"/>
+      <c r="BK160" s="3"/>
+      <c r="BL160" s="3"/>
+      <c r="BM160" s="3"/>
+      <c r="BN160" s="3"/>
+      <c r="BO160" s="3"/>
+      <c r="BP160" s="3"/>
+      <c r="BQ160" s="3"/>
+      <c r="BR160" s="3"/>
+      <c r="BS160" s="3"/>
+      <c r="BT160" s="3"/>
+      <c r="BU160" s="3"/>
+      <c r="BV160" s="3"/>
+      <c r="BW160" s="3"/>
+      <c r="BX160" s="3"/>
+      <c r="BY160" s="3"/>
+      <c r="BZ160" s="3"/>
+      <c r="CA160" s="3"/>
+      <c r="CB160" s="3"/>
+      <c r="CC160" s="3"/>
+      <c r="CD160" s="3"/>
+      <c r="CE160" s="3"/>
+      <c r="CF160" s="3"/>
+      <c r="CG160" s="3"/>
+      <c r="CH160" s="3"/>
+      <c r="CI160" s="3"/>
+      <c r="CJ160" s="3"/>
+      <c r="CK160" s="3"/>
+      <c r="CL160" s="3"/>
+      <c r="CM160" s="3"/>
+      <c r="CN160" s="3"/>
+      <c r="CO160" s="3"/>
+      <c r="CP160" s="3"/>
+      <c r="CQ160" s="3"/>
+      <c r="CR160" s="3"/>
+      <c r="CS160" s="3"/>
+      <c r="CT160" s="3"/>
+      <c r="CU160" s="3"/>
+      <c r="CV160" s="3"/>
+      <c r="CW160" s="3"/>
+      <c r="CX160" s="3"/>
+      <c r="CY160" s="3"/>
+      <c r="CZ160" s="3"/>
+      <c r="DA160" s="3"/>
+      <c r="DB160" s="3"/>
+      <c r="DC160" s="3"/>
+      <c r="DD160" s="3"/>
+      <c r="DE160" s="3"/>
+      <c r="DF160" s="3"/>
+      <c r="DG160" s="3"/>
+      <c r="DH160" s="3"/>
+      <c r="DI160" s="3"/>
+      <c r="DJ160" s="3"/>
+      <c r="DK160" s="3"/>
+      <c r="DL160" s="3"/>
+      <c r="DM160" s="3"/>
+      <c r="DN160" s="3"/>
+      <c r="DO160" s="3"/>
+      <c r="DP160" s="3"/>
+      <c r="DQ160" s="3"/>
+      <c r="DR160" s="3"/>
+      <c r="DS160" s="3"/>
+      <c r="DT160" s="3"/>
+      <c r="DU160" s="3"/>
+      <c r="DV160" s="3"/>
+      <c r="DW160" s="3"/>
+      <c r="DX160" s="3"/>
+      <c r="DY160" s="3"/>
+      <c r="DZ160" s="3"/>
+      <c r="EA160" s="3"/>
+      <c r="EB160" s="3"/>
+      <c r="EC160" s="3"/>
+      <c r="ED160" s="3"/>
+      <c r="EE160" s="3"/>
+      <c r="EF160" s="3"/>
+      <c r="EG160" s="3"/>
+      <c r="EH160" s="3"/>
+      <c r="EI160" s="3"/>
+      <c r="EJ160" s="3"/>
+      <c r="EK160" s="3"/>
+      <c r="EL160" s="3"/>
+      <c r="EM160" s="3"/>
+      <c r="EN160" s="3"/>
+      <c r="EO160" s="3"/>
+      <c r="EP160" s="3"/>
+      <c r="EQ160" s="3"/>
+      <c r="ER160" s="3"/>
+      <c r="ES160" s="3"/>
+      <c r="ET160" s="3"/>
+      <c r="EU160" s="3"/>
+      <c r="EV160" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -68919,14 +69226,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d74e12c9-bdf3-447e-ac63-b8aa30cb912e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006D6901F31B669244A77CF3DC592DC06F" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f07ba37d9f6a9a16ab78a3833be08f3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d74e12c9-bdf3-447e-ac63-b8aa30cb912e" xmlns:ns4="7ce3718d-1d19-4340-bc07-211e3ea25757" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3d76b4510715f63c0dd84a4bd0fa290f" ns3:_="" ns4:_="">
     <xsd:import namespace="d74e12c9-bdf3-447e-ac63-b8aa30cb912e"/>
@@ -69141,6 +69440,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d74e12c9-bdf3-447e-ac63-b8aa30cb912e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -69151,23 +69458,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E2E85D4-37C6-4843-9D21-AD40AB5F6E3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d74e12c9-bdf3-447e-ac63-b8aa30cb912e"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7ce3718d-1d19-4340-bc07-211e3ea25757"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D93BBC3-F948-4065-9078-5D0662F77D28}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -69186,6 +69476,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E2E85D4-37C6-4843-9D21-AD40AB5F6E3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d74e12c9-bdf3-447e-ac63-b8aa30cb912e"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7ce3718d-1d19-4340-bc07-211e3ea25757"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF8F943-7811-4141-8F4E-8FF466B07D87}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
added new function and added getters to change when new roles/players are added
</commit_message>
<xml_diff>
--- a/BotC-Stats.xlsx
+++ b/BotC-Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rainb\Documents\code\BotC-GroupTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7ECE2CD-E455-4323-BF8B-4952BE732D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322EA92F-30EE-40E6-A63E-776AF9C67C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{6A883E2E-6B2D-4BEF-9626-D6F4FED911C1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6A883E2E-6B2D-4BEF-9626-D6F4FED911C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1065,23 +1065,23 @@
   <dimension ref="A1:EV164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="DR146" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="EU161" sqref="EU161"/>
+      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="7" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.75" customWidth="1"/>
+    <col min="2" max="7" width="15.25" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="88" max="92" width="15.42578125" customWidth="1"/>
-    <col min="93" max="97" width="14.140625" customWidth="1"/>
-    <col min="103" max="107" width="13.28515625" customWidth="1"/>
+    <col min="88" max="92" width="15.4140625" customWidth="1"/>
+    <col min="93" max="97" width="14.1640625" customWidth="1"/>
+    <col min="103" max="107" width="13.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:152">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1297,7 +1297,7 @@
       <c r="EU1" s="4"/>
       <c r="EV1" s="3"/>
     </row>
-    <row r="2" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:152">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1451,7 +1451,7 @@
       <c r="EU2" s="3"/>
       <c r="EV2" s="3"/>
     </row>
-    <row r="3" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:152">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1605,7 +1605,7 @@
       <c r="EU3" s="3"/>
       <c r="EV3" s="3"/>
     </row>
-    <row r="4" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:152">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="EV4" s="3"/>
     </row>
-    <row r="5" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:152">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -2459,7 +2459,7 @@
       </c>
       <c r="EV5" s="3"/>
     </row>
-    <row r="6" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:152">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="EV6" s="3"/>
     </row>
-    <row r="7" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:152">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -3375,7 +3375,7 @@
       </c>
       <c r="EV7" s="3"/>
     </row>
-    <row r="8" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:152">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -3833,7 +3833,7 @@
       </c>
       <c r="EV8" s="3"/>
     </row>
-    <row r="9" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:152">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="EV9" s="3"/>
     </row>
-    <row r="10" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:152">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -4749,7 +4749,7 @@
       </c>
       <c r="EV10" s="3"/>
     </row>
-    <row r="11" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:152">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -5207,7 +5207,7 @@
       </c>
       <c r="EV11" s="3"/>
     </row>
-    <row r="12" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:152">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -5665,7 +5665,7 @@
       </c>
       <c r="EV12" s="3"/>
     </row>
-    <row r="13" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:152">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -6123,7 +6123,7 @@
       </c>
       <c r="EV13" s="3"/>
     </row>
-    <row r="14" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:152">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -6581,7 +6581,7 @@
       </c>
       <c r="EV14" s="3"/>
     </row>
-    <row r="15" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:152">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -7039,7 +7039,7 @@
       </c>
       <c r="EV15" s="3"/>
     </row>
-    <row r="16" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:152">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
@@ -7497,7 +7497,7 @@
       </c>
       <c r="EV16" s="3"/>
     </row>
-    <row r="17" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:152">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
@@ -7955,7 +7955,7 @@
       </c>
       <c r="EV17" s="3"/>
     </row>
-    <row r="18" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:152">
       <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
@@ -8413,7 +8413,7 @@
       </c>
       <c r="EV18" s="3"/>
     </row>
-    <row r="19" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:152">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -8871,7 +8871,7 @@
       </c>
       <c r="EV19" s="3"/>
     </row>
-    <row r="20" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:152">
       <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
@@ -9329,7 +9329,7 @@
       </c>
       <c r="EV20" s="3"/>
     </row>
-    <row r="21" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:152">
       <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
@@ -9787,7 +9787,7 @@
       </c>
       <c r="EV21" s="3"/>
     </row>
-    <row r="22" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:152">
       <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
@@ -10245,7 +10245,7 @@
       </c>
       <c r="EV22" s="3"/>
     </row>
-    <row r="23" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:152">
       <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
@@ -10703,7 +10703,7 @@
       </c>
       <c r="EV23" s="3"/>
     </row>
-    <row r="24" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:152">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -11161,7 +11161,7 @@
       </c>
       <c r="EV24" s="3"/>
     </row>
-    <row r="25" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:152">
       <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
@@ -11619,7 +11619,7 @@
       </c>
       <c r="EV25" s="3"/>
     </row>
-    <row r="26" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:152">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
@@ -12077,7 +12077,7 @@
       </c>
       <c r="EV26" s="3"/>
     </row>
-    <row r="27" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:152">
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
@@ -12535,7 +12535,7 @@
       </c>
       <c r="EV27" s="3"/>
     </row>
-    <row r="28" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:152">
       <c r="A28" s="1" t="s">
         <v>50</v>
       </c>
@@ -12993,7 +12993,7 @@
       </c>
       <c r="EV28" s="3"/>
     </row>
-    <row r="29" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:152">
       <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
@@ -13451,7 +13451,7 @@
       </c>
       <c r="EV29" s="3"/>
     </row>
-    <row r="30" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:152">
       <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
@@ -13909,7 +13909,7 @@
       </c>
       <c r="EV30" s="3"/>
     </row>
-    <row r="31" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:152">
       <c r="A31" s="1" t="s">
         <v>52</v>
       </c>
@@ -14367,7 +14367,7 @@
       </c>
       <c r="EV31" s="3"/>
     </row>
-    <row r="32" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:152">
       <c r="A32" s="1" t="s">
         <v>53</v>
       </c>
@@ -14825,7 +14825,7 @@
       </c>
       <c r="EV32" s="3"/>
     </row>
-    <row r="33" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:152">
       <c r="A33" s="1" t="s">
         <v>54</v>
       </c>
@@ -15283,7 +15283,7 @@
       </c>
       <c r="EV33" s="3"/>
     </row>
-    <row r="34" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:152">
       <c r="A34" s="1" t="s">
         <v>56</v>
       </c>
@@ -15741,7 +15741,7 @@
       </c>
       <c r="EV34" s="3"/>
     </row>
-    <row r="35" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:152">
       <c r="A35" s="1" t="s">
         <v>57</v>
       </c>
@@ -16199,7 +16199,7 @@
       </c>
       <c r="EV35" s="3"/>
     </row>
-    <row r="36" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:152">
       <c r="A36" s="1" t="s">
         <v>58</v>
       </c>
@@ -16657,7 +16657,7 @@
       </c>
       <c r="EV36" s="3"/>
     </row>
-    <row r="37" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:152">
       <c r="A37" s="1" t="s">
         <v>59</v>
       </c>
@@ -17115,7 +17115,7 @@
       </c>
       <c r="EV37" s="3"/>
     </row>
-    <row r="38" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:152">
       <c r="A38" s="1" t="s">
         <v>60</v>
       </c>
@@ -17573,7 +17573,7 @@
       </c>
       <c r="EV38" s="3"/>
     </row>
-    <row r="39" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:152">
       <c r="A39" s="1" t="s">
         <v>61</v>
       </c>
@@ -18031,7 +18031,7 @@
       </c>
       <c r="EV39" s="3"/>
     </row>
-    <row r="40" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:152">
       <c r="A40" s="1" t="s">
         <v>62</v>
       </c>
@@ -18489,7 +18489,7 @@
       </c>
       <c r="EV40" s="3"/>
     </row>
-    <row r="41" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:152">
       <c r="A41" s="1" t="s">
         <v>63</v>
       </c>
@@ -18947,7 +18947,7 @@
       </c>
       <c r="EV41" s="3"/>
     </row>
-    <row r="42" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:152">
       <c r="A42" s="1" t="s">
         <v>64</v>
       </c>
@@ -19405,7 +19405,7 @@
       </c>
       <c r="EV42" s="3"/>
     </row>
-    <row r="43" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:152">
       <c r="A43" s="1" t="s">
         <v>65</v>
       </c>
@@ -19863,7 +19863,7 @@
       </c>
       <c r="EV43" s="3"/>
     </row>
-    <row r="44" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:152">
       <c r="A44" s="1" t="s">
         <v>66</v>
       </c>
@@ -20321,7 +20321,7 @@
       </c>
       <c r="EV44" s="3"/>
     </row>
-    <row r="45" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:152">
       <c r="A45" s="1" t="s">
         <v>67</v>
       </c>
@@ -20779,7 +20779,7 @@
       </c>
       <c r="EV45" s="3"/>
     </row>
-    <row r="46" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:152">
       <c r="A46" s="1" t="s">
         <v>68</v>
       </c>
@@ -21237,7 +21237,7 @@
       </c>
       <c r="EV46" s="3"/>
     </row>
-    <row r="47" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:152">
       <c r="A47" s="1" t="s">
         <v>69</v>
       </c>
@@ -21695,7 +21695,7 @@
       </c>
       <c r="EV47" s="3"/>
     </row>
-    <row r="48" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:152">
       <c r="A48" s="1" t="s">
         <v>70</v>
       </c>
@@ -22153,7 +22153,7 @@
       </c>
       <c r="EV48" s="3"/>
     </row>
-    <row r="49" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:152">
       <c r="A49" s="1" t="s">
         <v>71</v>
       </c>
@@ -22611,7 +22611,7 @@
       </c>
       <c r="EV49" s="3"/>
     </row>
-    <row r="50" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:152">
       <c r="A50" s="1" t="s">
         <v>72</v>
       </c>
@@ -23069,7 +23069,7 @@
       </c>
       <c r="EV50" s="3"/>
     </row>
-    <row r="51" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:152">
       <c r="A51" s="1" t="s">
         <v>73</v>
       </c>
@@ -23527,7 +23527,7 @@
       </c>
       <c r="EV51" s="3"/>
     </row>
-    <row r="52" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:152">
       <c r="A52" s="1" t="s">
         <v>74</v>
       </c>
@@ -23985,7 +23985,7 @@
       </c>
       <c r="EV52" s="3"/>
     </row>
-    <row r="53" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:152">
       <c r="A53" s="1" t="s">
         <v>75</v>
       </c>
@@ -24443,7 +24443,7 @@
       </c>
       <c r="EV53" s="3"/>
     </row>
-    <row r="54" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:152">
       <c r="A54" s="1" t="s">
         <v>76</v>
       </c>
@@ -24901,7 +24901,7 @@
       </c>
       <c r="EV54" s="3"/>
     </row>
-    <row r="55" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:152">
       <c r="A55" s="1" t="s">
         <v>77</v>
       </c>
@@ -25359,7 +25359,7 @@
       </c>
       <c r="EV55" s="3"/>
     </row>
-    <row r="56" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:152">
       <c r="A56" s="1" t="s">
         <v>78</v>
       </c>
@@ -25817,7 +25817,7 @@
       </c>
       <c r="EV56" s="3"/>
     </row>
-    <row r="57" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:152">
       <c r="A57" s="1" t="s">
         <v>79</v>
       </c>
@@ -26275,7 +26275,7 @@
       </c>
       <c r="EV57" s="3"/>
     </row>
-    <row r="58" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:152">
       <c r="A58" s="1" t="s">
         <v>80</v>
       </c>
@@ -26733,7 +26733,7 @@
       </c>
       <c r="EV58" s="3"/>
     </row>
-    <row r="59" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:152">
       <c r="A59" s="1" t="s">
         <v>81</v>
       </c>
@@ -27191,7 +27191,7 @@
       </c>
       <c r="EV59" s="3"/>
     </row>
-    <row r="60" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:152">
       <c r="A60" s="1" t="s">
         <v>82</v>
       </c>
@@ -27649,7 +27649,7 @@
       </c>
       <c r="EV60" s="3"/>
     </row>
-    <row r="61" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:152">
       <c r="A61" s="1" t="s">
         <v>83</v>
       </c>
@@ -28107,7 +28107,7 @@
       </c>
       <c r="EV61" s="3"/>
     </row>
-    <row r="62" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:152">
       <c r="A62" s="1" t="s">
         <v>84</v>
       </c>
@@ -28565,7 +28565,7 @@
       </c>
       <c r="EV62" s="3"/>
     </row>
-    <row r="63" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:152">
       <c r="A63" s="1" t="s">
         <v>85</v>
       </c>
@@ -29023,7 +29023,7 @@
       </c>
       <c r="EV63" s="3"/>
     </row>
-    <row r="64" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:152">
       <c r="A64" s="1" t="s">
         <v>86</v>
       </c>
@@ -29481,7 +29481,7 @@
       </c>
       <c r="EV64" s="3"/>
     </row>
-    <row r="65" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:152">
       <c r="A65" s="1" t="s">
         <v>87</v>
       </c>
@@ -29939,7 +29939,7 @@
       </c>
       <c r="EV65" s="3"/>
     </row>
-    <row r="66" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:152">
       <c r="A66" s="1" t="s">
         <v>88</v>
       </c>
@@ -30397,7 +30397,7 @@
       </c>
       <c r="EV66" s="3"/>
     </row>
-    <row r="67" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:152">
       <c r="A67" s="1" t="s">
         <v>89</v>
       </c>
@@ -30855,7 +30855,7 @@
       </c>
       <c r="EV67" s="3"/>
     </row>
-    <row r="68" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:152">
       <c r="A68" s="1" t="s">
         <v>90</v>
       </c>
@@ -31313,7 +31313,7 @@
       </c>
       <c r="EV68" s="3"/>
     </row>
-    <row r="69" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:152">
       <c r="A69" s="1" t="s">
         <v>91</v>
       </c>
@@ -31771,7 +31771,7 @@
       </c>
       <c r="EV69" s="3"/>
     </row>
-    <row r="70" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:152">
       <c r="A70" s="1" t="s">
         <v>92</v>
       </c>
@@ -32229,7 +32229,7 @@
       </c>
       <c r="EV70" s="3"/>
     </row>
-    <row r="71" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:152">
       <c r="A71" s="1" t="s">
         <v>93</v>
       </c>
@@ -32687,7 +32687,7 @@
       </c>
       <c r="EV71" s="3"/>
     </row>
-    <row r="72" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:152">
       <c r="A72" s="1" t="s">
         <v>94</v>
       </c>
@@ -33145,7 +33145,7 @@
       </c>
       <c r="EV72" s="3"/>
     </row>
-    <row r="73" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:152">
       <c r="A73" s="1" t="s">
         <v>180</v>
       </c>
@@ -33603,7 +33603,7 @@
       </c>
       <c r="EV73" s="3"/>
     </row>
-    <row r="74" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:152">
       <c r="A74" s="1" t="s">
         <v>95</v>
       </c>
@@ -34119,7 +34119,7 @@
       </c>
       <c r="EV74" s="3"/>
     </row>
-    <row r="75" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:152">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -34273,7 +34273,7 @@
       <c r="EU75" s="3"/>
       <c r="EV75" s="3"/>
     </row>
-    <row r="76" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:152">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -34427,7 +34427,7 @@
       <c r="EU76" s="3"/>
       <c r="EV76" s="3"/>
     </row>
-    <row r="77" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:152">
       <c r="A77" s="2" t="s">
         <v>100</v>
       </c>
@@ -34823,7 +34823,7 @@
       </c>
       <c r="EV77" s="3"/>
     </row>
-    <row r="78" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:152">
       <c r="A78" s="2" t="s">
         <v>101</v>
       </c>
@@ -35281,7 +35281,7 @@
       </c>
       <c r="EV78" s="3"/>
     </row>
-    <row r="79" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:152">
       <c r="A79" s="2" t="s">
         <v>102</v>
       </c>
@@ -35739,7 +35739,7 @@
       </c>
       <c r="EV79" s="3"/>
     </row>
-    <row r="80" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:152">
       <c r="A80" s="2" t="s">
         <v>103</v>
       </c>
@@ -36197,7 +36197,7 @@
       </c>
       <c r="EV80" s="3"/>
     </row>
-    <row r="81" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:152">
       <c r="A81" s="2" t="s">
         <v>104</v>
       </c>
@@ -36655,7 +36655,7 @@
       </c>
       <c r="EV81" s="3"/>
     </row>
-    <row r="82" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:152">
       <c r="A82" s="2" t="s">
         <v>105</v>
       </c>
@@ -37113,7 +37113,7 @@
       </c>
       <c r="EV82" s="3"/>
     </row>
-    <row r="83" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:152">
       <c r="A83" s="2" t="s">
         <v>106</v>
       </c>
@@ -37571,7 +37571,7 @@
       </c>
       <c r="EV83" s="3"/>
     </row>
-    <row r="84" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:152">
       <c r="A84" s="2" t="s">
         <v>107</v>
       </c>
@@ -38029,7 +38029,7 @@
       </c>
       <c r="EV84" s="3"/>
     </row>
-    <row r="85" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:152">
       <c r="A85" s="2" t="s">
         <v>108</v>
       </c>
@@ -38487,7 +38487,7 @@
       </c>
       <c r="EV85" s="3"/>
     </row>
-    <row r="86" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:152">
       <c r="A86" s="2" t="s">
         <v>109</v>
       </c>
@@ -38945,7 +38945,7 @@
       </c>
       <c r="EV86" s="3"/>
     </row>
-    <row r="87" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:152">
       <c r="A87" s="2" t="s">
         <v>110</v>
       </c>
@@ -39403,7 +39403,7 @@
       </c>
       <c r="EV87" s="3"/>
     </row>
-    <row r="88" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:152">
       <c r="A88" s="2" t="s">
         <v>111</v>
       </c>
@@ -39861,7 +39861,7 @@
       </c>
       <c r="EV88" s="3"/>
     </row>
-    <row r="89" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:152">
       <c r="A89" s="2" t="s">
         <v>112</v>
       </c>
@@ -40319,7 +40319,7 @@
       </c>
       <c r="EV89" s="3"/>
     </row>
-    <row r="90" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:152">
       <c r="A90" s="2" t="s">
         <v>113</v>
       </c>
@@ -40777,7 +40777,7 @@
       </c>
       <c r="EV90" s="3"/>
     </row>
-    <row r="91" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:152">
       <c r="A91" s="2" t="s">
         <v>114</v>
       </c>
@@ -41235,7 +41235,7 @@
       </c>
       <c r="EV91" s="3"/>
     </row>
-    <row r="92" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:152">
       <c r="A92" s="2" t="s">
         <v>115</v>
       </c>
@@ -41693,7 +41693,7 @@
       </c>
       <c r="EV92" s="3"/>
     </row>
-    <row r="93" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:152">
       <c r="A93" s="2" t="s">
         <v>116</v>
       </c>
@@ -42151,7 +42151,7 @@
       </c>
       <c r="EV93" s="3"/>
     </row>
-    <row r="94" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:152">
       <c r="A94" s="2" t="s">
         <v>117</v>
       </c>
@@ -42609,7 +42609,7 @@
       </c>
       <c r="EV94" s="3"/>
     </row>
-    <row r="95" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:152">
       <c r="A95" s="2" t="s">
         <v>118</v>
       </c>
@@ -43067,7 +43067,7 @@
       </c>
       <c r="EV95" s="3"/>
     </row>
-    <row r="96" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:152">
       <c r="A96" s="2" t="s">
         <v>119</v>
       </c>
@@ -43525,7 +43525,7 @@
       </c>
       <c r="EV96" s="3"/>
     </row>
-    <row r="97" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:152">
       <c r="A97" s="2" t="s">
         <v>120</v>
       </c>
@@ -43983,7 +43983,7 @@
       </c>
       <c r="EV97" s="3"/>
     </row>
-    <row r="98" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:152">
       <c r="A98" s="2" t="s">
         <v>121</v>
       </c>
@@ -44441,7 +44441,7 @@
       </c>
       <c r="EV98" s="3"/>
     </row>
-    <row r="99" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:152">
       <c r="A99" s="2" t="s">
         <v>122</v>
       </c>
@@ -44899,7 +44899,7 @@
       </c>
       <c r="EV99" s="3"/>
     </row>
-    <row r="100" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:152">
       <c r="A100" s="2" t="s">
         <v>181</v>
       </c>
@@ -45357,7 +45357,7 @@
       </c>
       <c r="EV100" s="3"/>
     </row>
-    <row r="101" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:152">
       <c r="A101" s="2" t="s">
         <v>95</v>
       </c>
@@ -45873,7 +45873,7 @@
       </c>
       <c r="EV101" s="3"/>
     </row>
-    <row r="102" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:152">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="6"/>
@@ -46027,7 +46027,7 @@
       <c r="EU102" s="3"/>
       <c r="EV102" s="3"/>
     </row>
-    <row r="103" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:152">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="6"/>
@@ -46181,7 +46181,7 @@
       <c r="EU103" s="3"/>
       <c r="EV103" s="3"/>
     </row>
-    <row r="104" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:152">
       <c r="A104" s="9" t="s">
         <v>172</v>
       </c>
@@ -46487,7 +46487,7 @@
       </c>
       <c r="EV104" s="3"/>
     </row>
-    <row r="105" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:152">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="6"/>
@@ -46641,7 +46641,7 @@
       <c r="EU105" s="3"/>
       <c r="EV105" s="3"/>
     </row>
-    <row r="106" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:152">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -46795,7 +46795,7 @@
       <c r="EU106" s="3"/>
       <c r="EV106" s="3"/>
     </row>
-    <row r="107" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:152">
       <c r="A107" s="7" t="s">
         <v>123</v>
       </c>
@@ -47191,7 +47191,7 @@
       </c>
       <c r="EV107" s="3"/>
     </row>
-    <row r="108" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:152">
       <c r="A108" s="7" t="s">
         <v>124</v>
       </c>
@@ -47649,7 +47649,7 @@
       </c>
       <c r="EV108" s="3"/>
     </row>
-    <row r="109" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:152">
       <c r="A109" s="7" t="s">
         <v>125</v>
       </c>
@@ -48107,7 +48107,7 @@
       </c>
       <c r="EV109" s="3"/>
     </row>
-    <row r="110" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:152">
       <c r="A110" s="7" t="s">
         <v>126</v>
       </c>
@@ -48565,7 +48565,7 @@
       </c>
       <c r="EV110" s="3"/>
     </row>
-    <row r="111" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:152">
       <c r="A111" s="7" t="s">
         <v>127</v>
       </c>
@@ -49023,7 +49023,7 @@
       </c>
       <c r="EV111" s="3"/>
     </row>
-    <row r="112" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:152">
       <c r="A112" s="7" t="s">
         <v>128</v>
       </c>
@@ -49481,7 +49481,7 @@
       </c>
       <c r="EV112" s="3"/>
     </row>
-    <row r="113" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:152">
       <c r="A113" s="7" t="s">
         <v>129</v>
       </c>
@@ -49939,7 +49939,7 @@
       </c>
       <c r="EV113" s="3"/>
     </row>
-    <row r="114" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:152">
       <c r="A114" s="7" t="s">
         <v>130</v>
       </c>
@@ -50397,7 +50397,7 @@
       </c>
       <c r="EV114" s="3"/>
     </row>
-    <row r="115" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:152">
       <c r="A115" s="7" t="s">
         <v>131</v>
       </c>
@@ -50855,7 +50855,7 @@
       </c>
       <c r="EV115" s="3"/>
     </row>
-    <row r="116" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:152">
       <c r="A116" s="7" t="s">
         <v>132</v>
       </c>
@@ -51313,7 +51313,7 @@
       </c>
       <c r="EV116" s="3"/>
     </row>
-    <row r="117" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:152">
       <c r="A117" s="7" t="s">
         <v>133</v>
       </c>
@@ -51771,7 +51771,7 @@
       </c>
       <c r="EV117" s="3"/>
     </row>
-    <row r="118" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:152">
       <c r="A118" s="7" t="s">
         <v>134</v>
       </c>
@@ -52229,7 +52229,7 @@
       </c>
       <c r="EV118" s="3"/>
     </row>
-    <row r="119" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:152">
       <c r="A119" s="7" t="s">
         <v>135</v>
       </c>
@@ -52687,7 +52687,7 @@
       </c>
       <c r="EV119" s="3"/>
     </row>
-    <row r="120" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:152">
       <c r="A120" s="7" t="s">
         <v>136</v>
       </c>
@@ -53145,7 +53145,7 @@
       </c>
       <c r="EV120" s="3"/>
     </row>
-    <row r="121" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:152">
       <c r="A121" s="7" t="s">
         <v>137</v>
       </c>
@@ -53603,7 +53603,7 @@
       </c>
       <c r="EV121" s="3"/>
     </row>
-    <row r="122" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:152">
       <c r="A122" s="7" t="s">
         <v>138</v>
       </c>
@@ -54061,7 +54061,7 @@
       </c>
       <c r="EV122" s="3"/>
     </row>
-    <row r="123" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:152">
       <c r="A123" s="7" t="s">
         <v>139</v>
       </c>
@@ -54519,7 +54519,7 @@
       </c>
       <c r="EV123" s="3"/>
     </row>
-    <row r="124" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:152">
       <c r="A124" s="7" t="s">
         <v>140</v>
       </c>
@@ -54977,7 +54977,7 @@
       </c>
       <c r="EV124" s="3"/>
     </row>
-    <row r="125" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:152">
       <c r="A125" s="7" t="s">
         <v>141</v>
       </c>
@@ -55435,7 +55435,7 @@
       </c>
       <c r="EV125" s="3"/>
     </row>
-    <row r="126" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:152">
       <c r="A126" s="7" t="s">
         <v>142</v>
       </c>
@@ -55893,7 +55893,7 @@
       </c>
       <c r="EV126" s="3"/>
     </row>
-    <row r="127" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:152">
       <c r="A127" s="7" t="s">
         <v>143</v>
       </c>
@@ -56351,7 +56351,7 @@
       </c>
       <c r="EV127" s="3"/>
     </row>
-    <row r="128" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:152">
       <c r="A128" s="7" t="s">
         <v>144</v>
       </c>
@@ -56809,7 +56809,7 @@
       </c>
       <c r="EV128" s="3"/>
     </row>
-    <row r="129" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:152">
       <c r="A129" s="7" t="s">
         <v>145</v>
       </c>
@@ -57267,7 +57267,7 @@
       </c>
       <c r="EV129" s="3"/>
     </row>
-    <row r="130" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:152">
       <c r="A130" s="7" t="s">
         <v>146</v>
       </c>
@@ -57725,7 +57725,7 @@
       </c>
       <c r="EV130" s="3"/>
     </row>
-    <row r="131" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:152">
       <c r="A131" s="7" t="s">
         <v>147</v>
       </c>
@@ -58183,7 +58183,7 @@
       </c>
       <c r="EV131" s="3"/>
     </row>
-    <row r="132" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:152">
       <c r="A132" s="7" t="s">
         <v>182</v>
       </c>
@@ -58641,7 +58641,7 @@
       </c>
       <c r="EV132" s="3"/>
     </row>
-    <row r="133" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:152">
       <c r="A133" s="7" t="s">
         <v>95</v>
       </c>
@@ -59157,7 +59157,7 @@
       </c>
       <c r="EV133" s="3"/>
     </row>
-    <row r="134" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:152">
       <c r="A134" s="3"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
@@ -59311,7 +59311,7 @@
       <c r="EU134" s="3"/>
       <c r="EV134" s="3"/>
     </row>
-    <row r="135" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:152">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
@@ -59465,7 +59465,7 @@
       <c r="EU135" s="3"/>
       <c r="EV135" s="3"/>
     </row>
-    <row r="136" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:152">
       <c r="A136" s="12" t="s">
         <v>149</v>
       </c>
@@ -59861,7 +59861,7 @@
       </c>
       <c r="EV136" s="3"/>
     </row>
-    <row r="137" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:152">
       <c r="A137" s="12" t="s">
         <v>150</v>
       </c>
@@ -60319,7 +60319,7 @@
       </c>
       <c r="EV137" s="3"/>
     </row>
-    <row r="138" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:152">
       <c r="A138" s="12" t="s">
         <v>151</v>
       </c>
@@ -60777,7 +60777,7 @@
       </c>
       <c r="EV138" s="3"/>
     </row>
-    <row r="139" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:152">
       <c r="A139" s="12" t="s">
         <v>152</v>
       </c>
@@ -61235,7 +61235,7 @@
       </c>
       <c r="EV139" s="3"/>
     </row>
-    <row r="140" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:152">
       <c r="A140" s="12" t="s">
         <v>153</v>
       </c>
@@ -61693,7 +61693,7 @@
       </c>
       <c r="EV140" s="3"/>
     </row>
-    <row r="141" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:152">
       <c r="A141" s="12" t="s">
         <v>154</v>
       </c>
@@ -62151,7 +62151,7 @@
       </c>
       <c r="EV141" s="3"/>
     </row>
-    <row r="142" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:152">
       <c r="A142" s="12" t="s">
         <v>155</v>
       </c>
@@ -62609,7 +62609,7 @@
       </c>
       <c r="EV142" s="3"/>
     </row>
-    <row r="143" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:152">
       <c r="A143" s="12" t="s">
         <v>156</v>
       </c>
@@ -63067,7 +63067,7 @@
       </c>
       <c r="EV143" s="3"/>
     </row>
-    <row r="144" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:152">
       <c r="A144" s="12" t="s">
         <v>157</v>
       </c>
@@ -63525,7 +63525,7 @@
       </c>
       <c r="EV144" s="3"/>
     </row>
-    <row r="145" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:152">
       <c r="A145" s="12" t="s">
         <v>158</v>
       </c>
@@ -63983,7 +63983,7 @@
       </c>
       <c r="EV145" s="3"/>
     </row>
-    <row r="146" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:152">
       <c r="A146" s="12" t="s">
         <v>159</v>
       </c>
@@ -64441,7 +64441,7 @@
       </c>
       <c r="EV146" s="3"/>
     </row>
-    <row r="147" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:152">
       <c r="A147" s="12" t="s">
         <v>160</v>
       </c>
@@ -64899,7 +64899,7 @@
       </c>
       <c r="EV147" s="3"/>
     </row>
-    <row r="148" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:152">
       <c r="A148" s="12" t="s">
         <v>161</v>
       </c>
@@ -65357,7 +65357,7 @@
       </c>
       <c r="EV148" s="3"/>
     </row>
-    <row r="149" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:152">
       <c r="A149" s="12" t="s">
         <v>162</v>
       </c>
@@ -65815,7 +65815,7 @@
       </c>
       <c r="EV149" s="3"/>
     </row>
-    <row r="150" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:152">
       <c r="A150" s="12" t="s">
         <v>163</v>
       </c>
@@ -66273,7 +66273,7 @@
       </c>
       <c r="EV150" s="3"/>
     </row>
-    <row r="151" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:152">
       <c r="A151" s="12" t="s">
         <v>164</v>
       </c>
@@ -66731,7 +66731,7 @@
       </c>
       <c r="EV151" s="3"/>
     </row>
-    <row r="152" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:152">
       <c r="A152" s="12" t="s">
         <v>165</v>
       </c>
@@ -67189,7 +67189,7 @@
       </c>
       <c r="EV152" s="3"/>
     </row>
-    <row r="153" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:152">
       <c r="A153" s="12" t="s">
         <v>166</v>
       </c>
@@ -67647,7 +67647,7 @@
       </c>
       <c r="EV153" s="3"/>
     </row>
-    <row r="154" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:152">
       <c r="A154" s="12" t="s">
         <v>167</v>
       </c>
@@ -68105,7 +68105,7 @@
       </c>
       <c r="EV154" s="3"/>
     </row>
-    <row r="155" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:152">
       <c r="A155" s="12" t="s">
         <v>168</v>
       </c>
@@ -68563,7 +68563,7 @@
       </c>
       <c r="EV155" s="3"/>
     </row>
-    <row r="156" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:152">
       <c r="A156" s="12" t="s">
         <v>183</v>
       </c>
@@ -69021,7 +69021,7 @@
       </c>
       <c r="EV156" s="3"/>
     </row>
-    <row r="157" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:152">
       <c r="A157" s="12" t="s">
         <v>95</v>
       </c>
@@ -69536,7 +69536,7 @@
       </c>
       <c r="EV157" s="3"/>
     </row>
-    <row r="158" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:152">
       <c r="A158" s="3"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
@@ -69690,7 +69690,7 @@
       <c r="EU158" s="3"/>
       <c r="EV158" s="3"/>
     </row>
-    <row r="159" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:152">
       <c r="A159" s="3"/>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
@@ -69844,7 +69844,7 @@
       <c r="EU159" s="3"/>
       <c r="EV159" s="3"/>
     </row>
-    <row r="160" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:152">
       <c r="A160" s="9" t="s">
         <v>172</v>
       </c>
@@ -70150,7 +70150,7 @@
       </c>
       <c r="EV160" s="3"/>
     </row>
-    <row r="161" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:152">
       <c r="A161" s="9"/>
       <c r="B161" s="10"/>
       <c r="C161" s="9" t="s">
@@ -70454,7 +70454,7 @@
       </c>
       <c r="EV161" s="3"/>
     </row>
-    <row r="162" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:152">
       <c r="A162" s="9"/>
       <c r="B162" s="10"/>
       <c r="C162" s="9" t="s">
@@ -70758,7 +70758,7 @@
       </c>
       <c r="EV162" s="3"/>
     </row>
-    <row r="163" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:152">
       <c r="A163" s="3"/>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
@@ -70912,7 +70912,7 @@
       <c r="EU163" s="3"/>
       <c r="EV163" s="3"/>
     </row>
-    <row r="164" spans="1:152" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:152">
       <c r="A164" s="3"/>
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
@@ -71073,6 +71073,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d74e12c9-bdf3-447e-ac63-b8aa30cb912e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006D6901F31B669244A77CF3DC592DC06F" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f07ba37d9f6a9a16ab78a3833be08f3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d74e12c9-bdf3-447e-ac63-b8aa30cb912e" xmlns:ns4="7ce3718d-1d19-4340-bc07-211e3ea25757" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3d76b4510715f63c0dd84a4bd0fa290f" ns3:_="" ns4:_="">
     <xsd:import namespace="d74e12c9-bdf3-447e-ac63-b8aa30cb912e"/>
@@ -71287,14 +71295,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d74e12c9-bdf3-447e-ac63-b8aa30cb912e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -71305,6 +71305,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E2E85D4-37C6-4843-9D21-AD40AB5F6E3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d74e12c9-bdf3-447e-ac63-b8aa30cb912e"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7ce3718d-1d19-4340-bc07-211e3ea25757"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D93BBC3-F948-4065-9078-5D0662F77D28}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -71323,23 +71340,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E2E85D4-37C6-4843-9D21-AD40AB5F6E3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d74e12c9-bdf3-447e-ac63-b8aa30cb912e"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7ce3718d-1d19-4340-bc07-211e3ea25757"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF8F943-7811-4141-8F4E-8FF466B07D87}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fixed Stats  in Spreadsheet
</commit_message>
<xml_diff>
--- a/BotC-Stats.xlsx
+++ b/BotC-Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rainb\Documents\code\BotC-GroupTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25A5377-B699-4561-BD10-FBC21F9682F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB4C0A5-47B7-4446-A266-FEAF3E334FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6A883E2E-6B2D-4BEF-9626-D6F4FED911C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{6A883E2E-6B2D-4BEF-9626-D6F4FED911C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -594,7 +594,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1062,23 +1062,23 @@
   <dimension ref="A1:EV164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="I76" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B122" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="U82" sqref="U82"/>
+      <selection pane="bottomRight" activeCell="G158" sqref="G158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.75" customWidth="1"/>
-    <col min="2" max="7" width="15.25" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="7" width="15.28515625" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="88" max="92" width="15.4140625" customWidth="1"/>
-    <col min="93" max="97" width="14.1640625" customWidth="1"/>
-    <col min="103" max="107" width="13.25" customWidth="1"/>
+    <col min="88" max="92" width="15.42578125" customWidth="1"/>
+    <col min="93" max="97" width="14.140625" customWidth="1"/>
+    <col min="103" max="107" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:152">
+    <row r="1" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1294,7 +1294,7 @@
       <c r="EU1" s="4"/>
       <c r="EV1" s="3"/>
     </row>
-    <row r="2" spans="1:152">
+    <row r="2" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1448,7 +1448,7 @@
       <c r="EU2" s="3"/>
       <c r="EV2" s="3"/>
     </row>
-    <row r="3" spans="1:152">
+    <row r="3" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1602,7 +1602,7 @@
       <c r="EU3" s="3"/>
       <c r="EV3" s="3"/>
     </row>
-    <row r="4" spans="1:152">
+    <row r="4" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1998,7 +1998,7 @@
       </c>
       <c r="EV4" s="3"/>
     </row>
-    <row r="5" spans="1:152">
+    <row r="5" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -2456,7 +2456,7 @@
       </c>
       <c r="EV5" s="3"/>
     </row>
-    <row r="6" spans="1:152">
+    <row r="6" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -2914,7 +2914,7 @@
       </c>
       <c r="EV6" s="3"/>
     </row>
-    <row r="7" spans="1:152">
+    <row r="7" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -3372,7 +3372,7 @@
       </c>
       <c r="EV7" s="3"/>
     </row>
-    <row r="8" spans="1:152">
+    <row r="8" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -3830,18 +3830,18 @@
       </c>
       <c r="EV8" s="3"/>
     </row>
-    <row r="9" spans="1:152">
+    <row r="9" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
@@ -3849,7 +3849,7 @@
       </c>
       <c r="F9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="1">
@@ -3929,17 +3929,17 @@
       <c r="AF9" s="2"/>
       <c r="AG9" s="1">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI9" s="1">
         <v>0</v>
       </c>
       <c r="AJ9" s="1" t="str">
         <f t="shared" si="14"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AK9" s="2"/>
       <c r="AL9" s="1">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="EV9" s="3"/>
     </row>
-    <row r="10" spans="1:152">
+    <row r="10" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -4746,7 +4746,7 @@
       </c>
       <c r="EV10" s="3"/>
     </row>
-    <row r="11" spans="1:152">
+    <row r="11" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -5204,7 +5204,7 @@
       </c>
       <c r="EV11" s="3"/>
     </row>
-    <row r="12" spans="1:152">
+    <row r="12" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -5662,7 +5662,7 @@
       </c>
       <c r="EV12" s="3"/>
     </row>
-    <row r="13" spans="1:152">
+    <row r="13" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -6120,7 +6120,7 @@
       </c>
       <c r="EV13" s="3"/>
     </row>
-    <row r="14" spans="1:152">
+    <row r="14" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -6578,7 +6578,7 @@
       </c>
       <c r="EV14" s="3"/>
     </row>
-    <row r="15" spans="1:152">
+    <row r="15" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -7036,7 +7036,7 @@
       </c>
       <c r="EV15" s="3"/>
     </row>
-    <row r="16" spans="1:152">
+    <row r="16" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
@@ -7494,7 +7494,7 @@
       </c>
       <c r="EV16" s="3"/>
     </row>
-    <row r="17" spans="1:152">
+    <row r="17" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
@@ -7952,7 +7952,7 @@
       </c>
       <c r="EV17" s="3"/>
     </row>
-    <row r="18" spans="1:152">
+    <row r="18" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
@@ -8410,7 +8410,7 @@
       </c>
       <c r="EV18" s="3"/>
     </row>
-    <row r="19" spans="1:152">
+    <row r="19" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -8868,7 +8868,7 @@
       </c>
       <c r="EV19" s="3"/>
     </row>
-    <row r="20" spans="1:152">
+    <row r="20" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
@@ -9326,7 +9326,7 @@
       </c>
       <c r="EV20" s="3"/>
     </row>
-    <row r="21" spans="1:152">
+    <row r="21" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
@@ -9784,7 +9784,7 @@
       </c>
       <c r="EV21" s="3"/>
     </row>
-    <row r="22" spans="1:152">
+    <row r="22" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
@@ -10242,7 +10242,7 @@
       </c>
       <c r="EV22" s="3"/>
     </row>
-    <row r="23" spans="1:152">
+    <row r="23" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
@@ -10700,7 +10700,7 @@
       </c>
       <c r="EV23" s="3"/>
     </row>
-    <row r="24" spans="1:152">
+    <row r="24" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -11158,7 +11158,7 @@
       </c>
       <c r="EV24" s="3"/>
     </row>
-    <row r="25" spans="1:152">
+    <row r="25" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
@@ -11616,14 +11616,14 @@
       </c>
       <c r="EV25" s="3"/>
     </row>
-    <row r="26" spans="1:152">
+    <row r="26" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" si="61"/>
@@ -11631,7 +11631,7 @@
       </c>
       <c r="E26" s="1">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F26" s="1" t="str">
         <f t="shared" si="2"/>
@@ -11655,13 +11655,13 @@
       <c r="L26" s="2"/>
       <c r="M26" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N26" s="1">
         <v>0</v>
       </c>
       <c r="O26" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P26" s="1" t="str">
         <f t="shared" si="6"/>
@@ -11700,13 +11700,13 @@
       <c r="AA26" s="2"/>
       <c r="AB26" s="1">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC26" s="1">
         <v>0</v>
       </c>
       <c r="AD26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE26" s="1" t="str">
         <f t="shared" si="12"/>
@@ -12074,26 +12074,26 @@
       </c>
       <c r="EV26" s="3"/>
     </row>
-    <row r="27" spans="1:152">
+    <row r="27" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="1">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="1">
@@ -12428,17 +12428,17 @@
       <c r="DM27" s="2"/>
       <c r="DN27" s="1">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="DO27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DP27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DQ27" s="1" t="str">
         <f t="shared" si="48"/>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="DR27" s="2"/>
       <c r="DS27" s="1">
@@ -12532,7 +12532,7 @@
       </c>
       <c r="EV27" s="3"/>
     </row>
-    <row r="28" spans="1:152">
+    <row r="28" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>50</v>
       </c>
@@ -12990,7 +12990,7 @@
       </c>
       <c r="EV28" s="3"/>
     </row>
-    <row r="29" spans="1:152">
+    <row r="29" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
@@ -13448,18 +13448,18 @@
       </c>
       <c r="EV29" s="3"/>
     </row>
-    <row r="30" spans="1:152">
+    <row r="30" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="1">
         <f t="shared" si="62"/>
@@ -13467,7 +13467,7 @@
       </c>
       <c r="F30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="1">
@@ -13892,40 +13892,40 @@
       <c r="EQ30" s="2"/>
       <c r="ER30" s="1">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ES30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ET30" s="1">
         <v>0</v>
       </c>
       <c r="EU30" s="1" t="str">
         <f t="shared" si="60"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="EV30" s="3"/>
     </row>
-    <row r="31" spans="1:152">
+    <row r="31" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="1">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="1">
@@ -13945,13 +13945,13 @@
       <c r="L31" s="2"/>
       <c r="M31" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N31" s="1">
         <v>0</v>
       </c>
       <c r="O31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P31" s="1" t="str">
         <f t="shared" si="6"/>
@@ -13975,17 +13975,17 @@
       <c r="V31" s="2"/>
       <c r="W31" s="1">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y31" s="1">
         <v>0</v>
       </c>
       <c r="Z31" s="1" t="str">
         <f t="shared" si="10"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AA31" s="2"/>
       <c r="AB31" s="1">
@@ -14364,7 +14364,7 @@
       </c>
       <c r="EV31" s="3"/>
     </row>
-    <row r="32" spans="1:152">
+    <row r="32" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>53</v>
       </c>
@@ -14822,18 +14822,18 @@
       </c>
       <c r="EV32" s="3"/>
     </row>
-    <row r="33" spans="1:152">
+    <row r="33" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="1">
         <f t="shared" si="62"/>
@@ -14841,7 +14841,7 @@
       </c>
       <c r="F33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="1">
@@ -14936,17 +14936,17 @@
       <c r="AK33" s="2"/>
       <c r="AL33" s="1">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM33" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN33" s="1">
         <v>0</v>
       </c>
       <c r="AO33" s="1" t="str">
         <f t="shared" si="16"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AP33" s="2"/>
       <c r="AQ33" s="1">
@@ -15280,14 +15280,14 @@
       </c>
       <c r="EV33" s="3"/>
     </row>
-    <row r="34" spans="1:152">
+    <row r="34" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" si="61"/>
@@ -15295,7 +15295,7 @@
       </c>
       <c r="E34" s="1">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F34" s="1" t="str">
         <f t="shared" si="2"/>
@@ -15334,13 +15334,13 @@
       <c r="Q34" s="2"/>
       <c r="R34" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S34" s="1">
         <v>0</v>
       </c>
       <c r="T34" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U34" s="1" t="str">
         <f t="shared" si="8"/>
@@ -15364,13 +15364,13 @@
       <c r="AA34" s="2"/>
       <c r="AB34" s="1">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC34" s="1">
         <v>0</v>
       </c>
       <c r="AD34" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE34" s="1" t="str">
         <f t="shared" si="12"/>
@@ -15738,7 +15738,7 @@
       </c>
       <c r="EV34" s="3"/>
     </row>
-    <row r="35" spans="1:152">
+    <row r="35" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>57</v>
       </c>
@@ -16196,18 +16196,18 @@
       </c>
       <c r="EV35" s="3"/>
     </row>
-    <row r="36" spans="1:152">
+    <row r="36" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" s="1">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" s="1">
         <f t="shared" si="62"/>
@@ -16215,7 +16215,7 @@
       </c>
       <c r="F36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="1">
@@ -16295,17 +16295,17 @@
       <c r="AF36" s="2"/>
       <c r="AG36" s="1">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH36" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI36" s="1">
         <v>0</v>
       </c>
       <c r="AJ36" s="1" t="str">
         <f t="shared" si="14"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AK36" s="2"/>
       <c r="AL36" s="1">
@@ -16654,7 +16654,7 @@
       </c>
       <c r="EV36" s="3"/>
     </row>
-    <row r="37" spans="1:152">
+    <row r="37" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>59</v>
       </c>
@@ -17112,14 +17112,14 @@
       </c>
       <c r="EV37" s="3"/>
     </row>
-    <row r="38" spans="1:152">
+    <row r="38" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D38" s="1">
         <f t="shared" si="61"/>
@@ -17127,7 +17127,7 @@
       </c>
       <c r="E38" s="1">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F38" s="1" t="str">
         <f t="shared" si="2"/>
@@ -17226,13 +17226,13 @@
       <c r="AK38" s="2"/>
       <c r="AL38" s="1">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM38" s="1">
         <v>0</v>
       </c>
       <c r="AN38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO38" s="1" t="str">
         <f t="shared" si="16"/>
@@ -17556,13 +17556,13 @@
       <c r="EQ38" s="2"/>
       <c r="ER38" s="1">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ES38" s="1">
         <v>0</v>
       </c>
       <c r="ET38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EU38" s="1" t="str">
         <f t="shared" si="60"/>
@@ -17570,7 +17570,7 @@
       </c>
       <c r="EV38" s="3"/>
     </row>
-    <row r="39" spans="1:152">
+    <row r="39" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>61</v>
       </c>
@@ -18028,7 +18028,7 @@
       </c>
       <c r="EV39" s="3"/>
     </row>
-    <row r="40" spans="1:152">
+    <row r="40" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>62</v>
       </c>
@@ -18486,7 +18486,7 @@
       </c>
       <c r="EV40" s="3"/>
     </row>
-    <row r="41" spans="1:152">
+    <row r="41" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>63</v>
       </c>
@@ -18944,7 +18944,7 @@
       </c>
       <c r="EV41" s="3"/>
     </row>
-    <row r="42" spans="1:152">
+    <row r="42" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>64</v>
       </c>
@@ -19402,7 +19402,7 @@
       </c>
       <c r="EV42" s="3"/>
     </row>
-    <row r="43" spans="1:152">
+    <row r="43" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>65</v>
       </c>
@@ -19860,7 +19860,7 @@
       </c>
       <c r="EV43" s="3"/>
     </row>
-    <row r="44" spans="1:152">
+    <row r="44" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>66</v>
       </c>
@@ -20318,7 +20318,7 @@
       </c>
       <c r="EV44" s="3"/>
     </row>
-    <row r="45" spans="1:152">
+    <row r="45" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>67</v>
       </c>
@@ -20776,7 +20776,7 @@
       </c>
       <c r="EV45" s="3"/>
     </row>
-    <row r="46" spans="1:152">
+    <row r="46" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>68</v>
       </c>
@@ -21234,26 +21234,26 @@
       </c>
       <c r="EV46" s="3"/>
     </row>
-    <row r="47" spans="1:152">
+    <row r="47" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D47" s="1">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" s="1">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F47" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0%</v>
+        <v>33.33%</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="1">
@@ -21633,13 +21633,13 @@
       <c r="EB47" s="2"/>
       <c r="EC47" s="1">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ED47" s="1">
         <v>0</v>
       </c>
       <c r="EE47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EF47" s="1" t="str">
         <f t="shared" si="54"/>
@@ -21678,21 +21678,21 @@
       <c r="EQ47" s="2"/>
       <c r="ER47" s="1">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="ES47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ET47" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EU47" s="1" t="str">
         <f t="shared" si="60"/>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="EV47" s="3"/>
     </row>
-    <row r="48" spans="1:152">
+    <row r="48" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>70</v>
       </c>
@@ -22150,7 +22150,7 @@
       </c>
       <c r="EV48" s="3"/>
     </row>
-    <row r="49" spans="1:152">
+    <row r="49" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>71</v>
       </c>
@@ -22608,7 +22608,7 @@
       </c>
       <c r="EV49" s="3"/>
     </row>
-    <row r="50" spans="1:152">
+    <row r="50" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>72</v>
       </c>
@@ -23066,7 +23066,7 @@
       </c>
       <c r="EV50" s="3"/>
     </row>
-    <row r="51" spans="1:152">
+    <row r="51" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>73</v>
       </c>
@@ -23524,7 +23524,7 @@
       </c>
       <c r="EV51" s="3"/>
     </row>
-    <row r="52" spans="1:152">
+    <row r="52" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>74</v>
       </c>
@@ -23982,7 +23982,7 @@
       </c>
       <c r="EV52" s="3"/>
     </row>
-    <row r="53" spans="1:152">
+    <row r="53" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>75</v>
       </c>
@@ -24440,7 +24440,7 @@
       </c>
       <c r="EV53" s="3"/>
     </row>
-    <row r="54" spans="1:152">
+    <row r="54" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>76</v>
       </c>
@@ -24898,7 +24898,7 @@
       </c>
       <c r="EV54" s="3"/>
     </row>
-    <row r="55" spans="1:152">
+    <row r="55" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>77</v>
       </c>
@@ -25356,18 +25356,18 @@
       </c>
       <c r="EV55" s="3"/>
     </row>
-    <row r="56" spans="1:152">
+    <row r="56" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56" s="1">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56" s="1">
         <f t="shared" si="62"/>
@@ -25375,7 +25375,7 @@
       </c>
       <c r="F56" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="1">
@@ -25710,17 +25710,17 @@
       <c r="DM56" s="2"/>
       <c r="DN56" s="1">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DO56" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DP56" s="1">
         <v>0</v>
       </c>
       <c r="DQ56" s="1" t="str">
         <f t="shared" si="48"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="DR56" s="2"/>
       <c r="DS56" s="1">
@@ -25814,7 +25814,7 @@
       </c>
       <c r="EV56" s="3"/>
     </row>
-    <row r="57" spans="1:152">
+    <row r="57" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>79</v>
       </c>
@@ -26272,7 +26272,7 @@
       </c>
       <c r="EV57" s="3"/>
     </row>
-    <row r="58" spans="1:152">
+    <row r="58" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>80</v>
       </c>
@@ -26730,18 +26730,18 @@
       </c>
       <c r="EV58" s="3"/>
     </row>
-    <row r="59" spans="1:152">
+    <row r="59" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59" s="1">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" s="1">
         <f t="shared" si="62"/>
@@ -26749,7 +26749,7 @@
       </c>
       <c r="F59" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="1">
@@ -26784,17 +26784,17 @@
       <c r="Q59" s="2"/>
       <c r="R59" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S59" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T59" s="1">
         <v>0</v>
       </c>
       <c r="U59" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="V59" s="2"/>
       <c r="W59" s="1">
@@ -27188,18 +27188,18 @@
       </c>
       <c r="EV59" s="3"/>
     </row>
-    <row r="60" spans="1:152">
+    <row r="60" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60" s="1">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" s="1">
         <f t="shared" si="62"/>
@@ -27207,7 +27207,7 @@
       </c>
       <c r="F60" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="1">
@@ -27242,17 +27242,17 @@
       <c r="Q60" s="2"/>
       <c r="R60" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S60" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T60" s="1">
         <v>0</v>
       </c>
       <c r="U60" s="1" t="str">
         <f t="shared" si="8"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="V60" s="2"/>
       <c r="W60" s="1">
@@ -27646,7 +27646,7 @@
       </c>
       <c r="EV60" s="3"/>
     </row>
-    <row r="61" spans="1:152">
+    <row r="61" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>83</v>
       </c>
@@ -28104,26 +28104,26 @@
       </c>
       <c r="EV61" s="3"/>
     </row>
-    <row r="62" spans="1:152">
+    <row r="62" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D62" s="1">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62" s="1">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F62" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0%</v>
+        <v>33.33%</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="1">
@@ -28188,17 +28188,17 @@
       <c r="AA62" s="2"/>
       <c r="AB62" s="1">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC62" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD62" s="1">
         <v>0</v>
       </c>
       <c r="AE62" s="1" t="str">
         <f t="shared" si="12"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AF62" s="2"/>
       <c r="AG62" s="1">
@@ -28233,13 +28233,13 @@
       <c r="AP62" s="2"/>
       <c r="AQ62" s="1">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR62" s="1">
         <v>0</v>
       </c>
       <c r="AS62" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT62" s="1" t="str">
         <f t="shared" si="18"/>
@@ -28562,14 +28562,14 @@
       </c>
       <c r="EV62" s="3"/>
     </row>
-    <row r="63" spans="1:152">
+    <row r="63" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D63" s="1">
         <f t="shared" si="61"/>
@@ -28577,7 +28577,7 @@
       </c>
       <c r="E63" s="1">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F63" s="1" t="str">
         <f t="shared" si="2"/>
@@ -28661,13 +28661,13 @@
       <c r="AF63" s="2"/>
       <c r="AG63" s="1">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH63" s="1">
         <v>0</v>
       </c>
       <c r="AI63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ63" s="1" t="str">
         <f t="shared" si="14"/>
@@ -28961,13 +28961,13 @@
       <c r="EB63" s="2"/>
       <c r="EC63" s="1">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ED63" s="1">
         <v>0</v>
       </c>
       <c r="EE63" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EF63" s="1" t="str">
         <f t="shared" si="54"/>
@@ -29020,7 +29020,7 @@
       </c>
       <c r="EV63" s="3"/>
     </row>
-    <row r="64" spans="1:152">
+    <row r="64" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>86</v>
       </c>
@@ -29478,7 +29478,7 @@
       </c>
       <c r="EV64" s="3"/>
     </row>
-    <row r="65" spans="1:152">
+    <row r="65" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>87</v>
       </c>
@@ -29936,7 +29936,7 @@
       </c>
       <c r="EV65" s="3"/>
     </row>
-    <row r="66" spans="1:152">
+    <row r="66" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>88</v>
       </c>
@@ -30394,18 +30394,18 @@
       </c>
       <c r="EV66" s="3"/>
     </row>
-    <row r="67" spans="1:152">
+    <row r="67" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67" s="1">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E67" s="1">
         <f t="shared" si="62"/>
@@ -30413,7 +30413,7 @@
       </c>
       <c r="F67" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="1">
@@ -30433,17 +30433,17 @@
       <c r="L67" s="2"/>
       <c r="M67" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N67" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O67" s="1">
         <v>0</v>
       </c>
       <c r="P67" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="Q67" s="2"/>
       <c r="R67" s="1">
@@ -30852,14 +30852,14 @@
       </c>
       <c r="EV67" s="3"/>
     </row>
-    <row r="68" spans="1:152">
+    <row r="68" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68" s="1">
         <f t="shared" si="61"/>
@@ -30867,7 +30867,7 @@
       </c>
       <c r="E68" s="1">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F68" s="1" t="str">
         <f t="shared" si="2"/>
@@ -30981,13 +30981,13 @@
       <c r="AP68" s="2"/>
       <c r="AQ68" s="1">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR68" s="1">
         <v>0</v>
       </c>
       <c r="AS68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT68" s="1" t="str">
         <f t="shared" si="18"/>
@@ -31310,7 +31310,7 @@
       </c>
       <c r="EV68" s="3"/>
     </row>
-    <row r="69" spans="1:152">
+    <row r="69" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>91</v>
       </c>
@@ -31768,7 +31768,7 @@
       </c>
       <c r="EV69" s="3"/>
     </row>
-    <row r="70" spans="1:152">
+    <row r="70" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>92</v>
       </c>
@@ -32226,14 +32226,14 @@
       </c>
       <c r="EV70" s="3"/>
     </row>
-    <row r="71" spans="1:152">
+    <row r="71" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="1">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D71" s="1">
         <f t="shared" si="61"/>
@@ -32241,7 +32241,7 @@
       </c>
       <c r="E71" s="1">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F71" s="1" t="str">
         <f t="shared" si="64"/>
@@ -32295,13 +32295,13 @@
       <c r="V71" s="2"/>
       <c r="W71" s="1">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X71" s="1">
         <v>0</v>
       </c>
       <c r="Y71" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z71" s="1" t="str">
         <f t="shared" si="72"/>
@@ -32684,7 +32684,7 @@
       </c>
       <c r="EV71" s="3"/>
     </row>
-    <row r="72" spans="1:152">
+    <row r="72" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>94</v>
       </c>
@@ -33142,101 +33142,101 @@
       </c>
       <c r="EV72" s="3"/>
     </row>
-    <row r="73" spans="1:152">
+    <row r="73" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>180</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="1">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D73" s="1">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E73" s="1">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F73" s="1" t="str">
         <f t="shared" si="64"/>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="1">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K73" s="1" t="str">
         <f t="shared" si="66"/>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="L73" s="2"/>
       <c r="M73" s="1">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N73" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O73" s="1">
         <v>0</v>
       </c>
       <c r="P73" s="1" t="str">
         <f t="shared" si="68"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="Q73" s="2"/>
       <c r="R73" s="1">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T73" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U73" s="1" t="str">
         <f t="shared" si="70"/>
-        <v>0%</v>
+        <v>33.33%</v>
       </c>
       <c r="V73" s="2"/>
       <c r="W73" s="1">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X73" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y73" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z73" s="1" t="str">
         <f t="shared" si="72"/>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="AA73" s="2"/>
       <c r="AB73" s="1">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AC73" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD73" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE73" s="1" t="str">
         <f t="shared" si="74"/>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="AF73" s="2"/>
       <c r="AG73" s="1">
@@ -33481,17 +33481,17 @@
       <c r="DH73" s="2"/>
       <c r="DI73" s="1">
         <f t="shared" si="107"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="DJ73" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DK73" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="DL73" s="1" t="str">
         <f t="shared" si="108"/>
-        <v>0%</v>
+        <v>33.33%</v>
       </c>
       <c r="DM73" s="2"/>
       <c r="DN73" s="1">
@@ -33600,150 +33600,150 @@
       </c>
       <c r="EV73" s="3"/>
     </row>
-    <row r="74" spans="1:152">
+    <row r="74" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="1">
         <f>SUM(C5:C73)</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="D74" s="1">
         <f t="shared" ref="D74:E74" si="123">SUM(D5:D73)</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E74" s="1">
         <f t="shared" si="123"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F74" s="1" t="str">
         <f>IF(C74,ROUND(D74/C74*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>44.68%</v>
       </c>
       <c r="G74" s="2"/>
       <c r="H74" s="1">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I74" s="1">
         <f>SUM(I5:I73)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J74" s="1">
         <f>SUM(J5:J73)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K74" s="1" t="str">
         <f>IF(H74,ROUND(I74/H74*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="L74" s="2"/>
       <c r="M74" s="1">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N74" s="1">
         <f>SUM(N5:N73)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O74" s="1">
         <f>SUM(O5:O73)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P74" s="1" t="str">
         <f>IF(M74,ROUND(N74/M74*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="Q74" s="2"/>
       <c r="R74" s="1">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="S74" s="1">
         <f>SUM(S5:S73)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T74" s="1">
         <f>SUM(T5:T73)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U74" s="1" t="str">
         <f>IF(R74,ROUND(S74/R74*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="V74" s="2"/>
       <c r="W74" s="1">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="X74" s="1">
         <f>SUM(X5:X73)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y74" s="1">
         <f>SUM(Y5:Y73)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z74" s="1" t="str">
         <f>IF(W74,ROUND(X74/W74*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="AA74" s="2"/>
       <c r="AB74" s="1">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AC74" s="1">
         <f>SUM(AC5:AC73)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD74" s="1">
         <f>SUM(AD5:AD73)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AE74" s="1" t="str">
         <f>IF(AB74,ROUND(AC74/AB74*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>42.86%</v>
       </c>
       <c r="AF74" s="2"/>
       <c r="AG74" s="1">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH74" s="1">
         <f>SUM(AH5:AH73)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI74" s="1">
         <f>SUM(AI5:AI73)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ74" s="1" t="str">
         <f>IF(AG74,ROUND(AH74/AG74*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>66.67%</v>
       </c>
       <c r="AK74" s="2"/>
       <c r="AL74" s="1">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM74" s="1">
         <f>SUM(AM5:AM73)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN74" s="1">
         <f>SUM(AN5:AN73)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO74" s="1" t="str">
         <f>IF(AL74,ROUND(AM74/AL74*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="AP74" s="2"/>
       <c r="AQ74" s="1">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR74" s="1">
         <f>SUM(AR5:AR73)</f>
@@ -33751,7 +33751,7 @@
       </c>
       <c r="AS74" s="1">
         <f>SUM(AS5:AS73)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AT74" s="1" t="str">
         <f>IF(AQ74,ROUND(AR74/AQ74*100,2),0) &amp; "%"</f>
@@ -33981,36 +33981,36 @@
       <c r="DH74" s="2"/>
       <c r="DI74" s="1">
         <f t="shared" si="107"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="DJ74" s="1">
         <f>SUM(DJ5:DJ73)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DK74" s="1">
         <f>SUM(DK5:DK73)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="DL74" s="1" t="str">
         <f>IF(DI74,ROUND(DJ74/DI74*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>33.33%</v>
       </c>
       <c r="DM74" s="2"/>
       <c r="DN74" s="1">
         <f t="shared" si="109"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="DO74" s="1">
         <f>SUM(DO5:DO73)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="DP74" s="1">
         <f>SUM(DP5:DP73)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DQ74" s="1" t="str">
         <f>IF(DN74,ROUND(DO74/DN74*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>66.67%</v>
       </c>
       <c r="DR74" s="2"/>
       <c r="DS74" s="1">
@@ -34049,7 +34049,7 @@
       <c r="EB74" s="2"/>
       <c r="EC74" s="1">
         <f t="shared" si="115"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="ED74" s="1">
         <f>SUM(ED5:ED73)</f>
@@ -34057,7 +34057,7 @@
       </c>
       <c r="EE74" s="1">
         <f>SUM(EE5:EE73)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="EF74" s="1" t="str">
         <f>IF(EC74,ROUND(ED74/EC74*100,2),0) &amp; "%"</f>
@@ -34100,23 +34100,23 @@
       <c r="EQ74" s="2"/>
       <c r="ER74" s="1">
         <f t="shared" si="121"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="ES74" s="1">
         <f>SUM(ES5:ES73)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="ET74" s="1">
         <f>SUM(ET5:ET73)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="EU74" s="1" t="str">
         <f>IF(ER74,ROUND(ES74/ER74*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="EV74" s="3"/>
     </row>
-    <row r="75" spans="1:152">
+    <row r="75" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -34270,7 +34270,7 @@
       <c r="EU75" s="3"/>
       <c r="EV75" s="3"/>
     </row>
-    <row r="76" spans="1:152">
+    <row r="76" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -34424,7 +34424,7 @@
       <c r="EU76" s="3"/>
       <c r="EV76" s="3"/>
     </row>
-    <row r="77" spans="1:152">
+    <row r="77" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>100</v>
       </c>
@@ -34820,7 +34820,7 @@
       </c>
       <c r="EV77" s="3"/>
     </row>
-    <row r="78" spans="1:152">
+    <row r="78" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>101</v>
       </c>
@@ -35278,7 +35278,7 @@
       </c>
       <c r="EV78" s="3"/>
     </row>
-    <row r="79" spans="1:152">
+    <row r="79" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>102</v>
       </c>
@@ -35736,7 +35736,7 @@
       </c>
       <c r="EV79" s="3"/>
     </row>
-    <row r="80" spans="1:152">
+    <row r="80" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>103</v>
       </c>
@@ -36194,7 +36194,7 @@
       </c>
       <c r="EV80" s="3"/>
     </row>
-    <row r="81" spans="1:152">
+    <row r="81" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>104</v>
       </c>
@@ -36652,14 +36652,14 @@
       </c>
       <c r="EV81" s="3"/>
     </row>
-    <row r="82" spans="1:152">
+    <row r="82" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B82" s="5"/>
       <c r="C82" s="2">
         <f t="shared" si="125"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D82" s="2">
         <f t="shared" si="124"/>
@@ -36667,7 +36667,7 @@
       </c>
       <c r="E82" s="2">
         <f t="shared" si="124"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F82" s="2" t="str">
         <f t="shared" si="126"/>
@@ -36706,13 +36706,13 @@
       <c r="Q82" s="5"/>
       <c r="R82" s="2">
         <f t="shared" si="131"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S82" s="2">
         <v>0</v>
       </c>
       <c r="T82" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U82" s="2" t="str">
         <f t="shared" si="132"/>
@@ -37110,18 +37110,18 @@
       </c>
       <c r="EV82" s="3"/>
     </row>
-    <row r="83" spans="1:152">
+    <row r="83" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B83" s="5"/>
       <c r="C83" s="2">
         <f t="shared" si="125"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D83" s="2">
         <f t="shared" si="124"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83" s="2">
         <f t="shared" si="124"/>
@@ -37129,7 +37129,7 @@
       </c>
       <c r="F83" s="2" t="str">
         <f t="shared" si="126"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G83" s="5"/>
       <c r="H83" s="2">
@@ -37239,17 +37239,17 @@
       <c r="AP83" s="5"/>
       <c r="AQ83" s="2">
         <f t="shared" si="141"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR83" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS83" s="2">
         <v>0</v>
       </c>
       <c r="AT83" s="2" t="str">
         <f t="shared" si="142"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AU83" s="5"/>
       <c r="AV83" s="2">
@@ -37568,7 +37568,7 @@
       </c>
       <c r="EV83" s="3"/>
     </row>
-    <row r="84" spans="1:152">
+    <row r="84" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>107</v>
       </c>
@@ -38026,7 +38026,7 @@
       </c>
       <c r="EV84" s="3"/>
     </row>
-    <row r="85" spans="1:152">
+    <row r="85" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>108</v>
       </c>
@@ -38484,18 +38484,18 @@
       </c>
       <c r="EV85" s="3"/>
     </row>
-    <row r="86" spans="1:152">
+    <row r="86" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="2">
         <f t="shared" si="125"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D86" s="2">
         <f t="shared" si="124"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E86" s="2">
         <f t="shared" si="124"/>
@@ -38503,7 +38503,7 @@
       </c>
       <c r="F86" s="2" t="str">
         <f t="shared" si="126"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G86" s="5"/>
       <c r="H86" s="2">
@@ -38523,17 +38523,17 @@
       <c r="L86" s="5"/>
       <c r="M86" s="2">
         <f t="shared" si="129"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N86" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O86" s="2">
         <v>0</v>
       </c>
       <c r="P86" s="2" t="str">
         <f t="shared" si="130"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="Q86" s="5"/>
       <c r="R86" s="2">
@@ -38942,7 +38942,7 @@
       </c>
       <c r="EV86" s="3"/>
     </row>
-    <row r="87" spans="1:152">
+    <row r="87" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>110</v>
       </c>
@@ -39400,7 +39400,7 @@
       </c>
       <c r="EV87" s="3"/>
     </row>
-    <row r="88" spans="1:152">
+    <row r="88" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>111</v>
       </c>
@@ -39858,7 +39858,7 @@
       </c>
       <c r="EV88" s="3"/>
     </row>
-    <row r="89" spans="1:152">
+    <row r="89" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>112</v>
       </c>
@@ -40316,7 +40316,7 @@
       </c>
       <c r="EV89" s="3"/>
     </row>
-    <row r="90" spans="1:152">
+    <row r="90" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>113</v>
       </c>
@@ -40774,7 +40774,7 @@
       </c>
       <c r="EV90" s="3"/>
     </row>
-    <row r="91" spans="1:152">
+    <row r="91" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>114</v>
       </c>
@@ -41232,7 +41232,7 @@
       </c>
       <c r="EV91" s="3"/>
     </row>
-    <row r="92" spans="1:152">
+    <row r="92" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>115</v>
       </c>
@@ -41690,14 +41690,14 @@
       </c>
       <c r="EV92" s="3"/>
     </row>
-    <row r="93" spans="1:152">
+    <row r="93" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B93" s="5"/>
       <c r="C93" s="2">
         <f t="shared" si="125"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D93" s="2">
         <f t="shared" si="124"/>
@@ -41705,7 +41705,7 @@
       </c>
       <c r="E93" s="2">
         <f t="shared" si="124"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F93" s="2" t="str">
         <f t="shared" si="126"/>
@@ -42089,13 +42089,13 @@
       <c r="EB93" s="5"/>
       <c r="EC93" s="2">
         <f t="shared" si="177"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ED93" s="2">
         <v>0</v>
       </c>
       <c r="EE93" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EF93" s="2" t="str">
         <f t="shared" si="178"/>
@@ -42148,7 +42148,7 @@
       </c>
       <c r="EV93" s="3"/>
     </row>
-    <row r="94" spans="1:152">
+    <row r="94" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>117</v>
       </c>
@@ -42606,7 +42606,7 @@
       </c>
       <c r="EV94" s="3"/>
     </row>
-    <row r="95" spans="1:152">
+    <row r="95" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>118</v>
       </c>
@@ -43064,7 +43064,7 @@
       </c>
       <c r="EV95" s="3"/>
     </row>
-    <row r="96" spans="1:152">
+    <row r="96" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>119</v>
       </c>
@@ -43522,7 +43522,7 @@
       </c>
       <c r="EV96" s="3"/>
     </row>
-    <row r="97" spans="1:152">
+    <row r="97" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>120</v>
       </c>
@@ -43980,7 +43980,7 @@
       </c>
       <c r="EV97" s="3"/>
     </row>
-    <row r="98" spans="1:152">
+    <row r="98" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>121</v>
       </c>
@@ -44438,7 +44438,7 @@
       </c>
       <c r="EV98" s="3"/>
     </row>
-    <row r="99" spans="1:152">
+    <row r="99" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>122</v>
       </c>
@@ -44896,18 +44896,18 @@
       </c>
       <c r="EV99" s="3"/>
     </row>
-    <row r="100" spans="1:152">
+    <row r="100" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>181</v>
       </c>
       <c r="B100" s="5"/>
       <c r="C100" s="2">
         <f t="shared" si="125"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D100" s="2">
         <f t="shared" si="185"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E100" s="2">
         <f t="shared" si="186"/>
@@ -44915,7 +44915,7 @@
       </c>
       <c r="F100" s="2" t="str">
         <f t="shared" si="126"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G100" s="5"/>
       <c r="H100" s="2">
@@ -44995,17 +44995,17 @@
       <c r="AF100" s="5"/>
       <c r="AG100" s="2">
         <f t="shared" si="137"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH100" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI100" s="2">
         <v>0</v>
       </c>
       <c r="AJ100" s="2" t="str">
         <f t="shared" si="138"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AK100" s="5"/>
       <c r="AL100" s="2">
@@ -45070,17 +45070,17 @@
       <c r="BE100" s="5"/>
       <c r="BF100" s="2">
         <f t="shared" si="147"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG100" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH100" s="2">
         <v>0</v>
       </c>
       <c r="BI100" s="2" t="str">
         <f t="shared" si="148"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="BJ100" s="5"/>
       <c r="BK100" s="2">
@@ -45354,26 +45354,26 @@
       </c>
       <c r="EV100" s="3"/>
     </row>
-    <row r="101" spans="1:152">
+    <row r="101" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B101" s="5"/>
       <c r="C101" s="2">
         <f>SUM(C78:C100)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D101" s="2">
         <f>SUM(D78:D100)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E101" s="2">
         <f>SUM(E78:E100)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F101" s="2" t="str">
         <f>IF(C101,ROUND(D101/C101*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>66.67%</v>
       </c>
       <c r="G101" s="5"/>
       <c r="H101" s="2">
@@ -45395,11 +45395,11 @@
       <c r="L101" s="5"/>
       <c r="M101" s="2">
         <f>+SUM(N101,O101)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N101" s="2">
         <f>SUM(N78:N100)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O101" s="2">
         <f>SUM(O78:O100)</f>
@@ -45407,12 +45407,12 @@
       </c>
       <c r="P101" s="2" t="str">
         <f>IF(M101,ROUND(N101/M101*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="Q101" s="5"/>
       <c r="R101" s="2">
         <f>+SUM(S101,T101)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S101" s="2">
         <f>SUM(S78:S100)</f>
@@ -45420,7 +45420,7 @@
       </c>
       <c r="T101" s="2">
         <f>SUM(T78:T100)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U101" s="2" t="str">
         <f>IF(R101,ROUND(S101/R101*100,2),0) &amp; "%"</f>
@@ -45463,11 +45463,11 @@
       <c r="AF101" s="5"/>
       <c r="AG101" s="2">
         <f>+SUM(AH101,AI101)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH101" s="2">
         <f>SUM(AH78:AH100)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI101" s="2">
         <f>SUM(AI78:AI100)</f>
@@ -45475,7 +45475,7 @@
       </c>
       <c r="AJ101" s="2" t="str">
         <f>IF(AG101,ROUND(AH101/AG101*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AK101" s="5"/>
       <c r="AL101" s="2">
@@ -45497,11 +45497,11 @@
       <c r="AP101" s="5"/>
       <c r="AQ101" s="2">
         <f>+SUM(AR101,AS101)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR101" s="2">
         <f>SUM(AR78:AR100)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS101" s="2">
         <f>SUM(AS78:AS100)</f>
@@ -45509,7 +45509,7 @@
       </c>
       <c r="AT101" s="2" t="str">
         <f>IF(AQ101,ROUND(AR101/AQ101*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AU101" s="5"/>
       <c r="AV101" s="2">
@@ -45548,11 +45548,11 @@
       <c r="BE101" s="5"/>
       <c r="BF101" s="2">
         <f>+SUM(BG101,BH101)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG101" s="2">
         <f>SUM(BG78:BG100)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH101" s="2">
         <f>SUM(BH78:BH100)</f>
@@ -45560,7 +45560,7 @@
       </c>
       <c r="BI101" s="2" t="str">
         <f>IF(BF101,ROUND(BG101/BF101*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="BJ101" s="5"/>
       <c r="BK101" s="2">
@@ -45803,7 +45803,7 @@
       <c r="EB101" s="5"/>
       <c r="EC101" s="2">
         <f>+SUM(ED101,EE101)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ED101" s="2">
         <f>SUM(ED78:ED100)</f>
@@ -45811,7 +45811,7 @@
       </c>
       <c r="EE101" s="2">
         <f>SUM(EE78:EE100)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EF101" s="2" t="str">
         <f>IF(EC101,ROUND(ED101/EC101*100,2),0) &amp; "%"</f>
@@ -45870,7 +45870,7 @@
       </c>
       <c r="EV101" s="3"/>
     </row>
-    <row r="102" spans="1:152">
+    <row r="102" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="6"/>
@@ -46024,7 +46024,7 @@
       <c r="EU102" s="3"/>
       <c r="EV102" s="3"/>
     </row>
-    <row r="103" spans="1:152">
+    <row r="103" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="6"/>
@@ -46178,7 +46178,7 @@
       <c r="EU103" s="3"/>
       <c r="EV103" s="3"/>
     </row>
-    <row r="104" spans="1:152">
+    <row r="104" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>172</v>
       </c>
@@ -46190,7 +46190,7 @@
       <c r="E104" s="9"/>
       <c r="F104" s="9" t="str">
         <f>IF(SUM(D74,D101),ROUND(SUM(D74,D101)*100/SUM(C74,C101),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>47.17%</v>
       </c>
       <c r="G104" s="10"/>
       <c r="H104" s="9" t="s">
@@ -46200,7 +46200,7 @@
       <c r="J104" s="9"/>
       <c r="K104" s="9" t="str">
         <f>IF(SUM(I74,I101),ROUND(SUM(I74,I101)*100/SUM(H74,H101),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="L104" s="10"/>
       <c r="M104" s="9" t="s">
@@ -46210,7 +46210,7 @@
       <c r="O104" s="9"/>
       <c r="P104" s="9" t="str">
         <f>IF(SUM(N74,N101),ROUND(SUM(N74,N101)*100/SUM(M74,M101),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>57.14%</v>
       </c>
       <c r="Q104" s="10"/>
       <c r="R104" s="9" t="s">
@@ -46220,7 +46220,7 @@
       <c r="T104" s="9"/>
       <c r="U104" s="9" t="str">
         <f>IF(SUM(S74,S101),ROUND(SUM(S74,S101)*100/SUM(R74,R101),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>42.86%</v>
       </c>
       <c r="V104" s="10"/>
       <c r="W104" s="9" t="s">
@@ -46230,7 +46230,7 @@
       <c r="Y104" s="9"/>
       <c r="Z104" s="9" t="str">
         <f>IF(SUM(X74,X101),ROUND(SUM(X74,X101)*100/SUM(W74,W101),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="AA104" s="10"/>
       <c r="AB104" s="9" t="s">
@@ -46240,7 +46240,7 @@
       <c r="AD104" s="9"/>
       <c r="AE104" s="9" t="str">
         <f>IF(SUM(AC74,AC101),ROUND(SUM(AC74,AC101)*100/SUM(AB74,AB101),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>42.86%</v>
       </c>
       <c r="AF104" s="10"/>
       <c r="AG104" s="9" t="s">
@@ -46250,7 +46250,7 @@
       <c r="AI104" s="9"/>
       <c r="AJ104" s="9" t="str">
         <f>IF(SUM(AH74,AH101),ROUND(SUM(AH74,AH101)*100/SUM(AG74,AG101),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>75%</v>
       </c>
       <c r="AK104" s="10"/>
       <c r="AL104" s="9" t="s">
@@ -46260,7 +46260,7 @@
       <c r="AN104" s="9"/>
       <c r="AO104" s="9" t="str">
         <f>IF(SUM(AM74,AM101),ROUND(SUM(AM74,AM101)*100/SUM(AL74,AL101),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="AP104" s="10"/>
       <c r="AQ104" s="9" t="s">
@@ -46270,7 +46270,7 @@
       <c r="AS104" s="9"/>
       <c r="AT104" s="9" t="str">
         <f>IF(SUM(AR74,AR101),ROUND(SUM(AR74,AR101)*100/SUM(AQ74,AQ101),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>25%</v>
       </c>
       <c r="AU104" s="10"/>
       <c r="AV104" s="9" t="s">
@@ -46300,7 +46300,7 @@
       <c r="BH104" s="9"/>
       <c r="BI104" s="9" t="str">
         <f>IF(SUM(BG74,BG101),ROUND(SUM(BG74,BG101)*100/SUM(BF74,BF101),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="BJ104" s="10"/>
       <c r="BK104" s="9" t="s">
@@ -46410,7 +46410,7 @@
       <c r="DK104" s="9"/>
       <c r="DL104" s="9" t="str">
         <f>IF(SUM(DJ74,DJ101),ROUND(SUM(DJ74,DJ101)*100/SUM(DI74,DI101),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>33.33%</v>
       </c>
       <c r="DM104" s="10"/>
       <c r="DN104" s="9" t="s">
@@ -46420,7 +46420,7 @@
       <c r="DP104" s="9"/>
       <c r="DQ104" s="9" t="str">
         <f>IF(SUM(DO74,DO101),ROUND(SUM(DO74,DO101)*100/SUM(DN74,DN101),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>66.67%</v>
       </c>
       <c r="DR104" s="10"/>
       <c r="DS104" s="9" t="s">
@@ -46480,11 +46480,11 @@
       <c r="ET104" s="9"/>
       <c r="EU104" s="9" t="str">
         <f>IF(SUM(ES74,ES101),ROUND(SUM(ES74,ES101)*100/SUM(ER74,ER101),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="EV104" s="3"/>
     </row>
-    <row r="105" spans="1:152">
+    <row r="105" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="6"/>
@@ -46638,7 +46638,7 @@
       <c r="EU105" s="3"/>
       <c r="EV105" s="3"/>
     </row>
-    <row r="106" spans="1:152">
+    <row r="106" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -46792,7 +46792,7 @@
       <c r="EU106" s="3"/>
       <c r="EV106" s="3"/>
     </row>
-    <row r="107" spans="1:152">
+    <row r="107" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>123</v>
       </c>
@@ -47188,7 +47188,7 @@
       </c>
       <c r="EV107" s="3"/>
     </row>
-    <row r="108" spans="1:152">
+    <row r="108" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
         <v>124</v>
       </c>
@@ -47646,7 +47646,7 @@
       </c>
       <c r="EV108" s="3"/>
     </row>
-    <row r="109" spans="1:152">
+    <row r="109" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>125</v>
       </c>
@@ -48104,14 +48104,14 @@
       </c>
       <c r="EV109" s="3"/>
     </row>
-    <row r="110" spans="1:152">
+    <row r="110" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>126</v>
       </c>
       <c r="B110" s="8"/>
       <c r="C110" s="7">
         <f t="shared" si="188"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D110" s="7">
         <f t="shared" si="187"/>
@@ -48119,7 +48119,7 @@
       </c>
       <c r="E110" s="7">
         <f t="shared" si="187"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F110" s="7" t="str">
         <f t="shared" si="189"/>
@@ -48218,13 +48218,13 @@
       <c r="AK110" s="8"/>
       <c r="AL110" s="7">
         <f t="shared" si="202"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM110" s="7">
         <v>0</v>
       </c>
       <c r="AN110" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO110" s="7" t="str">
         <f t="shared" si="203"/>
@@ -48562,7 +48562,7 @@
       </c>
       <c r="EV110" s="3"/>
     </row>
-    <row r="111" spans="1:152">
+    <row r="111" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
         <v>127</v>
       </c>
@@ -49020,7 +49020,7 @@
       </c>
       <c r="EV111" s="3"/>
     </row>
-    <row r="112" spans="1:152">
+    <row r="112" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
         <v>128</v>
       </c>
@@ -49478,7 +49478,7 @@
       </c>
       <c r="EV112" s="3"/>
     </row>
-    <row r="113" spans="1:152">
+    <row r="113" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
         <v>129</v>
       </c>
@@ -49936,7 +49936,7 @@
       </c>
       <c r="EV113" s="3"/>
     </row>
-    <row r="114" spans="1:152">
+    <row r="114" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>130</v>
       </c>
@@ -50394,18 +50394,18 @@
       </c>
       <c r="EV114" s="3"/>
     </row>
-    <row r="115" spans="1:152">
+    <row r="115" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>131</v>
       </c>
       <c r="B115" s="8"/>
       <c r="C115" s="7">
         <f t="shared" si="188"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D115" s="7">
         <f t="shared" si="187"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E115" s="7">
         <f t="shared" si="187"/>
@@ -50413,7 +50413,7 @@
       </c>
       <c r="F115" s="7" t="str">
         <f t="shared" si="189"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G115" s="8"/>
       <c r="H115" s="7">
@@ -50508,17 +50508,17 @@
       <c r="AK115" s="8"/>
       <c r="AL115" s="7">
         <f t="shared" si="202"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM115" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN115" s="7">
         <v>0</v>
       </c>
       <c r="AO115" s="7" t="str">
         <f t="shared" si="203"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AP115" s="8"/>
       <c r="AQ115" s="7">
@@ -50838,40 +50838,40 @@
       <c r="EQ115" s="8"/>
       <c r="ER115" s="7">
         <f t="shared" si="246"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ES115" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ET115" s="7">
         <v>0</v>
       </c>
       <c r="EU115" s="7" t="str">
         <f t="shared" si="247"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="EV115" s="3"/>
     </row>
-    <row r="116" spans="1:152">
+    <row r="116" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
         <v>132</v>
       </c>
       <c r="B116" s="8"/>
       <c r="C116" s="7">
         <f t="shared" si="188"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D116" s="7">
         <f t="shared" si="187"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E116" s="7">
         <f t="shared" si="187"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F116" s="7" t="str">
         <f t="shared" si="189"/>
-        <v>0%</v>
+        <v>66.67%</v>
       </c>
       <c r="G116" s="8"/>
       <c r="H116" s="7">
@@ -50906,17 +50906,17 @@
       <c r="Q116" s="8"/>
       <c r="R116" s="7">
         <f t="shared" si="194"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S116" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T116" s="7">
         <v>0</v>
       </c>
       <c r="U116" s="7" t="str">
         <f t="shared" si="195"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="V116" s="8"/>
       <c r="W116" s="7">
@@ -50951,17 +50951,17 @@
       <c r="AF116" s="8"/>
       <c r="AG116" s="7">
         <f t="shared" si="200"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH116" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI116" s="7">
         <v>0</v>
       </c>
       <c r="AJ116" s="7" t="str">
         <f t="shared" si="201"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AK116" s="8"/>
       <c r="AL116" s="7">
@@ -50981,13 +50981,13 @@
       <c r="AP116" s="8"/>
       <c r="AQ116" s="7">
         <f t="shared" si="204"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR116" s="7">
         <v>0</v>
       </c>
       <c r="AS116" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT116" s="7" t="str">
         <f t="shared" si="205"/>
@@ -51310,14 +51310,14 @@
       </c>
       <c r="EV116" s="3"/>
     </row>
-    <row r="117" spans="1:152">
+    <row r="117" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
         <v>133</v>
       </c>
       <c r="B117" s="8"/>
       <c r="C117" s="7">
         <f t="shared" si="188"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D117" s="7">
         <f t="shared" si="187"/>
@@ -51325,7 +51325,7 @@
       </c>
       <c r="E117" s="7">
         <f t="shared" si="187"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F117" s="7" t="str">
         <f t="shared" si="189"/>
@@ -51379,13 +51379,13 @@
       <c r="V117" s="8"/>
       <c r="W117" s="7">
         <f t="shared" si="196"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X117" s="7">
         <v>0</v>
       </c>
       <c r="Y117" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z117" s="7" t="str">
         <f t="shared" si="197"/>
@@ -51768,7 +51768,7 @@
       </c>
       <c r="EV117" s="3"/>
     </row>
-    <row r="118" spans="1:152">
+    <row r="118" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
         <v>134</v>
       </c>
@@ -52226,7 +52226,7 @@
       </c>
       <c r="EV118" s="3"/>
     </row>
-    <row r="119" spans="1:152">
+    <row r="119" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>135</v>
       </c>
@@ -52684,7 +52684,7 @@
       </c>
       <c r="EV119" s="3"/>
     </row>
-    <row r="120" spans="1:152">
+    <row r="120" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
         <v>136</v>
       </c>
@@ -53142,7 +53142,7 @@
       </c>
       <c r="EV120" s="3"/>
     </row>
-    <row r="121" spans="1:152">
+    <row r="121" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
         <v>137</v>
       </c>
@@ -53600,7 +53600,7 @@
       </c>
       <c r="EV121" s="3"/>
     </row>
-    <row r="122" spans="1:152">
+    <row r="122" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>138</v>
       </c>
@@ -54058,7 +54058,7 @@
       </c>
       <c r="EV122" s="3"/>
     </row>
-    <row r="123" spans="1:152">
+    <row r="123" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>139</v>
       </c>
@@ -54516,7 +54516,7 @@
       </c>
       <c r="EV123" s="3"/>
     </row>
-    <row r="124" spans="1:152">
+    <row r="124" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>140</v>
       </c>
@@ -54974,7 +54974,7 @@
       </c>
       <c r="EV124" s="3"/>
     </row>
-    <row r="125" spans="1:152">
+    <row r="125" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
         <v>141</v>
       </c>
@@ -55432,18 +55432,18 @@
       </c>
       <c r="EV125" s="3"/>
     </row>
-    <row r="126" spans="1:152">
+    <row r="126" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>142</v>
       </c>
       <c r="B126" s="8"/>
       <c r="C126" s="7">
         <f t="shared" si="188"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D126" s="7">
         <f t="shared" si="248"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E126" s="7">
         <f t="shared" si="249"/>
@@ -55451,7 +55451,7 @@
       </c>
       <c r="F126" s="7" t="str">
         <f t="shared" si="189"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G126" s="8"/>
       <c r="H126" s="7">
@@ -55501,17 +55501,17 @@
       <c r="V126" s="8"/>
       <c r="W126" s="7">
         <f t="shared" si="196"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X126" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y126" s="7">
         <v>0</v>
       </c>
       <c r="Z126" s="7" t="str">
         <f t="shared" si="197"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AA126" s="8"/>
       <c r="AB126" s="7">
@@ -55531,17 +55531,17 @@
       <c r="AF126" s="8"/>
       <c r="AG126" s="7">
         <f t="shared" si="200"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH126" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI126" s="7">
         <v>0</v>
       </c>
       <c r="AJ126" s="7" t="str">
         <f t="shared" si="201"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AK126" s="8"/>
       <c r="AL126" s="7">
@@ -55890,7 +55890,7 @@
       </c>
       <c r="EV126" s="3"/>
     </row>
-    <row r="127" spans="1:152">
+    <row r="127" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>143</v>
       </c>
@@ -56348,7 +56348,7 @@
       </c>
       <c r="EV127" s="3"/>
     </row>
-    <row r="128" spans="1:152">
+    <row r="128" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>144</v>
       </c>
@@ -56806,7 +56806,7 @@
       </c>
       <c r="EV128" s="3"/>
     </row>
-    <row r="129" spans="1:152">
+    <row r="129" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
         <v>145</v>
       </c>
@@ -57264,7 +57264,7 @@
       </c>
       <c r="EV129" s="3"/>
     </row>
-    <row r="130" spans="1:152">
+    <row r="130" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
         <v>146</v>
       </c>
@@ -57722,7 +57722,7 @@
       </c>
       <c r="EV130" s="3"/>
     </row>
-    <row r="131" spans="1:152">
+    <row r="131" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
         <v>147</v>
       </c>
@@ -58180,67 +58180,67 @@
       </c>
       <c r="EV131" s="3"/>
     </row>
-    <row r="132" spans="1:152">
+    <row r="132" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>182</v>
       </c>
       <c r="B132" s="8"/>
       <c r="C132" s="7">
         <f t="shared" si="188"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D132" s="7">
         <f t="shared" si="248"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E132" s="7">
         <f t="shared" si="249"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F132" s="7" t="str">
         <f t="shared" si="189"/>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="G132" s="8"/>
       <c r="H132" s="7">
         <f t="shared" si="190"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I132" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J132" s="7">
         <v>0</v>
       </c>
       <c r="K132" s="7" t="str">
         <f t="shared" si="191"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="L132" s="8"/>
       <c r="M132" s="7">
         <f t="shared" si="192"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N132" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O132" s="7">
         <v>0</v>
       </c>
       <c r="P132" s="7" t="str">
         <f t="shared" si="193"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="Q132" s="8"/>
       <c r="R132" s="7">
         <f t="shared" si="194"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S132" s="7">
         <v>0</v>
       </c>
       <c r="T132" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U132" s="7" t="str">
         <f t="shared" si="195"/>
@@ -58519,13 +58519,13 @@
       <c r="DH132" s="8"/>
       <c r="DI132" s="7">
         <f t="shared" si="232"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DJ132" s="7">
         <v>0</v>
       </c>
       <c r="DK132" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DL132" s="7" t="str">
         <f t="shared" si="233"/>
@@ -58638,35 +58638,35 @@
       </c>
       <c r="EV132" s="3"/>
     </row>
-    <row r="133" spans="1:152">
+    <row r="133" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
         <v>95</v>
       </c>
       <c r="B133" s="8"/>
       <c r="C133" s="7">
         <f>SUM(C108:C132)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D133" s="7">
         <f t="shared" ref="D133:E133" si="250">SUM(D108:D132)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E133" s="7">
         <f t="shared" si="250"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F133" s="7" t="str">
         <f>IF(C133,ROUND(D133/C133*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>61.54%</v>
       </c>
       <c r="G133" s="8"/>
       <c r="H133" s="7">
         <f>SUM(H108:H132)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I133" s="7">
         <f t="shared" ref="I133:J133" si="251">SUM(I108:I132)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J133" s="7">
         <f t="shared" si="251"/>
@@ -58674,16 +58674,16 @@
       </c>
       <c r="K133" s="7" t="str">
         <f>IF(H133,ROUND(I133/H133*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="L133" s="8"/>
       <c r="M133" s="7">
         <f>SUM(M108:M132)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N133" s="7">
         <f>SUM(N108:N132)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O133" s="7">
         <f t="shared" ref="O133" si="252">SUM(O108:O132)</f>
@@ -58691,41 +58691,41 @@
       </c>
       <c r="P133" s="7" t="str">
         <f>IF(M133,ROUND(N133/M133*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="Q133" s="8"/>
       <c r="R133" s="7">
         <f>SUM(R108:R132)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S133" s="7">
         <f t="shared" ref="S133" si="253">SUM(S108:S132)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T133" s="7">
         <f t="shared" ref="T133" si="254">SUM(T108:T132)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U133" s="7" t="str">
         <f>IF(R133,ROUND(S133/R133*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="V133" s="8"/>
       <c r="W133" s="7">
         <f>SUM(W108:W132)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X133" s="7">
         <f t="shared" ref="X133" si="255">SUM(X108:X132)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y133" s="7">
         <f t="shared" ref="Y133" si="256">SUM(Y108:Y132)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z133" s="7" t="str">
         <f>IF(W133,ROUND(X133/W133*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="AA133" s="8"/>
       <c r="AB133" s="7">
@@ -58747,11 +58747,11 @@
       <c r="AF133" s="8"/>
       <c r="AG133" s="7">
         <f>SUM(AG108:AG132)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH133" s="7">
         <f t="shared" ref="AH133" si="259">SUM(AH108:AH132)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI133" s="7">
         <f t="shared" ref="AI133" si="260">SUM(AI108:AI132)</f>
@@ -58759,29 +58759,29 @@
       </c>
       <c r="AJ133" s="7" t="str">
         <f>IF(AG133,ROUND(AH133/AG133*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AK133" s="8"/>
       <c r="AL133" s="7">
         <f>SUM(AL108:AL132)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM133" s="7">
         <f t="shared" ref="AM133" si="261">SUM(AM108:AM132)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN133" s="7">
         <f t="shared" ref="AN133" si="262">SUM(AN108:AN132)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO133" s="7" t="str">
         <f>IF(AL133,ROUND(AM133/AL133*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="AP133" s="8"/>
       <c r="AQ133" s="7">
         <f>SUM(AQ108:AQ132)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR133" s="7">
         <f t="shared" ref="AR133" si="263">SUM(AR108:AR132)</f>
@@ -58789,7 +58789,7 @@
       </c>
       <c r="AS133" s="7">
         <f t="shared" ref="AS133" si="264">SUM(AS108:AS132)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT133" s="7" t="str">
         <f>IF(AQ133,ROUND(AR133/AQ133*100,2),0) &amp; "%"</f>
@@ -59019,7 +59019,7 @@
       <c r="DH133" s="8"/>
       <c r="DI133" s="7">
         <f>SUM(DI108:DI132)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DJ133" s="7">
         <f t="shared" ref="DJ133" si="291">SUM(DJ108:DJ132)</f>
@@ -59027,7 +59027,7 @@
       </c>
       <c r="DK133" s="7">
         <f t="shared" ref="DK133" si="292">SUM(DK108:DK132)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DL133" s="7" t="str">
         <f>IF(DI133,ROUND(DJ133/DI133*100,2),0) &amp; "%"</f>
@@ -59138,11 +59138,11 @@
       <c r="EQ133" s="8"/>
       <c r="ER133" s="7">
         <f>SUM(ER108:ER132)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ES133" s="7">
         <f t="shared" ref="ES133" si="305">SUM(ES108:ES132)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ET133" s="7">
         <f t="shared" ref="ET133" si="306">SUM(ET108:ET132)</f>
@@ -59150,11 +59150,11 @@
       </c>
       <c r="EU133" s="7" t="str">
         <f>IF(ER133,ROUND(ES133/ER133*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="EV133" s="3"/>
     </row>
-    <row r="134" spans="1:152">
+    <row r="134" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
@@ -59308,7 +59308,7 @@
       <c r="EU134" s="3"/>
       <c r="EV134" s="3"/>
     </row>
-    <row r="135" spans="1:152">
+    <row r="135" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
@@ -59462,7 +59462,7 @@
       <c r="EU135" s="3"/>
       <c r="EV135" s="3"/>
     </row>
-    <row r="136" spans="1:152">
+    <row r="136" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A136" s="12" t="s">
         <v>149</v>
       </c>
@@ -59858,7 +59858,7 @@
       </c>
       <c r="EV136" s="3"/>
     </row>
-    <row r="137" spans="1:152">
+    <row r="137" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A137" s="12" t="s">
         <v>150</v>
       </c>
@@ -60316,14 +60316,14 @@
       </c>
       <c r="EV137" s="3"/>
     </row>
-    <row r="138" spans="1:152">
+    <row r="138" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A138" s="12" t="s">
         <v>151</v>
       </c>
       <c r="B138" s="11"/>
       <c r="C138" s="12">
         <f t="shared" ref="C138:C156" si="308">SUM(H138,M138,R138,W138,AB138,AG138,AL138,AQ138,AV138,BA138,BF138,BK138,BP138,BU138,BZ138,CE138,CJ138,CO138,CT138,CY138,DD138,DI138,DN138,DS138,DX138,EC138,EH138,EM138,ER138)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D138" s="12">
         <f t="shared" si="307"/>
@@ -60331,7 +60331,7 @@
       </c>
       <c r="E138" s="12">
         <f t="shared" si="307"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F138" s="13" t="str">
         <f t="shared" ref="F138:F156" si="309">IF(C138,ROUND(D138/C138*100,2),0) &amp; "%"</f>
@@ -60715,13 +60715,13 @@
       <c r="EB138" s="11"/>
       <c r="EC138" s="12">
         <f t="shared" ref="EC138:EC156" si="360">+SUM(ED138,EE138)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ED138" s="13">
         <v>0</v>
       </c>
       <c r="EE138" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EF138" s="13" t="str">
         <f t="shared" ref="EF138:EF156" si="361">IF(EC138,ROUND(ED138/EC138*100,2),0) &amp; "%"</f>
@@ -60774,7 +60774,7 @@
       </c>
       <c r="EV138" s="3"/>
     </row>
-    <row r="139" spans="1:152">
+    <row r="139" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A139" s="12" t="s">
         <v>152</v>
       </c>
@@ -61232,7 +61232,7 @@
       </c>
       <c r="EV139" s="3"/>
     </row>
-    <row r="140" spans="1:152">
+    <row r="140" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A140" s="12" t="s">
         <v>153</v>
       </c>
@@ -61690,7 +61690,7 @@
       </c>
       <c r="EV140" s="3"/>
     </row>
-    <row r="141" spans="1:152">
+    <row r="141" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A141" s="12" t="s">
         <v>154</v>
       </c>
@@ -62148,7 +62148,7 @@
       </c>
       <c r="EV141" s="3"/>
     </row>
-    <row r="142" spans="1:152">
+    <row r="142" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A142" s="12" t="s">
         <v>155</v>
       </c>
@@ -62606,7 +62606,7 @@
       </c>
       <c r="EV142" s="3"/>
     </row>
-    <row r="143" spans="1:152">
+    <row r="143" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A143" s="12" t="s">
         <v>156</v>
       </c>
@@ -63064,7 +63064,7 @@
       </c>
       <c r="EV143" s="3"/>
     </row>
-    <row r="144" spans="1:152">
+    <row r="144" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A144" s="12" t="s">
         <v>157</v>
       </c>
@@ -63522,18 +63522,18 @@
       </c>
       <c r="EV144" s="3"/>
     </row>
-    <row r="145" spans="1:152">
+    <row r="145" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A145" s="12" t="s">
         <v>158</v>
       </c>
       <c r="B145" s="11"/>
       <c r="C145" s="12">
         <f t="shared" si="308"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D145" s="12">
         <f t="shared" si="307"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E145" s="12">
         <f t="shared" si="307"/>
@@ -63541,7 +63541,7 @@
       </c>
       <c r="F145" s="13" t="str">
         <f t="shared" si="309"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G145" s="11"/>
       <c r="H145" s="12">
@@ -63876,17 +63876,17 @@
       <c r="DM145" s="11"/>
       <c r="DN145" s="12">
         <f t="shared" si="354"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DO145" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DP145" s="13">
         <v>0</v>
       </c>
       <c r="DQ145" s="13" t="str">
         <f t="shared" si="355"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="DR145" s="11"/>
       <c r="DS145" s="12">
@@ -63980,18 +63980,18 @@
       </c>
       <c r="EV145" s="3"/>
     </row>
-    <row r="146" spans="1:152">
+    <row r="146" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A146" s="12" t="s">
         <v>159</v>
       </c>
       <c r="B146" s="11"/>
       <c r="C146" s="12">
         <f t="shared" si="308"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D146" s="12">
         <f t="shared" si="307"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E146" s="12">
         <f t="shared" si="307"/>
@@ -63999,7 +63999,7 @@
       </c>
       <c r="F146" s="13" t="str">
         <f t="shared" si="309"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G146" s="11"/>
       <c r="H146" s="12">
@@ -64064,17 +64064,17 @@
       <c r="AA146" s="11"/>
       <c r="AB146" s="12">
         <f t="shared" si="318"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC146" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD146" s="13">
         <v>0</v>
       </c>
       <c r="AE146" s="13" t="str">
         <f t="shared" si="319"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AF146" s="11"/>
       <c r="AG146" s="12">
@@ -64438,7 +64438,7 @@
       </c>
       <c r="EV146" s="3"/>
     </row>
-    <row r="147" spans="1:152">
+    <row r="147" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A147" s="12" t="s">
         <v>160</v>
       </c>
@@ -64896,14 +64896,14 @@
       </c>
       <c r="EV147" s="3"/>
     </row>
-    <row r="148" spans="1:152">
+    <row r="148" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A148" s="12" t="s">
         <v>161</v>
       </c>
       <c r="B148" s="11"/>
       <c r="C148" s="12">
         <f t="shared" si="308"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D148" s="12">
         <f t="shared" si="307"/>
@@ -64911,7 +64911,7 @@
       </c>
       <c r="E148" s="12">
         <f t="shared" si="307"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F148" s="13" t="str">
         <f t="shared" si="309"/>
@@ -64980,13 +64980,13 @@
       <c r="AA148" s="11"/>
       <c r="AB148" s="12">
         <f t="shared" si="318"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC148" s="13">
         <v>0</v>
       </c>
       <c r="AD148" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE148" s="13" t="str">
         <f t="shared" si="319"/>
@@ -65354,18 +65354,18 @@
       </c>
       <c r="EV148" s="3"/>
     </row>
-    <row r="149" spans="1:152">
+    <row r="149" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A149" s="12" t="s">
         <v>162</v>
       </c>
       <c r="B149" s="11"/>
       <c r="C149" s="12">
         <f t="shared" si="308"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D149" s="12">
         <f t="shared" si="307"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E149" s="12">
         <f t="shared" si="307"/>
@@ -65373,7 +65373,7 @@
       </c>
       <c r="F149" s="13" t="str">
         <f t="shared" si="309"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="G149" s="11"/>
       <c r="H149" s="12">
@@ -65423,17 +65423,17 @@
       <c r="V149" s="11"/>
       <c r="W149" s="12">
         <f t="shared" si="316"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X149" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y149" s="13">
         <v>0</v>
       </c>
       <c r="Z149" s="13" t="str">
         <f t="shared" si="317"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AA149" s="11"/>
       <c r="AB149" s="12">
@@ -65812,7 +65812,7 @@
       </c>
       <c r="EV149" s="3"/>
     </row>
-    <row r="150" spans="1:152">
+    <row r="150" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A150" s="12" t="s">
         <v>163</v>
       </c>
@@ -66270,7 +66270,7 @@
       </c>
       <c r="EV150" s="3"/>
     </row>
-    <row r="151" spans="1:152">
+    <row r="151" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A151" s="12" t="s">
         <v>164</v>
       </c>
@@ -66728,7 +66728,7 @@
       </c>
       <c r="EV151" s="3"/>
     </row>
-    <row r="152" spans="1:152">
+    <row r="152" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A152" s="12" t="s">
         <v>165</v>
       </c>
@@ -67186,7 +67186,7 @@
       </c>
       <c r="EV152" s="3"/>
     </row>
-    <row r="153" spans="1:152">
+    <row r="153" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A153" s="12" t="s">
         <v>166</v>
       </c>
@@ -67644,7 +67644,7 @@
       </c>
       <c r="EV153" s="3"/>
     </row>
-    <row r="154" spans="1:152">
+    <row r="154" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A154" s="12" t="s">
         <v>167</v>
       </c>
@@ -68102,7 +68102,7 @@
       </c>
       <c r="EV154" s="3"/>
     </row>
-    <row r="155" spans="1:152">
+    <row r="155" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A155" s="12" t="s">
         <v>168</v>
       </c>
@@ -68560,37 +68560,37 @@
       </c>
       <c r="EV155" s="3"/>
     </row>
-    <row r="156" spans="1:152">
+    <row r="156" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A156" s="12" t="s">
         <v>183</v>
       </c>
       <c r="B156" s="11"/>
       <c r="C156" s="12">
         <f t="shared" si="308"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D156" s="12">
         <f t="shared" si="368"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E156" s="12">
         <f t="shared" si="369"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F156" s="13" t="str">
         <f t="shared" si="309"/>
-        <v>0%</v>
+        <v>40%</v>
       </c>
       <c r="G156" s="11"/>
       <c r="H156" s="12">
         <f t="shared" si="310"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I156" s="13">
         <v>0</v>
       </c>
       <c r="J156" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K156" s="13" t="str">
         <f t="shared" si="311"/>
@@ -68599,17 +68599,17 @@
       <c r="L156" s="11"/>
       <c r="M156" s="12">
         <f t="shared" si="312"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N156" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O156" s="13">
         <v>0</v>
       </c>
       <c r="P156" s="13" t="str">
         <f t="shared" si="313"/>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="Q156" s="11"/>
       <c r="R156" s="12">
@@ -68659,17 +68659,17 @@
       <c r="AF156" s="11"/>
       <c r="AG156" s="12">
         <f t="shared" si="320"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH156" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI156" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ156" s="13" t="str">
         <f t="shared" si="321"/>
-        <v>0%</v>
+        <v>33.33%</v>
       </c>
       <c r="AK156" s="11"/>
       <c r="AL156" s="12">
@@ -69018,31 +69018,31 @@
       </c>
       <c r="EV156" s="3"/>
     </row>
-    <row r="157" spans="1:152">
+    <row r="157" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A157" s="12" t="s">
         <v>95</v>
       </c>
       <c r="B157" s="11"/>
       <c r="C157" s="13">
         <f>SUM(C137:C156)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D157" s="13">
         <f t="shared" ref="D157:E157" si="370">SUM(D137:D156)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E157" s="13">
         <f t="shared" si="370"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F157" s="13" t="str">
         <f>IF(C157,ROUND(D157/C157*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="G157" s="11"/>
       <c r="H157" s="13">
         <f>SUM(H137:H156)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I157" s="12">
         <f>SUM(I137:I156)</f>
@@ -69058,11 +69058,11 @@
       <c r="L157" s="11"/>
       <c r="M157" s="13">
         <f>SUM(M137:M156)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N157" s="12">
         <f>SUM(N137:N156)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O157" s="12">
         <f>SUM(O137:O156)</f>
@@ -69070,7 +69070,7 @@
       </c>
       <c r="P157" s="13" t="str">
         <f>IF(M157,ROUND(N157/M157*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="Q157" s="11"/>
       <c r="R157" s="13">
@@ -69092,11 +69092,11 @@
       <c r="V157" s="11"/>
       <c r="W157" s="13">
         <f>SUM(W137:W156)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X157" s="12">
         <f>SUM(X137:X156)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y157" s="12">
         <f>SUM(Y137:Y156)</f>
@@ -69104,41 +69104,41 @@
       </c>
       <c r="Z157" s="13" t="str">
         <f>IF(W157,ROUND(X157/W157*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="AA157" s="11"/>
       <c r="AB157" s="13">
         <f>SUM(AB137:AB156)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC157" s="12">
         <f>SUM(AC137:AC156)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD157" s="12">
         <f>SUM(AD137:AD156)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE157" s="13" t="str">
         <f>IF(AB157,ROUND(AC157/AB157*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="AF157" s="11"/>
       <c r="AG157" s="13">
         <f>SUM(AG137:AG156)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH157" s="13">
         <f t="shared" ref="AH157:AI157" si="371">SUM(AH137:AH156)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI157" s="13">
         <f t="shared" si="371"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ157" s="13" t="str">
         <f>IF(AG157,ROUND(AH157/AG157*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>33.33%</v>
       </c>
       <c r="AK157" s="11"/>
       <c r="AL157" s="13">
@@ -69415,11 +69415,11 @@
       <c r="DM157" s="11"/>
       <c r="DN157" s="13">
         <f>SUM(DN137:DN156)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DO157" s="12">
         <f>SUM(DO137:DO156)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DP157" s="12">
         <f>SUM(DP137:DP156)</f>
@@ -69427,7 +69427,7 @@
       </c>
       <c r="DQ157" s="13" t="str">
         <f>IF(DN157,ROUND(DO157/DN157*100,2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="DR157" s="11"/>
       <c r="DS157" s="13">
@@ -69466,7 +69466,7 @@
       <c r="EB157" s="11"/>
       <c r="EC157" s="13">
         <f>SUM(EC137:EC156)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ED157" s="12">
         <f>SUM(ED137:ED156)</f>
@@ -69474,7 +69474,7 @@
       </c>
       <c r="EE157" s="12">
         <f>SUM(EE137:EE156)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EF157" s="13" t="str">
         <f>IF(EC157,ROUND(ED157/EC157*100,2),0) &amp; "%"</f>
@@ -69533,7 +69533,7 @@
       </c>
       <c r="EV157" s="3"/>
     </row>
-    <row r="158" spans="1:152">
+    <row r="158" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A158" s="3"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
@@ -69687,7 +69687,7 @@
       <c r="EU158" s="3"/>
       <c r="EV158" s="3"/>
     </row>
-    <row r="159" spans="1:152">
+    <row r="159" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A159" s="3"/>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
@@ -69841,7 +69841,7 @@
       <c r="EU159" s="3"/>
       <c r="EV159" s="3"/>
     </row>
-    <row r="160" spans="1:152">
+    <row r="160" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A160" s="9" t="s">
         <v>172</v>
       </c>
@@ -69853,7 +69853,7 @@
       <c r="E160" s="9"/>
       <c r="F160" s="9" t="str">
         <f>IF(SUM(D133,D157),ROUND(SUM(D133,D157)*100/SUM(C133,C157),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>56.52%</v>
       </c>
       <c r="G160" s="10"/>
       <c r="H160" s="9" t="s">
@@ -69863,7 +69863,7 @@
       <c r="J160" s="9"/>
       <c r="K160" s="9" t="str">
         <f>IF(SUM(I133,I157),ROUND(SUM(I133,I157)*100/SUM(H133,H157),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="L160" s="10"/>
       <c r="M160" s="9" t="s">
@@ -69873,7 +69873,7 @@
       <c r="O160" s="9"/>
       <c r="P160" s="9" t="str">
         <f>IF(SUM(N133,N157),ROUND(SUM(N133,N157)*100/SUM(M133,M157),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="Q160" s="10"/>
       <c r="R160" s="9" t="s">
@@ -69883,7 +69883,7 @@
       <c r="T160" s="9"/>
       <c r="U160" s="9" t="str">
         <f>IF(SUM(S133,S157),ROUND(SUM(S133,S157)*100/SUM(R133,R157),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="V160" s="10"/>
       <c r="W160" s="9" t="s">
@@ -69893,7 +69893,7 @@
       <c r="Y160" s="9"/>
       <c r="Z160" s="9" t="str">
         <f>IF(SUM(X133,X157),ROUND(SUM(X133,X157)*100/SUM(W133,W157),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>66.67%</v>
       </c>
       <c r="AA160" s="10"/>
       <c r="AB160" s="9" t="s">
@@ -69903,7 +69903,7 @@
       <c r="AD160" s="9"/>
       <c r="AE160" s="9" t="str">
         <f>IF(SUM(AC133,AC157),ROUND(SUM(AC133,AC157)*100/SUM(AB133,AB157),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="AF160" s="10"/>
       <c r="AG160" s="9" t="s">
@@ -69913,7 +69913,7 @@
       <c r="AI160" s="9"/>
       <c r="AJ160" s="9" t="str">
         <f>IF(SUM(AH133,AH157),ROUND(SUM(AH133,AH157)*100/SUM(AG133,AG157),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>60%</v>
       </c>
       <c r="AK160" s="10"/>
       <c r="AL160" s="9" t="s">
@@ -69923,7 +69923,7 @@
       <c r="AN160" s="9"/>
       <c r="AO160" s="9" t="str">
         <f>IF(SUM(AM133,AM157),ROUND(SUM(AM133,AM157)*100/SUM(AL133,AL157),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>50%</v>
       </c>
       <c r="AP160" s="10"/>
       <c r="AQ160" s="9" t="s">
@@ -70083,7 +70083,7 @@
       <c r="DP160" s="9"/>
       <c r="DQ160" s="9" t="str">
         <f>IF(SUM(DO133,DO157),ROUND(SUM(DO133,DO157)*100/SUM(DN133,DN157),2),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="DR160" s="10"/>
       <c r="DS160" s="9" t="s">
@@ -70143,11 +70143,11 @@
       <c r="ET160" s="9"/>
       <c r="EU160" s="9" t="str">
         <f>IF(SUM(ES133,ES157),SUM(ES133,ES157)*100/SUM(ER133,ER157),0) &amp; "%"</f>
-        <v>0%</v>
+        <v>100%</v>
       </c>
       <c r="EV160" s="3"/>
     </row>
-    <row r="161" spans="1:152">
+    <row r="161" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A161" s="9"/>
       <c r="B161" s="10"/>
       <c r="C161" s="9" t="s">
@@ -70155,9 +70155,9 @@
       </c>
       <c r="D161" s="9"/>
       <c r="E161" s="9"/>
-      <c r="F161" s="16" t="e">
+      <c r="F161" s="16" t="str">
         <f>ROUND(((SUM(D74,D101)/SUM(C74,C101)+SUM(D133,D157)/SUM(C133,C157))/2)*100,2) &amp; "%"</f>
-        <v>#DIV/0!</v>
+        <v>51.85%</v>
       </c>
       <c r="G161" s="10"/>
       <c r="H161" s="9" t="s">
@@ -70165,9 +70165,9 @@
       </c>
       <c r="I161" s="9"/>
       <c r="J161" s="9"/>
-      <c r="K161" s="16" t="e">
+      <c r="K161" s="16" t="str">
         <f>ROUND(((SUM(I74,I101)/SUM(H74,H101)+SUM(I133,I157)/SUM(H133,H157))/2)*100,2) &amp; "%"</f>
-        <v>#DIV/0!</v>
+        <v>50%</v>
       </c>
       <c r="L161" s="10"/>
       <c r="M161" s="9" t="s">
@@ -70175,9 +70175,9 @@
       </c>
       <c r="N161" s="9"/>
       <c r="O161" s="9"/>
-      <c r="P161" s="16" t="e">
+      <c r="P161" s="16" t="str">
         <f>ROUND(((SUM(N74,N101)/SUM(M74,M101)+SUM(N133,N157)/SUM(M133,M157))/2)*100,2) &amp; "%"</f>
-        <v>#DIV/0!</v>
+        <v>78.57%</v>
       </c>
       <c r="Q161" s="10"/>
       <c r="R161" s="9" t="s">
@@ -70185,9 +70185,9 @@
       </c>
       <c r="S161" s="9"/>
       <c r="T161" s="9"/>
-      <c r="U161" s="16" t="e">
+      <c r="U161" s="16" t="str">
         <f>ROUND(((SUM(S74,S101)/SUM(R74,R101)+SUM(S133,S157)/SUM(R133,R157))/2)*100,2) &amp; "%"</f>
-        <v>#DIV/0!</v>
+        <v>46.43%</v>
       </c>
       <c r="V161" s="10"/>
       <c r="W161" s="9" t="s">
@@ -70195,9 +70195,9 @@
       </c>
       <c r="X161" s="9"/>
       <c r="Y161" s="9"/>
-      <c r="Z161" s="16" t="e">
+      <c r="Z161" s="16" t="str">
         <f>ROUND(((SUM(X74,X101)/SUM(W74,W101)+SUM(X133,X157)/SUM(W133,W157))/2)*100,2) &amp; "%"</f>
-        <v>#DIV/0!</v>
+        <v>58.33%</v>
       </c>
       <c r="AA161" s="10"/>
       <c r="AB161" s="9" t="s">
@@ -70205,9 +70205,9 @@
       </c>
       <c r="AC161" s="9"/>
       <c r="AD161" s="9"/>
-      <c r="AE161" s="16" t="e">
+      <c r="AE161" s="16" t="str">
         <f>ROUND(((SUM(AC74,AC101)/SUM(AB74,AB101)+SUM(AC133,AC157)/SUM(AB133,AB157))/2)*100,2) &amp; "%"</f>
-        <v>#DIV/0!</v>
+        <v>46.43%</v>
       </c>
       <c r="AF161" s="10"/>
       <c r="AG161" s="9" t="s">
@@ -70215,9 +70215,9 @@
       </c>
       <c r="AH161" s="9"/>
       <c r="AI161" s="9"/>
-      <c r="AJ161" s="16" t="e">
+      <c r="AJ161" s="16" t="str">
         <f>ROUND(((SUM(AH74,AH101)/SUM(AG74,AG101)+SUM(AH133,AH157)/SUM(AG133,AG157))/2)*100,2) &amp; "%"</f>
-        <v>#DIV/0!</v>
+        <v>67.5%</v>
       </c>
       <c r="AK161" s="10"/>
       <c r="AL161" s="9" t="s">
@@ -70225,9 +70225,9 @@
       </c>
       <c r="AM161" s="9"/>
       <c r="AN161" s="9"/>
-      <c r="AO161" s="16" t="e">
+      <c r="AO161" s="16" t="str">
         <f>ROUND(((SUM(AM74,AM101)/SUM(AL74,AL101)+SUM(AM133,AM157)/SUM(AL133,AL157))/2)*100,2) &amp; "%"</f>
-        <v>#DIV/0!</v>
+        <v>50%</v>
       </c>
       <c r="AP161" s="10"/>
       <c r="AQ161" s="9" t="s">
@@ -70235,9 +70235,9 @@
       </c>
       <c r="AR161" s="9"/>
       <c r="AS161" s="9"/>
-      <c r="AT161" s="16" t="e">
+      <c r="AT161" s="16" t="str">
         <f>ROUND(((SUM(AR74,AR101)/SUM(AQ74,AQ101)+SUM(AR133,AR157)/SUM(AQ133,AQ157))/2)*100,2) &amp; "%"</f>
-        <v>#DIV/0!</v>
+        <v>12.5%</v>
       </c>
       <c r="AU161" s="10"/>
       <c r="AV161" s="9" t="s">
@@ -70375,9 +70375,9 @@
       </c>
       <c r="DJ161" s="9"/>
       <c r="DK161" s="9"/>
-      <c r="DL161" s="16" t="e">
+      <c r="DL161" s="16" t="str">
         <f>ROUND(((SUM(DJ74,DJ101)/SUM(DI74,DI101)+SUM(DJ133,DJ157)/SUM(DI133,DI157))/2)*100,2) &amp; "%"</f>
-        <v>#DIV/0!</v>
+        <v>16.67%</v>
       </c>
       <c r="DM161" s="10"/>
       <c r="DN161" s="9" t="s">
@@ -70385,9 +70385,9 @@
       </c>
       <c r="DO161" s="9"/>
       <c r="DP161" s="9"/>
-      <c r="DQ161" s="16" t="e">
+      <c r="DQ161" s="16" t="str">
         <f>ROUND(((SUM(DO74,DO101)/SUM(DN74,DN101)+SUM(DO133,DO157)/SUM(DN133,DN157))/2)*100,2) &amp; "%"</f>
-        <v>#DIV/0!</v>
+        <v>83.33%</v>
       </c>
       <c r="DR161" s="10"/>
       <c r="DS161" s="9" t="s">
@@ -70415,9 +70415,9 @@
       </c>
       <c r="ED161" s="9"/>
       <c r="EE161" s="9"/>
-      <c r="EF161" s="16" t="e">
+      <c r="EF161" s="16" t="str">
         <f>ROUND(((SUM(ED74,ED101)/SUM(EC74,EC101)+SUM(ED133,ED157)/SUM(EC133,EC157))/2)*100,2) &amp; "%"</f>
-        <v>#DIV/0!</v>
+        <v>0%</v>
       </c>
       <c r="EG161" s="10"/>
       <c r="EH161" s="9" t="s">
@@ -70445,13 +70445,13 @@
       </c>
       <c r="ES161" s="9"/>
       <c r="ET161" s="9"/>
-      <c r="EU161" s="16" t="e">
+      <c r="EU161" s="16" t="str">
         <f>ROUND(((SUM(ES74,ES101)/SUM(ER74,ER101)+SUM(ES133,ES157)/SUM(ER133,ER157))/2)*100,2) &amp; "%"</f>
-        <v>#DIV/0!</v>
+        <v>75%</v>
       </c>
       <c r="EV161" s="3"/>
     </row>
-    <row r="162" spans="1:152">
+    <row r="162" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A162" s="9"/>
       <c r="B162" s="10"/>
       <c r="C162" s="9" t="s">
@@ -70461,7 +70461,7 @@
       <c r="E162" s="9"/>
       <c r="F162" s="9">
         <f>+SUM(C157,C133,C101,C74)</f>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="G162" s="10"/>
       <c r="H162" s="9" t="s">
@@ -70471,7 +70471,7 @@
       <c r="J162" s="9"/>
       <c r="K162" s="9">
         <f>+SUM(H157,H133,H101,H74)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L162" s="10"/>
       <c r="M162" s="9" t="s">
@@ -70481,7 +70481,7 @@
       <c r="O162" s="9"/>
       <c r="P162" s="9">
         <f>+SUM(M157,M133,M101,M74)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q162" s="10"/>
       <c r="R162" s="9" t="s">
@@ -70491,7 +70491,7 @@
       <c r="T162" s="9"/>
       <c r="U162" s="9">
         <f>+SUM(R157,R133,R101,R74)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="V162" s="10"/>
       <c r="W162" s="9" t="s">
@@ -70501,7 +70501,7 @@
       <c r="Y162" s="9"/>
       <c r="Z162" s="9">
         <f>+SUM(W157,W133,W101,W74)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AA162" s="10"/>
       <c r="AB162" s="9" t="s">
@@ -70511,7 +70511,7 @@
       <c r="AD162" s="9"/>
       <c r="AE162" s="9">
         <f>+SUM(AB157,AB133,AB101,AB74)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AF162" s="10"/>
       <c r="AG162" s="9" t="s">
@@ -70521,7 +70521,7 @@
       <c r="AI162" s="9"/>
       <c r="AJ162" s="9">
         <f>+SUM(AG157,AG133,AG101,AG74)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AK162" s="10"/>
       <c r="AL162" s="9" t="s">
@@ -70531,7 +70531,7 @@
       <c r="AN162" s="9"/>
       <c r="AO162" s="9">
         <f>+SUM(AL157,AL133,AL101,AL74)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AP162" s="10"/>
       <c r="AQ162" s="9" t="s">
@@ -70541,7 +70541,7 @@
       <c r="AS162" s="9"/>
       <c r="AT162" s="9">
         <f>+SUM(AQ157,AQ133,AQ101,AQ74)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AU162" s="10"/>
       <c r="AV162" s="9" t="s">
@@ -70571,7 +70571,7 @@
       <c r="BH162" s="9"/>
       <c r="BI162" s="9">
         <f>+SUM(BF157,BF133,BF101,BF74)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ162" s="10"/>
       <c r="BK162" s="9" t="s">
@@ -70681,7 +70681,7 @@
       <c r="DK162" s="9"/>
       <c r="DL162" s="9">
         <f>+SUM(DI157,DI133,DI101,DI74)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DM162" s="10"/>
       <c r="DN162" s="9" t="s">
@@ -70691,7 +70691,7 @@
       <c r="DP162" s="9"/>
       <c r="DQ162" s="9">
         <f>+SUM(DN157,DN133,DN101,DN74)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DR162" s="10"/>
       <c r="DS162" s="9" t="s">
@@ -70721,7 +70721,7 @@
       <c r="EE162" s="9"/>
       <c r="EF162" s="9">
         <f>+SUM(EC157,EC133,EC101,EC74)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="EG162" s="10"/>
       <c r="EH162" s="9" t="s">
@@ -70751,11 +70751,11 @@
       <c r="ET162" s="9"/>
       <c r="EU162" s="9">
         <f>+SUM(ER157,ER133,ER101,ER74)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="EV162" s="3"/>
     </row>
-    <row r="163" spans="1:152">
+    <row r="163" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A163" s="3"/>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
@@ -70909,7 +70909,7 @@
       <c r="EU163" s="3"/>
       <c r="EV163" s="3"/>
     </row>
-    <row r="164" spans="1:152">
+    <row r="164" spans="1:152" x14ac:dyDescent="0.25">
       <c r="A164" s="3"/>
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
@@ -71070,6 +71070,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d74e12c9-bdf3-447e-ac63-b8aa30cb912e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006D6901F31B669244A77CF3DC592DC06F" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f07ba37d9f6a9a16ab78a3833be08f3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d74e12c9-bdf3-447e-ac63-b8aa30cb912e" xmlns:ns4="7ce3718d-1d19-4340-bc07-211e3ea25757" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3d76b4510715f63c0dd84a4bd0fa290f" ns3:_="" ns4:_="">
     <xsd:import namespace="d74e12c9-bdf3-447e-ac63-b8aa30cb912e"/>
@@ -71284,14 +71292,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d74e12c9-bdf3-447e-ac63-b8aa30cb912e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -71302,6 +71302,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E2E85D4-37C6-4843-9D21-AD40AB5F6E3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="d74e12c9-bdf3-447e-ac63-b8aa30cb912e"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7ce3718d-1d19-4340-bc07-211e3ea25757"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D93BBC3-F948-4065-9078-5D0662F77D28}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -71320,23 +71337,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E2E85D4-37C6-4843-9D21-AD40AB5F6E3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d74e12c9-bdf3-447e-ac63-b8aa30cb912e"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7ce3718d-1d19-4340-bc07-211e3ea25757"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF8F943-7811-4141-8F4E-8FF466B07D87}">
   <ds:schemaRefs>

</xml_diff>